<commit_message>
Modification SRS CRS Login Register IDs
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI9M-Testing\Core\QA\WorkShop\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3E7B9A-91A7-455C-9D71-B3EA798688D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34ECEA55-D9A7-4A57-AFB4-772C85F380AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>CRS ID</t>
   </si>
@@ -127,24 +127,6 @@
     <t>SRS_Reg_019</t>
   </si>
   <si>
-    <t>SRS_Reg_020</t>
-  </si>
-  <si>
-    <t>SRS_Reg_021</t>
-  </si>
-  <si>
-    <t>SRS_Reg_022</t>
-  </si>
-  <si>
-    <t>SRS_Reg_023</t>
-  </si>
-  <si>
-    <t>SRS_Reg_024</t>
-  </si>
-  <si>
-    <t>SRS_Reg_025</t>
-  </si>
-  <si>
     <t>SRS_Login_001</t>
   </si>
   <si>
@@ -158,15 +140,6 @@
   </si>
   <si>
     <t>SRS_Login_005</t>
-  </si>
-  <si>
-    <t>SRS_Login_006</t>
-  </si>
-  <si>
-    <t>SRS_Login_007</t>
-  </si>
-  <si>
-    <t>SRS_Login_008</t>
   </si>
 </sst>
 </file>
@@ -510,8 +483,8 @@
   </sheetPr>
   <dimension ref="A1:B230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -561,7 +534,7 @@
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>20</v>
@@ -569,7 +542,7 @@
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>21</v>
@@ -577,7 +550,7 @@
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>22</v>
@@ -585,31 +558,31 @@
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
-        <v>7</v>
+      <c r="A10" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
-        <v>7</v>
+      <c r="A11" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>5</v>
+      <c r="A12" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>26</v>
@@ -617,7 +590,7 @@
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>27</v>
@@ -625,7 +598,7 @@
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>28</v>
@@ -633,7 +606,7 @@
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>29</v>
@@ -641,7 +614,7 @@
     </row>
     <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>30</v>
@@ -649,7 +622,7 @@
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>31</v>
@@ -657,7 +630,7 @@
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>32</v>
@@ -665,7 +638,7 @@
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>33</v>
@@ -673,7 +646,7 @@
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>34</v>
@@ -681,115 +654,79 @@
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="A26" s="5"/>
+      <c r="B26" s="3"/>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>43</v>
-      </c>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>44</v>
-      </c>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>48</v>
-      </c>
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>

</xml_diff>

<commit_message>
Remove CRS SRS IDs
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI9M-Testing\Core\QA\WorkShop\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34ECEA55-D9A7-4A57-AFB4-772C85F380AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8108B41E-661A-4556-AEAF-A6D7085E1026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,126 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>CRS ID</t>
   </si>
   <si>
     <t>SRS ID</t>
-  </si>
-  <si>
-    <t>CRS_Reg_001</t>
-  </si>
-  <si>
-    <t>CRS_Reg_002</t>
-  </si>
-  <si>
-    <t>CRS_Reg_003</t>
-  </si>
-  <si>
-    <t>CRS_Reg_011</t>
-  </si>
-  <si>
-    <t>CRS_Reg_010</t>
-  </si>
-  <si>
-    <t>CRS_Reg_004</t>
-  </si>
-  <si>
-    <t>CRS_Reg_005</t>
-  </si>
-  <si>
-    <t>CRS_Reg_006</t>
-  </si>
-  <si>
-    <t>CRS_Reg_007</t>
-  </si>
-  <si>
-    <t>CRS_Reg_008</t>
-  </si>
-  <si>
-    <t>CRS_Reg_009</t>
-  </si>
-  <si>
-    <t>CRS_Reg_012</t>
-  </si>
-  <si>
-    <t>CRS_Login_001</t>
-  </si>
-  <si>
-    <t>CRS_Login_003</t>
-  </si>
-  <si>
-    <t>SRS_Reg_001</t>
-  </si>
-  <si>
-    <t>SRS_Reg_002</t>
-  </si>
-  <si>
-    <t>SRS_Reg_003</t>
-  </si>
-  <si>
-    <t>SRS_Reg_004</t>
-  </si>
-  <si>
-    <t>SRS_Reg_005</t>
-  </si>
-  <si>
-    <t>SRS_Reg_006</t>
-  </si>
-  <si>
-    <t>SRS_Reg_007</t>
-  </si>
-  <si>
-    <t>SRS_Reg_008</t>
-  </si>
-  <si>
-    <t>SRS_Reg_009</t>
-  </si>
-  <si>
-    <t>SRS_Reg_010</t>
-  </si>
-  <si>
-    <t>SRS_Reg_011</t>
-  </si>
-  <si>
-    <t>SRS_Reg_012</t>
-  </si>
-  <si>
-    <t>SRS_Reg_013</t>
-  </si>
-  <si>
-    <t>SRS_Reg_014</t>
-  </si>
-  <si>
-    <t>SRS_Reg_015</t>
-  </si>
-  <si>
-    <t>SRS_Reg_016</t>
-  </si>
-  <si>
-    <t>SRS_Reg_017</t>
-  </si>
-  <si>
-    <t>SRS_Reg_018</t>
-  </si>
-  <si>
-    <t>SRS_Reg_019</t>
-  </si>
-  <si>
-    <t>SRS_Login_001</t>
-  </si>
-  <si>
-    <t>SRS_Login_002</t>
-  </si>
-  <si>
-    <t>SRS_Login_003</t>
-  </si>
-  <si>
-    <t>SRS_Login_004</t>
-  </si>
-  <si>
-    <t>SRS_Login_005</t>
   </si>
 </sst>
 </file>
@@ -484,7 +370,7 @@
   <dimension ref="A1:B230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -501,196 +387,100 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="A2" s="4"/>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="A3" s="4"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="A4" s="4"/>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="A6" s="4"/>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="A7" s="4"/>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="A8" s="4"/>
+      <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A9" s="4"/>
+      <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="A10" s="5"/>
+      <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="A11" s="5"/>
+      <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="A12" s="5"/>
+      <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="A13" s="5"/>
+      <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="A14" s="5"/>
+      <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="A15" s="5"/>
+      <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="A16" s="5"/>
+      <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>31</v>
-      </c>
+      <c r="A17" s="5"/>
+      <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="A18" s="5"/>
+      <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="A19" s="5"/>
+      <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="A20" s="5"/>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>36</v>
-      </c>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>

</xml_diff>

<commit_message>
Doc: Updated RTM file with traceability between SRS file and Test cases file for login feature
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Online-Mobile-Store-WebSite\RTM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75945F41-DE25-4DEE-B736-B6AB8D61537D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB33DAF-CAA0-4564-ABA7-D7E758DE3183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>CRS ID</t>
+    <t>SRS ID</t>
   </si>
   <si>
-    <t>SRS ID</t>
+    <t>Test case ID</t>
+  </si>
+  <si>
+    <t>SRS_Login_001</t>
+  </si>
+  <si>
+    <t>SRS_Login_002</t>
+  </si>
+  <si>
+    <t>SRS_Login_003</t>
+  </si>
+  <si>
+    <t>SRS_Login_004</t>
+  </si>
+  <si>
+    <t>SRS_Login_005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_Login_001 </t>
+  </si>
+  <si>
+    <t>TC_Login_001  
+TC-Login_008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_Login_001  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_Login_002
+TC_Login_003
+TC_Login_004
+TC_Login_009
+TC_Login_0010
+TC_Login_0011
+</t>
+  </si>
+  <si>
+    <t>TC_Login_014</t>
   </si>
 </sst>
 </file>
@@ -140,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -149,6 +186,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,16 +409,17 @@
   </sheetPr>
   <dimension ref="A1:B230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="D163" sqref="D163"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="23.90625" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -386,919 +427,939 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="4"/>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="4"/>
-      <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="4"/>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="4"/>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="4"/>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="131.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="3"/>
     </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
     </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
     </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
     </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
     </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
     </row>
-    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
     </row>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
     </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
     </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
     </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
     </row>
-    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
     </row>
-    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
     </row>
-    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
     </row>
-    <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
     </row>
-    <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
     </row>
-    <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
     </row>
-    <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
     </row>
-    <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
     </row>
-    <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
     </row>
-    <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
     </row>
-    <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
     </row>
-    <row r="62" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
     </row>
-    <row r="63" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
     </row>
-    <row r="64" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
     </row>
-    <row r="65" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
     </row>
-    <row r="66" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
     </row>
-    <row r="67" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
     </row>
-    <row r="68" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
     </row>
-    <row r="69" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
     </row>
-    <row r="70" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
     </row>
-    <row r="71" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
     </row>
-    <row r="72" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
     </row>
-    <row r="74" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
     </row>
-    <row r="75" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
     </row>
-    <row r="76" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
     </row>
-    <row r="77" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
     </row>
-    <row r="78" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
     </row>
-    <row r="79" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
     </row>
-    <row r="80" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
     </row>
-    <row r="81" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
     </row>
-    <row r="82" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
     </row>
-    <row r="83" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
     </row>
-    <row r="84" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
     </row>
-    <row r="85" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
     </row>
-    <row r="86" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
     </row>
-    <row r="87" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
     </row>
-    <row r="88" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
     </row>
-    <row r="89" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
     </row>
-    <row r="90" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
     </row>
-    <row r="91" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
     </row>
-    <row r="92" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
     </row>
-    <row r="93" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
     </row>
-    <row r="94" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
     </row>
-    <row r="95" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
     </row>
-    <row r="96" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
     </row>
-    <row r="97" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
     </row>
-    <row r="98" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
     </row>
-    <row r="99" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
     </row>
-    <row r="100" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
     </row>
-    <row r="101" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
     </row>
-    <row r="102" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
     </row>
-    <row r="103" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
     </row>
-    <row r="104" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
     </row>
-    <row r="105" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
     </row>
-    <row r="106" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
     </row>
-    <row r="107" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
     </row>
-    <row r="108" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
     </row>
-    <row r="109" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
     </row>
-    <row r="110" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
     </row>
-    <row r="111" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
     </row>
-    <row r="112" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
     </row>
-    <row r="113" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
     </row>
-    <row r="114" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
     </row>
-    <row r="115" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
     </row>
-    <row r="116" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
     </row>
-    <row r="117" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
     </row>
-    <row r="118" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
     </row>
-    <row r="119" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
     </row>
-    <row r="120" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
     </row>
-    <row r="121" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
     </row>
-    <row r="122" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
     </row>
-    <row r="123" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
     </row>
-    <row r="124" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
     </row>
-    <row r="125" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
     </row>
-    <row r="126" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
     </row>
-    <row r="127" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
     </row>
-    <row r="128" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
     </row>
-    <row r="129" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
     </row>
-    <row r="130" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
     </row>
-    <row r="131" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
     </row>
-    <row r="132" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
     </row>
-    <row r="133" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
     </row>
-    <row r="134" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
     </row>
-    <row r="135" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
     </row>
-    <row r="136" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
     </row>
-    <row r="137" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
     </row>
-    <row r="138" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
     </row>
-    <row r="139" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
     </row>
-    <row r="140" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
     </row>
-    <row r="141" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
     </row>
-    <row r="142" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
     </row>
-    <row r="143" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
     </row>
-    <row r="144" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
     </row>
-    <row r="145" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
     </row>
-    <row r="146" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
     </row>
-    <row r="147" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
     </row>
-    <row r="148" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
     </row>
-    <row r="149" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
     </row>
-    <row r="150" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
     </row>
-    <row r="151" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
     </row>
-    <row r="152" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
     </row>
-    <row r="153" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
     </row>
-    <row r="154" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
     </row>
-    <row r="155" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
     </row>
-    <row r="156" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
     </row>
-    <row r="157" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
     </row>
-    <row r="158" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
     </row>
-    <row r="159" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
     </row>
-    <row r="160" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
     </row>
-    <row r="161" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2"/>
       <c r="B161" s="2"/>
     </row>
-    <row r="162" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
     </row>
-    <row r="163" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
       <c r="B163" s="2"/>
     </row>
-    <row r="164" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2"/>
       <c r="B164" s="2"/>
     </row>
-    <row r="165" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2"/>
       <c r="B165" s="2"/>
     </row>
-    <row r="166" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2"/>
       <c r="B166" s="2"/>
     </row>
-    <row r="167" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2"/>
       <c r="B167" s="2"/>
     </row>
-    <row r="168" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2"/>
       <c r="B168" s="2"/>
     </row>
-    <row r="169" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2"/>
       <c r="B169" s="2"/>
     </row>
-    <row r="170" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2"/>
       <c r="B170" s="2"/>
     </row>
-    <row r="171" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2"/>
       <c r="B171" s="2"/>
     </row>
-    <row r="172" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2"/>
       <c r="B172" s="2"/>
     </row>
-    <row r="173" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
     </row>
-    <row r="174" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2"/>
       <c r="B174" s="2"/>
     </row>
-    <row r="175" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
     </row>
-    <row r="176" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
     </row>
-    <row r="177" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
     </row>
-    <row r="178" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
     </row>
-    <row r="179" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
     </row>
-    <row r="180" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
     </row>
-    <row r="181" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
     </row>
-    <row r="182" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
     </row>
-    <row r="183" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
     </row>
-    <row r="184" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
     </row>
-    <row r="185" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2"/>
       <c r="B185" s="2"/>
     </row>
-    <row r="186" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
     </row>
-    <row r="187" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
     </row>
-    <row r="188" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
     </row>
-    <row r="189" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2"/>
       <c r="B189" s="2"/>
     </row>
-    <row r="190" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2"/>
       <c r="B190" s="2"/>
     </row>
-    <row r="191" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2"/>
       <c r="B191" s="2"/>
     </row>
-    <row r="192" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2"/>
       <c r="B192" s="2"/>
     </row>
-    <row r="193" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="2"/>
       <c r="B193" s="2"/>
     </row>
-    <row r="194" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2"/>
       <c r="B194" s="2"/>
     </row>
-    <row r="195" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="2"/>
       <c r="B195" s="2"/>
     </row>
-    <row r="196" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="2"/>
       <c r="B196" s="2"/>
     </row>
-    <row r="197" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="2"/>
       <c r="B197" s="2"/>
     </row>
-    <row r="198" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="2"/>
       <c r="B198" s="2"/>
     </row>
-    <row r="199" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="2"/>
       <c r="B199" s="2"/>
     </row>
-    <row r="200" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="2"/>
       <c r="B200" s="2"/>
     </row>
-    <row r="201" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="2"/>
       <c r="B201" s="2"/>
     </row>
-    <row r="202" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2"/>
       <c r="B202" s="2"/>
     </row>
-    <row r="203" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2"/>
       <c r="B203" s="2"/>
     </row>
-    <row r="204" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="2"/>
       <c r="B204" s="2"/>
     </row>
-    <row r="205" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2"/>
       <c r="B205" s="2"/>
     </row>
-    <row r="206" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2"/>
       <c r="B206" s="2"/>
     </row>
-    <row r="207" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2"/>
       <c r="B207" s="2"/>
     </row>
-    <row r="208" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2"/>
       <c r="B208" s="2"/>
     </row>
-    <row r="209" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2"/>
       <c r="B209" s="2"/>
     </row>
-    <row r="210" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2"/>
       <c r="B210" s="2"/>
     </row>
-    <row r="211" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2"/>
       <c r="B211" s="2"/>
     </row>
-    <row r="212" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2"/>
       <c r="B212" s="2"/>
     </row>
-    <row r="213" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2"/>
       <c r="B213" s="2"/>
     </row>
-    <row r="214" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2"/>
       <c r="B214" s="2"/>
     </row>
-    <row r="215" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="2"/>
       <c r="B215" s="2"/>
     </row>
-    <row r="216" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="2"/>
       <c r="B216" s="2"/>
     </row>
-    <row r="217" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2"/>
       <c r="B217" s="2"/>
     </row>
-    <row r="218" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="2"/>
       <c r="B218" s="2"/>
     </row>
-    <row r="219" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="2"/>
       <c r="B219" s="2"/>
     </row>
-    <row r="220" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="2"/>
       <c r="B220" s="2"/>
     </row>
-    <row r="221" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="2"/>
       <c r="B221" s="2"/>
     </row>
-    <row r="222" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="2"/>
       <c r="B222" s="2"/>
     </row>
-    <row r="223" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2"/>
       <c r="B223" s="2"/>
     </row>
-    <row r="224" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="2"/>
       <c r="B224" s="2"/>
     </row>
-    <row r="225" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="2"/>
       <c r="B225" s="2"/>
     </row>
-    <row r="226" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2"/>
       <c r="B226" s="2"/>
     </row>
-    <row r="227" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2"/>
       <c r="B227" s="2"/>
     </row>
-    <row r="228" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="2"/>
       <c r="B228" s="2"/>
     </row>
-    <row r="229" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="2"/>
       <c r="B229" s="2"/>
     </row>
-    <row r="230" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="2"/>
       <c r="B230" s="2"/>
     </row>

</xml_diff>

<commit_message>
Doc: Added traceabililty between SRS ID's and test cases for Registration and supllier
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB33DAF-CAA0-4564-ABA7-D7E758DE3183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F23F2E0-2247-4900-BCD8-29E0600C8A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
   <si>
     <t>SRS ID</t>
   </si>
@@ -63,6 +63,175 @@
   </si>
   <si>
     <t>TC_Login_014</t>
+  </si>
+  <si>
+    <t>SRS_Register_001</t>
+  </si>
+  <si>
+    <t>TC_Register_001</t>
+  </si>
+  <si>
+    <t>SRS_Register_002</t>
+  </si>
+  <si>
+    <t>TC_Register_002</t>
+  </si>
+  <si>
+    <t>SRS_Register_003</t>
+  </si>
+  <si>
+    <t>TC_Register_003</t>
+  </si>
+  <si>
+    <t>SRS_Register_004</t>
+  </si>
+  <si>
+    <t>TC_Register_004</t>
+  </si>
+  <si>
+    <t>SRS_Register_005</t>
+  </si>
+  <si>
+    <t>TC_Register_005</t>
+  </si>
+  <si>
+    <t>SRS_Register_006</t>
+  </si>
+  <si>
+    <t>TC_Register_006</t>
+  </si>
+  <si>
+    <t>SRS_Register_007</t>
+  </si>
+  <si>
+    <t>TC_Register_007</t>
+  </si>
+  <si>
+    <t>SRS_Register_008</t>
+  </si>
+  <si>
+    <t>TC_Register_008</t>
+  </si>
+  <si>
+    <t>SRS_Register_009</t>
+  </si>
+  <si>
+    <t>TC_Register_009</t>
+  </si>
+  <si>
+    <t>SRS_Register_010</t>
+  </si>
+  <si>
+    <t>TC_Register_010</t>
+  </si>
+  <si>
+    <t>SRS_Register_011</t>
+  </si>
+  <si>
+    <t>TC_Register_011</t>
+  </si>
+  <si>
+    <t>SRS_Register_012</t>
+  </si>
+  <si>
+    <t>TC_Register_012</t>
+  </si>
+  <si>
+    <t>SRS_Register_013</t>
+  </si>
+  <si>
+    <t>TC_Register_013</t>
+  </si>
+  <si>
+    <t>SRS_Register_014</t>
+  </si>
+  <si>
+    <t>TC_Register_014</t>
+  </si>
+  <si>
+    <t>SRS_Register_015</t>
+  </si>
+  <si>
+    <t>TC_Register_015</t>
+  </si>
+  <si>
+    <t>SRS_Register_016</t>
+  </si>
+  <si>
+    <t>TC_Register_016</t>
+  </si>
+  <si>
+    <t>SRS_Register_017</t>
+  </si>
+  <si>
+    <t>TC_Register_017</t>
+  </si>
+  <si>
+    <t>SRS_Register_018</t>
+  </si>
+  <si>
+    <t>SRS_Register_019</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_001</t>
+  </si>
+  <si>
+    <t>TC_Supplier_001</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_002</t>
+  </si>
+  <si>
+    <t>TC_Supplier_002
+TC_Supplier_003</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_003</t>
+  </si>
+  <si>
+    <t>TC_Supplier_004</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_004</t>
+  </si>
+  <si>
+    <t>TC_Supplier_005</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_005</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_006</t>
+  </si>
+  <si>
+    <t>TC_Supplier_006</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_007</t>
+  </si>
+  <si>
+    <t>TC_Supplier_007</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_008</t>
+  </si>
+  <si>
+    <t>TC_Supplier_008</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_009</t>
+  </si>
+  <si>
+    <t>TC_Supplier_009</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_010</t>
+  </si>
+  <si>
+    <t>TC_Supplier_003
+TC_Supplier_005
+TC_Supplier_006
+TC_Supplier_007</t>
   </si>
 </sst>
 </file>
@@ -177,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -187,6 +356,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -407,10 +582,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B230"/>
+  <dimension ref="A1:B249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -427,233 +602,349 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+    <row r="22" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B22" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+    <row r="23" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+    <row r="24" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B24" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="131.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+    <row r="25" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B25" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-    </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-    </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-    </row>
-    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-    </row>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-    </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-    </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-    </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-    </row>
-    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-    </row>
-    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-    </row>
-    <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-    </row>
-    <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-    </row>
-    <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-    </row>
-    <row r="48" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-    </row>
-    <row r="49" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-    </row>
-    <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
+    <row r="26" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="5"/>
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="5"/>
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="5"/>
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="5"/>
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+    </row>
+    <row r="41" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+    </row>
+    <row r="42" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+    </row>
+    <row r="43" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+    </row>
+    <row r="44" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+    </row>
+    <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="5"/>
+      <c r="B45" s="3"/>
+    </row>
+    <row r="46" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+    </row>
+    <row r="47" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+    </row>
+    <row r="48" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+    </row>
+    <row r="49" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+    </row>
+    <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
     </row>
     <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
@@ -1362,6 +1653,82 @@
     <row r="230" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="2"/>
       <c r="B230" s="2"/>
+    </row>
+    <row r="231" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="2"/>
+      <c r="B231" s="2"/>
+    </row>
+    <row r="232" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="2"/>
+      <c r="B232" s="2"/>
+    </row>
+    <row r="233" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="2"/>
+      <c r="B233" s="2"/>
+    </row>
+    <row r="234" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="2"/>
+      <c r="B234" s="2"/>
+    </row>
+    <row r="235" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="2"/>
+      <c r="B235" s="2"/>
+    </row>
+    <row r="236" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="2"/>
+      <c r="B236" s="2"/>
+    </row>
+    <row r="237" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="2"/>
+      <c r="B237" s="2"/>
+    </row>
+    <row r="238" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="2"/>
+      <c r="B238" s="2"/>
+    </row>
+    <row r="239" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="2"/>
+      <c r="B239" s="2"/>
+    </row>
+    <row r="240" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="2"/>
+      <c r="B240" s="2"/>
+    </row>
+    <row r="241" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="2"/>
+      <c r="B241" s="2"/>
+    </row>
+    <row r="242" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="2"/>
+      <c r="B242" s="2"/>
+    </row>
+    <row r="243" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="2"/>
+      <c r="B243" s="2"/>
+    </row>
+    <row r="244" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="2"/>
+      <c r="B244" s="2"/>
+    </row>
+    <row r="245" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="2"/>
+      <c r="B245" s="2"/>
+    </row>
+    <row r="246" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="2"/>
+      <c r="B246" s="2"/>
+    </row>
+    <row r="247" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="2"/>
+      <c r="B247" s="2"/>
+    </row>
+    <row r="248" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A248" s="2"/>
+      <c r="B248" s="2"/>
+    </row>
+    <row r="249" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A249" s="2"/>
+      <c r="B249" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Client Test Cases and RTM Updated
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\RTM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI9M-Testing\Core\QA\WorkShop\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F23F2E0-2247-4900-BCD8-29E0600C8A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC9739A-7DB2-4ACE-A29E-9B43F836BE11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="95">
   <si>
     <t>SRS ID</t>
   </si>
@@ -232,6 +232,90 @@
 TC_Supplier_005
 TC_Supplier_006
 TC_Supplier_007</t>
+  </si>
+  <si>
+    <t>SRS_Client_001</t>
+  </si>
+  <si>
+    <t>SRS_Client_002</t>
+  </si>
+  <si>
+    <t>SRS_Client_003</t>
+  </si>
+  <si>
+    <t>SRS_Client_004</t>
+  </si>
+  <si>
+    <t>SRS_Client_005</t>
+  </si>
+  <si>
+    <t>SRS_Client_006</t>
+  </si>
+  <si>
+    <t>SRS_Client_007</t>
+  </si>
+  <si>
+    <t>SRS_Client_008</t>
+  </si>
+  <si>
+    <t>SRS_Client_009</t>
+  </si>
+  <si>
+    <t>SRS_Client_0010</t>
+  </si>
+  <si>
+    <t>SRS_Client_011</t>
+  </si>
+  <si>
+    <t>SRS_Client_012</t>
+  </si>
+  <si>
+    <t>SRS_Client_013</t>
+  </si>
+  <si>
+    <t>SRS_Client_014</t>
+  </si>
+  <si>
+    <t>SRS_Client_015</t>
+  </si>
+  <si>
+    <t>TC_Client_001</t>
+  </si>
+  <si>
+    <t>TC_Client_002</t>
+  </si>
+  <si>
+    <t>TC_Client_007</t>
+  </si>
+  <si>
+    <t>TC_Client_008</t>
+  </si>
+  <si>
+    <t>TC_Client_009</t>
+  </si>
+  <si>
+    <t>TC_Client_013</t>
+  </si>
+  <si>
+    <t>TC_Client_014</t>
+  </si>
+  <si>
+    <t>TC_Client_003</t>
+  </si>
+  <si>
+    <t>TC_Client_004                            TC_Client_005                             TC_Client_006</t>
+  </si>
+  <si>
+    <t>TC_Client_010                               TC_Client_011                       TC_Client_012</t>
+  </si>
+  <si>
+    <t>TC_Client_015                             TC_Client_016</t>
+  </si>
+  <si>
+    <t>TC_Client_017</t>
+  </si>
+  <si>
+    <t>TC_Client_018</t>
   </si>
 </sst>
 </file>
@@ -584,17 +668,17 @@
   </sheetPr>
   <dimension ref="A1:B249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" customWidth="1"/>
+    <col min="2" max="2" width="37.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,7 +686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -610,7 +694,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -618,7 +702,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -626,7 +710,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -634,7 +718,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -642,7 +726,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
@@ -650,7 +734,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
@@ -658,7 +742,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
@@ -666,7 +750,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
@@ -674,7 +758,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>30</v>
       </c>
@@ -682,7 +766,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>32</v>
       </c>
@@ -690,7 +774,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>34</v>
       </c>
@@ -698,7 +782,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>36</v>
       </c>
@@ -706,7 +790,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>38</v>
       </c>
@@ -714,7 +798,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>40</v>
       </c>
@@ -722,7 +806,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>42</v>
       </c>
@@ -730,7 +814,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>44</v>
       </c>
@@ -738,7 +822,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>46</v>
       </c>
@@ -746,7 +830,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>47</v>
       </c>
@@ -754,7 +838,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>2</v>
       </c>
@@ -762,7 +846,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>3</v>
       </c>
@@ -770,7 +854,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>4</v>
       </c>
@@ -778,7 +862,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>5</v>
       </c>
@@ -786,7 +870,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>6</v>
       </c>
@@ -794,7 +878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>48</v>
       </c>
@@ -802,7 +886,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>50</v>
       </c>
@@ -810,7 +894,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>52</v>
       </c>
@@ -818,7 +902,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>54</v>
       </c>
@@ -826,7 +910,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>56</v>
       </c>
@@ -834,7 +918,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>57</v>
       </c>
@@ -842,7 +926,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>59</v>
       </c>
@@ -850,7 +934,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>61</v>
       </c>
@@ -858,7 +942,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>63</v>
       </c>
@@ -866,7 +950,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>65</v>
       </c>
@@ -874,859 +958,919 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="5"/>
-      <c r="B36" s="3"/>
-    </row>
-    <row r="37" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5"/>
-      <c r="B37" s="3"/>
-    </row>
-    <row r="38" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5"/>
-      <c r="B38" s="3"/>
-    </row>
-    <row r="39" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
-      <c r="B39" s="3"/>
-    </row>
-    <row r="40" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-    </row>
-    <row r="41" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-    </row>
-    <row r="42" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-    </row>
-    <row r="43" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-    </row>
-    <row r="44" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-    </row>
-    <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="5"/>
-      <c r="B45" s="3"/>
-    </row>
-    <row r="46" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
-    </row>
-    <row r="47" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-    </row>
-    <row r="48" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-    </row>
-    <row r="49" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
-    </row>
-    <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-    </row>
-    <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A39" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="54" x14ac:dyDescent="0.35">
+      <c r="A40" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A42" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="54" x14ac:dyDescent="0.35">
+      <c r="A43" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A44" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A45" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="36" x14ac:dyDescent="0.35">
+      <c r="A47" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A49" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
     </row>
-    <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
     </row>
-    <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
     </row>
-    <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
     </row>
-    <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
     </row>
-    <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
     </row>
-    <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
     </row>
-    <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
     </row>
-    <row r="62" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
     </row>
-    <row r="63" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
     </row>
-    <row r="64" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
     </row>
-    <row r="65" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
     </row>
-    <row r="66" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
     </row>
-    <row r="67" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
     </row>
-    <row r="68" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
     </row>
-    <row r="69" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
     </row>
-    <row r="70" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
     </row>
-    <row r="71" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
     </row>
-    <row r="72" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
     </row>
-    <row r="74" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
     </row>
-    <row r="75" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
     </row>
-    <row r="76" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
     </row>
-    <row r="77" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
     </row>
-    <row r="78" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
     </row>
-    <row r="79" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
     </row>
-    <row r="80" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
     </row>
-    <row r="81" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
     </row>
-    <row r="82" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
     </row>
-    <row r="83" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
     </row>
-    <row r="84" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
     </row>
-    <row r="85" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
     </row>
-    <row r="86" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
     </row>
-    <row r="87" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
     </row>
-    <row r="88" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
     </row>
-    <row r="89" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
     </row>
-    <row r="90" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
     </row>
-    <row r="91" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
     </row>
-    <row r="92" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
     </row>
-    <row r="93" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
     </row>
-    <row r="94" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
     </row>
-    <row r="95" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
     </row>
-    <row r="96" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
     </row>
-    <row r="97" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
     </row>
-    <row r="98" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
     </row>
-    <row r="99" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
     </row>
-    <row r="100" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
     </row>
-    <row r="101" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
     </row>
-    <row r="102" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
     </row>
-    <row r="103" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
     </row>
-    <row r="104" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
     </row>
-    <row r="105" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
     </row>
-    <row r="106" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
     </row>
-    <row r="107" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
     </row>
-    <row r="108" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
     </row>
-    <row r="109" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
     </row>
-    <row r="110" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
     </row>
-    <row r="111" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
     </row>
-    <row r="112" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
     </row>
-    <row r="113" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
     </row>
-    <row r="114" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
     </row>
-    <row r="115" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
     </row>
-    <row r="116" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
     </row>
-    <row r="117" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
     </row>
-    <row r="118" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
     </row>
-    <row r="119" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
     </row>
-    <row r="120" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
     </row>
-    <row r="121" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
     </row>
-    <row r="122" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
     </row>
-    <row r="123" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
     </row>
-    <row r="124" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
     </row>
-    <row r="125" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
     </row>
-    <row r="126" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
     </row>
-    <row r="127" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
     </row>
-    <row r="128" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
     </row>
-    <row r="129" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
     </row>
-    <row r="130" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
     </row>
-    <row r="131" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
     </row>
-    <row r="132" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
     </row>
-    <row r="133" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
     </row>
-    <row r="134" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
     </row>
-    <row r="135" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
     </row>
-    <row r="136" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
     </row>
-    <row r="137" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
     </row>
-    <row r="138" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
     </row>
-    <row r="139" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
     </row>
-    <row r="140" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
     </row>
-    <row r="141" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
     </row>
-    <row r="142" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
     </row>
-    <row r="143" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
     </row>
-    <row r="144" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
     </row>
-    <row r="145" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
     </row>
-    <row r="146" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
     </row>
-    <row r="147" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
     </row>
-    <row r="148" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
     </row>
-    <row r="149" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
     </row>
-    <row r="150" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
     </row>
-    <row r="151" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
     </row>
-    <row r="152" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
     </row>
-    <row r="153" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
     </row>
-    <row r="154" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
     </row>
-    <row r="155" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
     </row>
-    <row r="156" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
     </row>
-    <row r="157" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
     </row>
-    <row r="158" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
     </row>
-    <row r="159" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
     </row>
-    <row r="160" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
     </row>
-    <row r="161" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="2"/>
       <c r="B161" s="2"/>
     </row>
-    <row r="162" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
     </row>
-    <row r="163" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="2"/>
       <c r="B163" s="2"/>
     </row>
-    <row r="164" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="2"/>
       <c r="B164" s="2"/>
     </row>
-    <row r="165" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="2"/>
       <c r="B165" s="2"/>
     </row>
-    <row r="166" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="2"/>
       <c r="B166" s="2"/>
     </row>
-    <row r="167" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="2"/>
       <c r="B167" s="2"/>
     </row>
-    <row r="168" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="2"/>
       <c r="B168" s="2"/>
     </row>
-    <row r="169" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="2"/>
       <c r="B169" s="2"/>
     </row>
-    <row r="170" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="2"/>
       <c r="B170" s="2"/>
     </row>
-    <row r="171" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="2"/>
       <c r="B171" s="2"/>
     </row>
-    <row r="172" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="2"/>
       <c r="B172" s="2"/>
     </row>
-    <row r="173" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
     </row>
-    <row r="174" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="2"/>
       <c r="B174" s="2"/>
     </row>
-    <row r="175" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
     </row>
-    <row r="176" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
     </row>
-    <row r="177" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
     </row>
-    <row r="178" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
     </row>
-    <row r="179" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
     </row>
-    <row r="180" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
     </row>
-    <row r="181" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
     </row>
-    <row r="182" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
     </row>
-    <row r="183" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
     </row>
-    <row r="184" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
     </row>
-    <row r="185" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="2"/>
       <c r="B185" s="2"/>
     </row>
-    <row r="186" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
     </row>
-    <row r="187" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
     </row>
-    <row r="188" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
     </row>
-    <row r="189" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="2"/>
       <c r="B189" s="2"/>
     </row>
-    <row r="190" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="2"/>
       <c r="B190" s="2"/>
     </row>
-    <row r="191" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="2"/>
       <c r="B191" s="2"/>
     </row>
-    <row r="192" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="2"/>
       <c r="B192" s="2"/>
     </row>
-    <row r="193" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="2"/>
       <c r="B193" s="2"/>
     </row>
-    <row r="194" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="2"/>
       <c r="B194" s="2"/>
     </row>
-    <row r="195" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="2"/>
       <c r="B195" s="2"/>
     </row>
-    <row r="196" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="2"/>
       <c r="B196" s="2"/>
     </row>
-    <row r="197" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="2"/>
       <c r="B197" s="2"/>
     </row>
-    <row r="198" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="2"/>
       <c r="B198" s="2"/>
     </row>
-    <row r="199" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="2"/>
       <c r="B199" s="2"/>
     </row>
-    <row r="200" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="2"/>
       <c r="B200" s="2"/>
     </row>
-    <row r="201" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="2"/>
       <c r="B201" s="2"/>
     </row>
-    <row r="202" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="2"/>
       <c r="B202" s="2"/>
     </row>
-    <row r="203" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="2"/>
       <c r="B203" s="2"/>
     </row>
-    <row r="204" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="2"/>
       <c r="B204" s="2"/>
     </row>
-    <row r="205" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="2"/>
       <c r="B205" s="2"/>
     </row>
-    <row r="206" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="2"/>
       <c r="B206" s="2"/>
     </row>
-    <row r="207" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="2"/>
       <c r="B207" s="2"/>
     </row>
-    <row r="208" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="2"/>
       <c r="B208" s="2"/>
     </row>
-    <row r="209" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="2"/>
       <c r="B209" s="2"/>
     </row>
-    <row r="210" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="2"/>
       <c r="B210" s="2"/>
     </row>
-    <row r="211" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="2"/>
       <c r="B211" s="2"/>
     </row>
-    <row r="212" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2"/>
       <c r="B212" s="2"/>
     </row>
-    <row r="213" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="2"/>
       <c r="B213" s="2"/>
     </row>
-    <row r="214" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="2"/>
       <c r="B214" s="2"/>
     </row>
-    <row r="215" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="2"/>
       <c r="B215" s="2"/>
     </row>
-    <row r="216" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="2"/>
       <c r="B216" s="2"/>
     </row>
-    <row r="217" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="2"/>
       <c r="B217" s="2"/>
     </row>
-    <row r="218" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="2"/>
       <c r="B218" s="2"/>
     </row>
-    <row r="219" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="2"/>
       <c r="B219" s="2"/>
     </row>
-    <row r="220" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="2"/>
       <c r="B220" s="2"/>
     </row>
-    <row r="221" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="2"/>
       <c r="B221" s="2"/>
     </row>
-    <row r="222" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="2"/>
       <c r="B222" s="2"/>
     </row>
-    <row r="223" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="2"/>
       <c r="B223" s="2"/>
     </row>
-    <row r="224" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="2"/>
       <c r="B224" s="2"/>
     </row>
-    <row r="225" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="2"/>
       <c r="B225" s="2"/>
     </row>
-    <row r="226" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="2"/>
       <c r="B226" s="2"/>
     </row>
-    <row r="227" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="2"/>
       <c r="B227" s="2"/>
     </row>
-    <row r="228" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="2"/>
       <c r="B228" s="2"/>
     </row>
-    <row r="229" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="2"/>
       <c r="B229" s="2"/>
     </row>
-    <row r="230" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="2"/>
       <c r="B230" s="2"/>
     </row>
-    <row r="231" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="2"/>
       <c r="B231" s="2"/>
     </row>
-    <row r="232" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="2"/>
       <c r="B232" s="2"/>
     </row>
-    <row r="233" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="2"/>
       <c r="B233" s="2"/>
     </row>
-    <row r="234" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="2"/>
       <c r="B234" s="2"/>
     </row>
-    <row r="235" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="2"/>
       <c r="B235" s="2"/>
     </row>
-    <row r="236" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="2"/>
       <c r="B236" s="2"/>
     </row>
-    <row r="237" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="2"/>
       <c r="B237" s="2"/>
     </row>
-    <row r="238" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="2"/>
       <c r="B238" s="2"/>
     </row>
-    <row r="239" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="2"/>
       <c r="B239" s="2"/>
     </row>
-    <row r="240" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="2"/>
       <c r="B240" s="2"/>
     </row>
-    <row r="241" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="2"/>
       <c r="B241" s="2"/>
     </row>
-    <row r="242" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="2"/>
       <c r="B242" s="2"/>
     </row>
-    <row r="243" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="2"/>
       <c r="B243" s="2"/>
     </row>
-    <row r="244" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="2"/>
       <c r="B244" s="2"/>
     </row>
-    <row r="245" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="2"/>
       <c r="B245" s="2"/>
     </row>
-    <row r="246" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="2"/>
       <c r="B246" s="2"/>
     </row>
-    <row r="247" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="2"/>
       <c r="B247" s="2"/>
     </row>
-    <row r="248" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="2"/>
       <c r="B248" s="2"/>
     </row>
-    <row r="249" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="2"/>
       <c r="B249" s="2"/>
     </row>

</xml_diff>

<commit_message>
Update RTM with UI Design ID of Register
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI9M-Testing\Core\QA\WorkShop\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC9739A-7DB2-4ACE-A29E-9B43F836BE11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8002942-1225-4C59-B1CF-FE642DBA0FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="109">
   <si>
     <t>SRS ID</t>
   </si>
@@ -316,6 +316,48 @@
   </si>
   <si>
     <t>TC_Client_018</t>
+  </si>
+  <si>
+    <t>UI Design ID</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_001</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_002</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_003</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_004</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_005</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_006</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_007</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_008</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_009</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_010</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_011</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_012</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_013</t>
   </si>
 </sst>
 </file>
@@ -666,155 +708,207 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B249"/>
+  <dimension ref="A1:C249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.88671875" customWidth="1"/>
     <col min="2" max="2" width="37.44140625" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>44</v>
       </c>
@@ -822,23 +916,29 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>2</v>
       </c>
@@ -846,7 +946,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>3</v>
       </c>
@@ -854,7 +954,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>4</v>
       </c>
@@ -862,7 +962,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>5</v>
       </c>
@@ -870,7 +970,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>6</v>
       </c>
@@ -878,7 +978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>48</v>
       </c>
@@ -886,7 +986,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>50</v>
       </c>
@@ -894,7 +994,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>52</v>
       </c>
@@ -902,7 +1002,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>54</v>
       </c>
@@ -910,7 +1010,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>56</v>
       </c>
@@ -918,7 +1018,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>57</v>
       </c>
@@ -926,7 +1026,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
add checkout wire frame and connect it with TC in RTM
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\RTM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D5869D-B6FD-4C35-9DA7-F9675C6B1CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18EFDDD6-FF51-4EC7-A042-4482670C7EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="114">
   <si>
     <t>SRS ID</t>
   </si>
@@ -368,6 +368,12 @@
   <si>
     <t>WireFrame_Client_002
 WireFrame_Client_003</t>
+  </si>
+  <si>
+    <t>Wireframe_Checkout_001</t>
+  </si>
+  <si>
+    <t>Wireframe_Checkout_002</t>
   </si>
 </sst>
 </file>
@@ -754,18 +760,18 @@
   </sheetPr>
   <dimension ref="A1:C249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.81640625" customWidth="1"/>
+    <col min="2" max="2" width="37.453125" customWidth="1"/>
+    <col min="3" max="3" width="45.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -776,7 +782,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -787,7 +793,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -798,7 +804,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -809,7 +815,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -820,7 +826,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -831,7 +837,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -842,7 +848,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -853,7 +859,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
@@ -864,7 +870,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
@@ -875,7 +881,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
@@ -886,7 +892,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
@@ -897,7 +903,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>34</v>
       </c>
@@ -908,7 +914,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>36</v>
       </c>
@@ -919,7 +925,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>38</v>
       </c>
@@ -930,7 +936,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>40</v>
       </c>
@@ -941,7 +947,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
@@ -952,7 +958,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>44</v>
       </c>
@@ -961,7 +967,7 @@
       </c>
       <c r="C18" s="13"/>
     </row>
-    <row r="19" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>46</v>
       </c>
@@ -972,7 +978,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>47</v>
       </c>
@@ -983,7 +989,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>2</v>
       </c>
@@ -994,7 +1000,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
         <v>3</v>
       </c>
@@ -1003,7 +1009,7 @@
       </c>
       <c r="C22" s="13"/>
     </row>
-    <row r="23" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
         <v>4</v>
       </c>
@@ -1012,7 +1018,7 @@
       </c>
       <c r="C23" s="13"/>
     </row>
-    <row r="24" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
@@ -1021,7 +1027,7 @@
       </c>
       <c r="C24" s="13"/>
     </row>
-    <row r="25" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="s">
         <v>6</v>
       </c>
@@ -1030,7 +1036,7 @@
       </c>
       <c r="C25" s="13"/>
     </row>
-    <row r="26" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
         <v>48</v>
       </c>
@@ -1039,7 +1045,7 @@
       </c>
       <c r="C26" s="13"/>
     </row>
-    <row r="27" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="4" t="s">
         <v>50</v>
       </c>
@@ -1048,7 +1054,7 @@
       </c>
       <c r="C27" s="13"/>
     </row>
-    <row r="28" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
         <v>52</v>
       </c>
@@ -1057,7 +1063,7 @@
       </c>
       <c r="C28" s="13"/>
     </row>
-    <row r="29" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="s">
         <v>54</v>
       </c>
@@ -1066,7 +1072,7 @@
       </c>
       <c r="C29" s="13"/>
     </row>
-    <row r="30" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="4" t="s">
         <v>56</v>
       </c>
@@ -1075,7 +1081,7 @@
       </c>
       <c r="C30" s="13"/>
     </row>
-    <row r="31" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="4" t="s">
         <v>57</v>
       </c>
@@ -1084,7 +1090,7 @@
       </c>
       <c r="C31" s="13"/>
     </row>
-    <row r="32" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="4" t="s">
         <v>59</v>
       </c>
@@ -1093,7 +1099,7 @@
       </c>
       <c r="C32" s="13"/>
     </row>
-    <row r="33" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="4" t="s">
         <v>61</v>
       </c>
@@ -1102,7 +1108,7 @@
       </c>
       <c r="C33" s="13"/>
     </row>
-    <row r="34" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="4" t="s">
         <v>63</v>
       </c>
@@ -1111,7 +1117,7 @@
       </c>
       <c r="C34" s="13"/>
     </row>
-    <row r="35" spans="1:3" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="76.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="4" t="s">
         <v>65</v>
       </c>
@@ -1120,7 +1126,7 @@
       </c>
       <c r="C35" s="13"/>
     </row>
-    <row r="36" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="4" t="s">
         <v>67</v>
       </c>
@@ -1129,7 +1135,7 @@
       </c>
       <c r="C36" s="13"/>
     </row>
-    <row r="37" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="4" t="s">
         <v>68</v>
       </c>
@@ -1138,7 +1144,7 @@
       </c>
       <c r="C37" s="13"/>
     </row>
-    <row r="38" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="4" t="s">
         <v>69</v>
       </c>
@@ -1147,7 +1153,7 @@
       </c>
       <c r="C38" s="13"/>
     </row>
-    <row r="39" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A39" s="4" t="s">
         <v>70</v>
       </c>
@@ -1156,7 +1162,7 @@
       </c>
       <c r="C39" s="13"/>
     </row>
-    <row r="40" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A40" s="4" t="s">
         <v>71</v>
       </c>
@@ -1167,7 +1173,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A41" s="4" t="s">
         <v>72</v>
       </c>
@@ -1178,7 +1184,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A42" s="4" t="s">
         <v>73</v>
       </c>
@@ -1187,7 +1193,7 @@
       </c>
       <c r="C42" s="13"/>
     </row>
-    <row r="43" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A43" s="4" t="s">
         <v>74</v>
       </c>
@@ -1196,7 +1202,7 @@
       </c>
       <c r="C43" s="13"/>
     </row>
-    <row r="44" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A44" s="4" t="s">
         <v>75</v>
       </c>
@@ -1205,7 +1211,7 @@
       </c>
       <c r="C44" s="13"/>
     </row>
-    <row r="45" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A45" s="4" t="s">
         <v>76</v>
       </c>
@@ -1214,7 +1220,7 @@
       </c>
       <c r="C45" s="13"/>
     </row>
-    <row r="46" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A46" s="4" t="s">
         <v>77</v>
       </c>
@@ -1223,25 +1229,29 @@
       </c>
       <c r="C46" s="13"/>
     </row>
-    <row r="47" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="37" x14ac:dyDescent="0.45">
       <c r="A47" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="13"/>
-    </row>
-    <row r="48" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C47" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A48" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C48" s="13"/>
-    </row>
-    <row r="49" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A49" s="4" t="s">
         <v>80</v>
       </c>
@@ -1250,7 +1260,7 @@
       </c>
       <c r="C49" s="13"/>
     </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="4" t="s">
         <v>81</v>
       </c>
@@ -1259,997 +1269,997 @@
       </c>
       <c r="C50" s="13"/>
     </row>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="4"/>
       <c r="B51" s="7"/>
       <c r="C51" s="13"/>
     </row>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="4"/>
       <c r="B52" s="7"/>
       <c r="C52" s="13"/>
     </row>
-    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="4"/>
       <c r="B53" s="7"/>
       <c r="C53" s="13"/>
     </row>
-    <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
       <c r="B54" s="11"/>
       <c r="C54" s="13"/>
     </row>
-    <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="2"/>
       <c r="B55" s="11"/>
       <c r="C55" s="13"/>
     </row>
-    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="2"/>
       <c r="B56" s="11"/>
       <c r="C56" s="13"/>
     </row>
-    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="2"/>
       <c r="B57" s="11"/>
       <c r="C57" s="13"/>
     </row>
-    <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="2"/>
       <c r="B58" s="11"/>
       <c r="C58" s="13"/>
     </row>
-    <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="2"/>
       <c r="B59" s="11"/>
       <c r="C59" s="13"/>
     </row>
-    <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="2"/>
       <c r="B60" s="11"/>
       <c r="C60" s="13"/>
     </row>
-    <row r="61" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="2"/>
       <c r="B61" s="11"/>
       <c r="C61" s="13"/>
     </row>
-    <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="2"/>
       <c r="B62" s="11"/>
       <c r="C62" s="13"/>
     </row>
-    <row r="63" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="2"/>
       <c r="B63" s="11"/>
       <c r="C63" s="13"/>
     </row>
-    <row r="64" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="2"/>
       <c r="B64" s="11"/>
       <c r="C64" s="13"/>
     </row>
-    <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="2"/>
       <c r="B65" s="11"/>
       <c r="C65" s="13"/>
     </row>
-    <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="2"/>
       <c r="B66" s="11"/>
       <c r="C66" s="13"/>
     </row>
-    <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="2"/>
       <c r="B67" s="11"/>
       <c r="C67" s="13"/>
     </row>
-    <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="2"/>
       <c r="B68" s="11"/>
       <c r="C68" s="13"/>
     </row>
-    <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="2"/>
       <c r="B69" s="11"/>
       <c r="C69" s="13"/>
     </row>
-    <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="2"/>
       <c r="B70" s="11"/>
       <c r="C70" s="13"/>
     </row>
-    <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="2"/>
       <c r="B71" s="11"/>
       <c r="C71" s="13"/>
     </row>
-    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="2"/>
       <c r="B72" s="11"/>
       <c r="C72" s="13"/>
     </row>
-    <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="2"/>
       <c r="B73" s="11"/>
       <c r="C73" s="13"/>
     </row>
-    <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="2"/>
       <c r="B74" s="11"/>
       <c r="C74" s="13"/>
     </row>
-    <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="2"/>
       <c r="B75" s="11"/>
       <c r="C75" s="13"/>
     </row>
-    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="2"/>
       <c r="B76" s="11"/>
       <c r="C76" s="13"/>
     </row>
-    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="2"/>
       <c r="B77" s="11"/>
       <c r="C77" s="13"/>
     </row>
-    <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="2"/>
       <c r="B78" s="11"/>
       <c r="C78" s="13"/>
     </row>
-    <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="2"/>
       <c r="B79" s="11"/>
       <c r="C79" s="13"/>
     </row>
-    <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="2"/>
       <c r="B80" s="11"/>
       <c r="C80" s="13"/>
     </row>
-    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="2"/>
       <c r="B81" s="11"/>
       <c r="C81" s="13"/>
     </row>
-    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="2"/>
       <c r="B82" s="11"/>
       <c r="C82" s="13"/>
     </row>
-    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="2"/>
       <c r="B83" s="11"/>
       <c r="C83" s="13"/>
     </row>
-    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
       <c r="B84" s="11"/>
       <c r="C84" s="13"/>
     </row>
-    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="2"/>
       <c r="B85" s="11"/>
       <c r="C85" s="13"/>
     </row>
-    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="2"/>
       <c r="B86" s="11"/>
       <c r="C86" s="13"/>
     </row>
-    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="2"/>
       <c r="B87" s="11"/>
       <c r="C87" s="13"/>
     </row>
-    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="2"/>
       <c r="B88" s="11"/>
       <c r="C88" s="13"/>
     </row>
-    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="2"/>
       <c r="B89" s="11"/>
       <c r="C89" s="13"/>
     </row>
-    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="2"/>
       <c r="B90" s="11"/>
       <c r="C90" s="13"/>
     </row>
-    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="2"/>
       <c r="B91" s="11"/>
       <c r="C91" s="13"/>
     </row>
-    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="2"/>
       <c r="B92" s="11"/>
       <c r="C92" s="13"/>
     </row>
-    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="2"/>
       <c r="B93" s="11"/>
       <c r="C93" s="13"/>
     </row>
-    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="2"/>
       <c r="B94" s="11"/>
       <c r="C94" s="13"/>
     </row>
-    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
       <c r="B95" s="11"/>
       <c r="C95" s="13"/>
     </row>
-    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="2"/>
       <c r="B96" s="11"/>
       <c r="C96" s="13"/>
     </row>
-    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="2"/>
       <c r="B97" s="11"/>
       <c r="C97" s="13"/>
     </row>
-    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="2"/>
       <c r="B98" s="11"/>
       <c r="C98" s="13"/>
     </row>
-    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="2"/>
       <c r="B99" s="11"/>
       <c r="C99" s="13"/>
     </row>
-    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="2"/>
       <c r="B100" s="11"/>
       <c r="C100" s="13"/>
     </row>
-    <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="2"/>
       <c r="B101" s="11"/>
       <c r="C101" s="13"/>
     </row>
-    <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="2"/>
       <c r="B102" s="11"/>
       <c r="C102" s="13"/>
     </row>
-    <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="2"/>
       <c r="B103" s="11"/>
       <c r="C103" s="13"/>
     </row>
-    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="2"/>
       <c r="B104" s="11"/>
       <c r="C104" s="13"/>
     </row>
-    <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="2"/>
       <c r="B105" s="11"/>
       <c r="C105" s="13"/>
     </row>
-    <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="2"/>
       <c r="B106" s="11"/>
       <c r="C106" s="13"/>
     </row>
-    <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="2"/>
       <c r="B107" s="11"/>
       <c r="C107" s="13"/>
     </row>
-    <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="2"/>
       <c r="B108" s="11"/>
       <c r="C108" s="13"/>
     </row>
-    <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="2"/>
       <c r="B109" s="11"/>
       <c r="C109" s="13"/>
     </row>
-    <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="2"/>
       <c r="B110" s="11"/>
       <c r="C110" s="13"/>
     </row>
-    <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="2"/>
       <c r="B111" s="11"/>
       <c r="C111" s="13"/>
     </row>
-    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="2"/>
       <c r="B112" s="11"/>
       <c r="C112" s="13"/>
     </row>
-    <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="2"/>
       <c r="B113" s="11"/>
       <c r="C113" s="13"/>
     </row>
-    <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="2"/>
       <c r="B114" s="11"/>
       <c r="C114" s="13"/>
     </row>
-    <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="2"/>
       <c r="B115" s="11"/>
       <c r="C115" s="13"/>
     </row>
-    <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="2"/>
       <c r="B116" s="11"/>
       <c r="C116" s="13"/>
     </row>
-    <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="2"/>
       <c r="B117" s="11"/>
       <c r="C117" s="13"/>
     </row>
-    <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="2"/>
       <c r="B118" s="11"/>
       <c r="C118" s="13"/>
     </row>
-    <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="2"/>
       <c r="B119" s="11"/>
       <c r="C119" s="13"/>
     </row>
-    <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="2"/>
       <c r="B120" s="11"/>
       <c r="C120" s="13"/>
     </row>
-    <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="2"/>
       <c r="B121" s="11"/>
       <c r="C121" s="13"/>
     </row>
-    <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="2"/>
       <c r="B122" s="11"/>
       <c r="C122" s="13"/>
     </row>
-    <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="2"/>
       <c r="B123" s="11"/>
       <c r="C123" s="13"/>
     </row>
-    <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="2"/>
       <c r="B124" s="11"/>
       <c r="C124" s="13"/>
     </row>
-    <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="2"/>
       <c r="B125" s="11"/>
       <c r="C125" s="13"/>
     </row>
-    <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="2"/>
       <c r="B126" s="11"/>
       <c r="C126" s="13"/>
     </row>
-    <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="2"/>
       <c r="B127" s="11"/>
       <c r="C127" s="13"/>
     </row>
-    <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="2"/>
       <c r="B128" s="11"/>
       <c r="C128" s="13"/>
     </row>
-    <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="2"/>
       <c r="B129" s="11"/>
       <c r="C129" s="13"/>
     </row>
-    <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="2"/>
       <c r="B130" s="11"/>
       <c r="C130" s="13"/>
     </row>
-    <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="2"/>
       <c r="B131" s="11"/>
       <c r="C131" s="13"/>
     </row>
-    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="2"/>
       <c r="B132" s="11"/>
       <c r="C132" s="13"/>
     </row>
-    <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="2"/>
       <c r="B133" s="11"/>
       <c r="C133" s="13"/>
     </row>
-    <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" s="2"/>
       <c r="B134" s="11"/>
       <c r="C134" s="13"/>
     </row>
-    <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" s="2"/>
       <c r="B135" s="11"/>
       <c r="C135" s="13"/>
     </row>
-    <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="2"/>
       <c r="B136" s="11"/>
       <c r="C136" s="13"/>
     </row>
-    <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="2"/>
       <c r="B137" s="11"/>
       <c r="C137" s="13"/>
     </row>
-    <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="2"/>
       <c r="B138" s="11"/>
       <c r="C138" s="13"/>
     </row>
-    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="2"/>
       <c r="B139" s="11"/>
       <c r="C139" s="13"/>
     </row>
-    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="2"/>
       <c r="B140" s="11"/>
       <c r="C140" s="13"/>
     </row>
-    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" s="2"/>
       <c r="B141" s="11"/>
       <c r="C141" s="13"/>
     </row>
-    <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" s="2"/>
       <c r="B142" s="11"/>
       <c r="C142" s="13"/>
     </row>
-    <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" s="2"/>
       <c r="B143" s="11"/>
       <c r="C143" s="13"/>
     </row>
-    <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" s="2"/>
       <c r="B144" s="11"/>
       <c r="C144" s="13"/>
     </row>
-    <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" s="2"/>
       <c r="B145" s="11"/>
       <c r="C145" s="13"/>
     </row>
-    <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" s="2"/>
       <c r="B146" s="11"/>
       <c r="C146" s="13"/>
     </row>
-    <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" s="2"/>
       <c r="B147" s="11"/>
       <c r="C147" s="13"/>
     </row>
-    <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" s="2"/>
       <c r="B148" s="11"/>
       <c r="C148" s="13"/>
     </row>
-    <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" s="2"/>
       <c r="B149" s="11"/>
       <c r="C149" s="13"/>
     </row>
-    <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" s="2"/>
       <c r="B150" s="11"/>
       <c r="C150" s="13"/>
     </row>
-    <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" s="2"/>
       <c r="B151" s="11"/>
       <c r="C151" s="13"/>
     </row>
-    <row r="152" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" s="2"/>
       <c r="B152" s="11"/>
       <c r="C152" s="13"/>
     </row>
-    <row r="153" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" s="2"/>
       <c r="B153" s="11"/>
       <c r="C153" s="13"/>
     </row>
-    <row r="154" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" s="2"/>
       <c r="B154" s="11"/>
       <c r="C154" s="13"/>
     </row>
-    <row r="155" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" s="2"/>
       <c r="B155" s="11"/>
       <c r="C155" s="13"/>
     </row>
-    <row r="156" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" s="2"/>
       <c r="B156" s="11"/>
       <c r="C156" s="13"/>
     </row>
-    <row r="157" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" s="2"/>
       <c r="B157" s="11"/>
       <c r="C157" s="13"/>
     </row>
-    <row r="158" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" s="2"/>
       <c r="B158" s="11"/>
       <c r="C158" s="13"/>
     </row>
-    <row r="159" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="2"/>
       <c r="B159" s="11"/>
       <c r="C159" s="13"/>
     </row>
-    <row r="160" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" s="2"/>
       <c r="B160" s="11"/>
       <c r="C160" s="13"/>
     </row>
-    <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="2"/>
       <c r="B161" s="11"/>
       <c r="C161" s="13"/>
     </row>
-    <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" s="2"/>
       <c r="B162" s="11"/>
       <c r="C162" s="13"/>
     </row>
-    <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" s="2"/>
       <c r="B163" s="11"/>
       <c r="C163" s="13"/>
     </row>
-    <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" s="2"/>
       <c r="B164" s="11"/>
       <c r="C164" s="13"/>
     </row>
-    <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" s="2"/>
       <c r="B165" s="11"/>
       <c r="C165" s="13"/>
     </row>
-    <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" s="2"/>
       <c r="B166" s="11"/>
       <c r="C166" s="13"/>
     </row>
-    <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" s="2"/>
       <c r="B167" s="11"/>
       <c r="C167" s="13"/>
     </row>
-    <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" s="2"/>
       <c r="B168" s="11"/>
       <c r="C168" s="13"/>
     </row>
-    <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" s="2"/>
       <c r="B169" s="11"/>
       <c r="C169" s="13"/>
     </row>
-    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" s="2"/>
       <c r="B170" s="11"/>
       <c r="C170" s="13"/>
     </row>
-    <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" s="2"/>
       <c r="B171" s="11"/>
       <c r="C171" s="13"/>
     </row>
-    <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" s="2"/>
       <c r="B172" s="11"/>
       <c r="C172" s="13"/>
     </row>
-    <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" s="2"/>
       <c r="B173" s="11"/>
       <c r="C173" s="13"/>
     </row>
-    <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" s="2"/>
       <c r="B174" s="11"/>
       <c r="C174" s="13"/>
     </row>
-    <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" s="2"/>
       <c r="B175" s="11"/>
       <c r="C175" s="13"/>
     </row>
-    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" s="2"/>
       <c r="B176" s="11"/>
       <c r="C176" s="13"/>
     </row>
-    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" s="2"/>
       <c r="B177" s="11"/>
       <c r="C177" s="13"/>
     </row>
-    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" s="2"/>
       <c r="B178" s="11"/>
       <c r="C178" s="13"/>
     </row>
-    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" s="2"/>
       <c r="B179" s="11"/>
       <c r="C179" s="13"/>
     </row>
-    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" s="2"/>
       <c r="B180" s="11"/>
       <c r="C180" s="13"/>
     </row>
-    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" s="2"/>
       <c r="B181" s="11"/>
       <c r="C181" s="13"/>
     </row>
-    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" s="2"/>
       <c r="B182" s="11"/>
       <c r="C182" s="13"/>
     </row>
-    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" s="2"/>
       <c r="B183" s="11"/>
       <c r="C183" s="13"/>
     </row>
-    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" s="2"/>
       <c r="B184" s="11"/>
       <c r="C184" s="13"/>
     </row>
-    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" s="2"/>
       <c r="B185" s="11"/>
       <c r="C185" s="13"/>
     </row>
-    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" s="2"/>
       <c r="B186" s="11"/>
       <c r="C186" s="13"/>
     </row>
-    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" s="2"/>
       <c r="B187" s="11"/>
       <c r="C187" s="13"/>
     </row>
-    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" s="2"/>
       <c r="B188" s="11"/>
       <c r="C188" s="13"/>
     </row>
-    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" s="2"/>
       <c r="B189" s="11"/>
       <c r="C189" s="13"/>
     </row>
-    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" s="2"/>
       <c r="B190" s="11"/>
       <c r="C190" s="13"/>
     </row>
-    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" s="2"/>
       <c r="B191" s="11"/>
       <c r="C191" s="13"/>
     </row>
-    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" s="2"/>
       <c r="B192" s="11"/>
       <c r="C192" s="13"/>
     </row>
-    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" s="2"/>
       <c r="B193" s="11"/>
       <c r="C193" s="13"/>
     </row>
-    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" s="2"/>
       <c r="B194" s="11"/>
       <c r="C194" s="13"/>
     </row>
-    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A195" s="2"/>
       <c r="B195" s="11"/>
       <c r="C195" s="13"/>
     </row>
-    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A196" s="2"/>
       <c r="B196" s="11"/>
       <c r="C196" s="13"/>
     </row>
-    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A197" s="2"/>
       <c r="B197" s="11"/>
       <c r="C197" s="13"/>
     </row>
-    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" s="2"/>
       <c r="B198" s="11"/>
       <c r="C198" s="13"/>
     </row>
-    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A199" s="2"/>
       <c r="B199" s="11"/>
       <c r="C199" s="13"/>
     </row>
-    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A200" s="2"/>
       <c r="B200" s="11"/>
       <c r="C200" s="13"/>
     </row>
-    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A201" s="2"/>
       <c r="B201" s="11"/>
       <c r="C201" s="13"/>
     </row>
-    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A202" s="2"/>
       <c r="B202" s="11"/>
       <c r="C202" s="13"/>
     </row>
-    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A203" s="2"/>
       <c r="B203" s="11"/>
       <c r="C203" s="13"/>
     </row>
-    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A204" s="2"/>
       <c r="B204" s="11"/>
       <c r="C204" s="13"/>
     </row>
-    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A205" s="2"/>
       <c r="B205" s="11"/>
       <c r="C205" s="13"/>
     </row>
-    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A206" s="2"/>
       <c r="B206" s="11"/>
       <c r="C206" s="13"/>
     </row>
-    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A207" s="2"/>
       <c r="B207" s="11"/>
       <c r="C207" s="13"/>
     </row>
-    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A208" s="2"/>
       <c r="B208" s="11"/>
       <c r="C208" s="13"/>
     </row>
-    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A209" s="2"/>
       <c r="B209" s="11"/>
       <c r="C209" s="13"/>
     </row>
-    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A210" s="2"/>
       <c r="B210" s="11"/>
       <c r="C210" s="13"/>
     </row>
-    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A211" s="2"/>
       <c r="B211" s="11"/>
       <c r="C211" s="13"/>
     </row>
-    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A212" s="2"/>
       <c r="B212" s="11"/>
       <c r="C212" s="13"/>
     </row>
-    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A213" s="2"/>
       <c r="B213" s="11"/>
       <c r="C213" s="13"/>
     </row>
-    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A214" s="2"/>
       <c r="B214" s="11"/>
       <c r="C214" s="13"/>
     </row>
-    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A215" s="2"/>
       <c r="B215" s="11"/>
       <c r="C215" s="13"/>
     </row>
-    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A216" s="2"/>
       <c r="B216" s="11"/>
       <c r="C216" s="13"/>
     </row>
-    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A217" s="2"/>
       <c r="B217" s="11"/>
       <c r="C217" s="13"/>
     </row>
-    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A218" s="2"/>
       <c r="B218" s="11"/>
       <c r="C218" s="13"/>
     </row>
-    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A219" s="2"/>
       <c r="B219" s="11"/>
       <c r="C219" s="13"/>
     </row>
-    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A220" s="2"/>
       <c r="B220" s="11"/>
       <c r="C220" s="13"/>
     </row>
-    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A221" s="2"/>
       <c r="B221" s="11"/>
       <c r="C221" s="13"/>
     </row>
-    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A222" s="2"/>
       <c r="B222" s="11"/>
       <c r="C222" s="13"/>
     </row>
-    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A223" s="2"/>
       <c r="B223" s="11"/>
       <c r="C223" s="13"/>
     </row>
-    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A224" s="2"/>
       <c r="B224" s="11"/>
       <c r="C224" s="13"/>
     </row>
-    <row r="225" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A225" s="2"/>
       <c r="B225" s="11"/>
       <c r="C225" s="13"/>
     </row>
-    <row r="226" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A226" s="2"/>
       <c r="B226" s="11"/>
       <c r="C226" s="13"/>
     </row>
-    <row r="227" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A227" s="2"/>
       <c r="B227" s="11"/>
       <c r="C227" s="13"/>
     </row>
-    <row r="228" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A228" s="2"/>
       <c r="B228" s="11"/>
       <c r="C228" s="13"/>
     </row>
-    <row r="229" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A229" s="2"/>
       <c r="B229" s="11"/>
       <c r="C229" s="13"/>
     </row>
-    <row r="230" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A230" s="2"/>
       <c r="B230" s="11"/>
       <c r="C230" s="13"/>
     </row>
-    <row r="231" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A231" s="2"/>
       <c r="B231" s="11"/>
       <c r="C231" s="13"/>
     </row>
-    <row r="232" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A232" s="2"/>
       <c r="B232" s="11"/>
       <c r="C232" s="13"/>
     </row>
-    <row r="233" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A233" s="2"/>
       <c r="B233" s="11"/>
       <c r="C233" s="13"/>
     </row>
-    <row r="234" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A234" s="2"/>
       <c r="B234" s="11"/>
       <c r="C234" s="13"/>
     </row>
-    <row r="235" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A235" s="2"/>
       <c r="B235" s="11"/>
       <c r="C235" s="13"/>
     </row>
-    <row r="236" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A236" s="2"/>
       <c r="B236" s="11"/>
       <c r="C236" s="13"/>
     </row>
-    <row r="237" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A237" s="2"/>
       <c r="B237" s="11"/>
       <c r="C237" s="13"/>
     </row>
-    <row r="238" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A238" s="2"/>
       <c r="B238" s="11"/>
       <c r="C238" s="13"/>
     </row>
-    <row r="239" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A239" s="2"/>
       <c r="B239" s="11"/>
       <c r="C239" s="13"/>
     </row>
-    <row r="240" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A240" s="2"/>
       <c r="B240" s="11"/>
       <c r="C240" s="13"/>
     </row>
-    <row r="241" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A241" s="2"/>
       <c r="B241" s="11"/>
       <c r="C241" s="13"/>
     </row>
-    <row r="242" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A242" s="2"/>
       <c r="B242" s="11"/>
       <c r="C242" s="13"/>
     </row>
-    <row r="243" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A243" s="2"/>
       <c r="B243" s="11"/>
       <c r="C243" s="13"/>
     </row>
-    <row r="244" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A244" s="2"/>
       <c r="B244" s="11"/>
       <c r="C244" s="13"/>
     </row>
-    <row r="245" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A245" s="2"/>
       <c r="B245" s="11"/>
       <c r="C245" s="13"/>
     </row>
-    <row r="246" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A246" s="2"/>
       <c r="B246" s="11"/>
       <c r="C246" s="13"/>
     </row>
-    <row r="247" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A247" s="2"/>
       <c r="B247" s="11"/>
       <c r="C247" s="13"/>
     </row>
-    <row r="248" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A248" s="2"/>
       <c r="B248" s="11"/>
       <c r="C248" s="13"/>
     </row>
-    <row r="249" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A249" s="2"/>
       <c r="B249" s="11"/>
       <c r="C249" s="13"/>

</xml_diff>

<commit_message>
add ui design id to test cases file
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Online-Mobile-Store-WebSite\RTM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI9M-Testing\Core\QA\WorkShop\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18EFDDD6-FF51-4EC7-A042-4482670C7EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9474CDB8-DF2A-412D-8352-D3AA62D8C964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="95">
   <si>
     <t>SRS ID</t>
   </si>
@@ -316,64 +316,6 @@
   </si>
   <si>
     <t>TC_Client_018</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_001</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_002</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_003</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_004</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_005</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_006</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_007</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_008</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_009</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_010</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_011</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_012</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_013</t>
-  </si>
-  <si>
-    <t>WireFrame Design ID</t>
-  </si>
-  <si>
-    <t>WireFrame_Client_001</t>
-  </si>
-  <si>
-    <t>WireFrame_Client_004</t>
-  </si>
-  <si>
-    <t>WireFrame_Client_002
-WireFrame_Client_003</t>
-  </si>
-  <si>
-    <t>Wireframe_Checkout_001</t>
-  </si>
-  <si>
-    <t>Wireframe_Checkout_002</t>
   </si>
 </sst>
 </file>
@@ -510,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -533,13 +475,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,1511 +693,1213 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C249"/>
+  <dimension ref="A1:B249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.81640625" customWidth="1"/>
-    <col min="2" max="2" width="37.453125" customWidth="1"/>
-    <col min="3" max="3" width="45.7265625" customWidth="1"/>
+    <col min="1" max="1" width="23.77734375" customWidth="1"/>
+    <col min="2" max="2" width="37.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="13"/>
-    </row>
-    <row r="19" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="13"/>
-    </row>
-    <row r="23" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="13"/>
-    </row>
-    <row r="24" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="13"/>
-    </row>
-    <row r="25" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="25" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="13"/>
-    </row>
-    <row r="26" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="13"/>
-    </row>
-    <row r="27" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="27" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="13"/>
-    </row>
-    <row r="28" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="28" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="13"/>
-    </row>
-    <row r="29" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="29" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="13"/>
-    </row>
-    <row r="30" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="30" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="13"/>
-    </row>
-    <row r="31" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="31" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="13"/>
-    </row>
-    <row r="32" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="32" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>59</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-    </row>
-    <row r="33" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="33" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="13"/>
-    </row>
-    <row r="34" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="34" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>63</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="13"/>
-    </row>
-    <row r="35" spans="1:3" ht="76.5" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="35" spans="1:2" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>65</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="13"/>
-    </row>
-    <row r="36" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="36" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C36" s="13"/>
-    </row>
-    <row r="37" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="37" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C37" s="13"/>
-    </row>
-    <row r="38" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="38" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C38" s="13"/>
-    </row>
-    <row r="39" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="39" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C39" s="13"/>
-    </row>
-    <row r="40" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="40" spans="1:2" ht="54" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C40" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="41" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>72</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C42" s="13"/>
-    </row>
-    <row r="43" spans="1:3" ht="55.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="43" spans="1:2" ht="54" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C43" s="13"/>
-    </row>
-    <row r="44" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C44" s="13"/>
-    </row>
-    <row r="45" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="13"/>
-    </row>
-    <row r="46" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="46" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>77</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C46" s="13"/>
-    </row>
-    <row r="47" spans="1:3" ht="37" x14ac:dyDescent="0.45">
+    </row>
+    <row r="47" spans="1:2" ht="36" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="48" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C48" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="13"/>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>81</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C50" s="13"/>
-    </row>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4"/>
       <c r="B51" s="7"/>
-      <c r="C51" s="13"/>
-    </row>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="4"/>
       <c r="B52" s="7"/>
-      <c r="C52" s="13"/>
-    </row>
-    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4"/>
       <c r="B53" s="7"/>
-      <c r="C53" s="13"/>
-    </row>
-    <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="11"/>
-      <c r="C54" s="13"/>
-    </row>
-    <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" s="11"/>
-      <c r="C55" s="13"/>
-    </row>
-    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="11"/>
-      <c r="C56" s="13"/>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="11"/>
-      <c r="C57" s="13"/>
-    </row>
-    <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="11"/>
-      <c r="C58" s="13"/>
-    </row>
-    <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="11"/>
-      <c r="C59" s="13"/>
-    </row>
-    <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="11"/>
-      <c r="C60" s="13"/>
-    </row>
-    <row r="61" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="11"/>
-      <c r="C61" s="13"/>
-    </row>
-    <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="11"/>
-      <c r="C62" s="13"/>
-    </row>
-    <row r="63" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="11"/>
-      <c r="C63" s="13"/>
-    </row>
-    <row r="64" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="11"/>
-      <c r="C64" s="13"/>
-    </row>
-    <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="11"/>
-      <c r="C65" s="13"/>
-    </row>
-    <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="11"/>
-      <c r="C66" s="13"/>
-    </row>
-    <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" s="11"/>
-      <c r="C67" s="13"/>
-    </row>
-    <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="68" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" s="11"/>
-      <c r="C68" s="13"/>
-    </row>
-    <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="69" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="11"/>
-      <c r="C69" s="13"/>
-    </row>
-    <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="70" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" s="11"/>
-      <c r="C70" s="13"/>
-    </row>
-    <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="71" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="11"/>
-      <c r="C71" s="13"/>
-    </row>
-    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="72" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="11"/>
-      <c r="C72" s="13"/>
-    </row>
-    <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="73" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="11"/>
-      <c r="C73" s="13"/>
-    </row>
-    <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="74" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="11"/>
-      <c r="C74" s="13"/>
-    </row>
-    <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="75" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="11"/>
-      <c r="C75" s="13"/>
-    </row>
-    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="76" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="11"/>
-      <c r="C76" s="13"/>
-    </row>
-    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="77" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" s="11"/>
-      <c r="C77" s="13"/>
-    </row>
-    <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="78" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" s="11"/>
-      <c r="C78" s="13"/>
-    </row>
-    <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="79" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" s="11"/>
-      <c r="C79" s="13"/>
-    </row>
-    <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="80" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" s="11"/>
-      <c r="C80" s="13"/>
-    </row>
-    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="81" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="B81" s="11"/>
-      <c r="C81" s="13"/>
-    </row>
-    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="82" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
       <c r="B82" s="11"/>
-      <c r="C82" s="13"/>
-    </row>
-    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="83" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2"/>
       <c r="B83" s="11"/>
-      <c r="C83" s="13"/>
-    </row>
-    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="84" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
       <c r="B84" s="11"/>
-      <c r="C84" s="13"/>
-    </row>
-    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="85" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2"/>
       <c r="B85" s="11"/>
-      <c r="C85" s="13"/>
-    </row>
-    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="86" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" s="11"/>
-      <c r="C86" s="13"/>
-    </row>
-    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="87" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
       <c r="B87" s="11"/>
-      <c r="C87" s="13"/>
-    </row>
-    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="88" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
       <c r="B88" s="11"/>
-      <c r="C88" s="13"/>
-    </row>
-    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="89" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" s="11"/>
-      <c r="C89" s="13"/>
-    </row>
-    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="90" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
       <c r="B90" s="11"/>
-      <c r="C90" s="13"/>
-    </row>
-    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="91" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
       <c r="B91" s="11"/>
-      <c r="C91" s="13"/>
-    </row>
-    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="92" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
       <c r="B92" s="11"/>
-      <c r="C92" s="13"/>
-    </row>
-    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="93" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
       <c r="B93" s="11"/>
-      <c r="C93" s="13"/>
-    </row>
-    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="94" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
       <c r="B94" s="11"/>
-      <c r="C94" s="13"/>
-    </row>
-    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="95" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2"/>
       <c r="B95" s="11"/>
-      <c r="C95" s="13"/>
-    </row>
-    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="96" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
       <c r="B96" s="11"/>
-      <c r="C96" s="13"/>
-    </row>
-    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="97" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
       <c r="B97" s="11"/>
-      <c r="C97" s="13"/>
-    </row>
-    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="98" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
       <c r="B98" s="11"/>
-      <c r="C98" s="13"/>
-    </row>
-    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="99" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
       <c r="B99" s="11"/>
-      <c r="C99" s="13"/>
-    </row>
-    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="100" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
       <c r="B100" s="11"/>
-      <c r="C100" s="13"/>
-    </row>
-    <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="101" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
       <c r="B101" s="11"/>
-      <c r="C101" s="13"/>
-    </row>
-    <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="102" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
       <c r="B102" s="11"/>
-      <c r="C102" s="13"/>
-    </row>
-    <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="103" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
       <c r="B103" s="11"/>
-      <c r="C103" s="13"/>
-    </row>
-    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="104" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="B104" s="11"/>
-      <c r="C104" s="13"/>
-    </row>
-    <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="105" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
       <c r="B105" s="11"/>
-      <c r="C105" s="13"/>
-    </row>
-    <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="106" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="B106" s="11"/>
-      <c r="C106" s="13"/>
-    </row>
-    <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="107" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" s="11"/>
-      <c r="C107" s="13"/>
-    </row>
-    <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="108" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
       <c r="B108" s="11"/>
-      <c r="C108" s="13"/>
-    </row>
-    <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="109" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2"/>
       <c r="B109" s="11"/>
-      <c r="C109" s="13"/>
-    </row>
-    <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="110" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="B110" s="11"/>
-      <c r="C110" s="13"/>
-    </row>
-    <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="111" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2"/>
       <c r="B111" s="11"/>
-      <c r="C111" s="13"/>
-    </row>
-    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="112" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
       <c r="B112" s="11"/>
-      <c r="C112" s="13"/>
-    </row>
-    <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="113" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
       <c r="B113" s="11"/>
-      <c r="C113" s="13"/>
-    </row>
-    <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="114" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="B114" s="11"/>
-      <c r="C114" s="13"/>
-    </row>
-    <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="115" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2"/>
       <c r="B115" s="11"/>
-      <c r="C115" s="13"/>
-    </row>
-    <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="116" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2"/>
       <c r="B116" s="11"/>
-      <c r="C116" s="13"/>
-    </row>
-    <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="117" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2"/>
       <c r="B117" s="11"/>
-      <c r="C117" s="13"/>
-    </row>
-    <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="118" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2"/>
       <c r="B118" s="11"/>
-      <c r="C118" s="13"/>
-    </row>
-    <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="119" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2"/>
       <c r="B119" s="11"/>
-      <c r="C119" s="13"/>
-    </row>
-    <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="120" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2"/>
       <c r="B120" s="11"/>
-      <c r="C120" s="13"/>
-    </row>
-    <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="121" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2"/>
       <c r="B121" s="11"/>
-      <c r="C121" s="13"/>
-    </row>
-    <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="122" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2"/>
       <c r="B122" s="11"/>
-      <c r="C122" s="13"/>
-    </row>
-    <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="123" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2"/>
       <c r="B123" s="11"/>
-      <c r="C123" s="13"/>
-    </row>
-    <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="124" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2"/>
       <c r="B124" s="11"/>
-      <c r="C124" s="13"/>
-    </row>
-    <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="125" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2"/>
       <c r="B125" s="11"/>
-      <c r="C125" s="13"/>
-    </row>
-    <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="126" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2"/>
       <c r="B126" s="11"/>
-      <c r="C126" s="13"/>
-    </row>
-    <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="127" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2"/>
       <c r="B127" s="11"/>
-      <c r="C127" s="13"/>
-    </row>
-    <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="128" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2"/>
       <c r="B128" s="11"/>
-      <c r="C128" s="13"/>
-    </row>
-    <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="129" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2"/>
       <c r="B129" s="11"/>
-      <c r="C129" s="13"/>
-    </row>
-    <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="130" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2"/>
       <c r="B130" s="11"/>
-      <c r="C130" s="13"/>
-    </row>
-    <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="131" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2"/>
       <c r="B131" s="11"/>
-      <c r="C131" s="13"/>
-    </row>
-    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="132" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2"/>
       <c r="B132" s="11"/>
-      <c r="C132" s="13"/>
-    </row>
-    <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="133" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2"/>
       <c r="B133" s="11"/>
-      <c r="C133" s="13"/>
-    </row>
-    <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="134" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2"/>
       <c r="B134" s="11"/>
-      <c r="C134" s="13"/>
-    </row>
-    <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="135" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2"/>
       <c r="B135" s="11"/>
-      <c r="C135" s="13"/>
-    </row>
-    <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="136" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2"/>
       <c r="B136" s="11"/>
-      <c r="C136" s="13"/>
-    </row>
-    <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="137" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2"/>
       <c r="B137" s="11"/>
-      <c r="C137" s="13"/>
-    </row>
-    <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="138" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2"/>
       <c r="B138" s="11"/>
-      <c r="C138" s="13"/>
-    </row>
-    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="139" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2"/>
       <c r="B139" s="11"/>
-      <c r="C139" s="13"/>
-    </row>
-    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="140" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2"/>
       <c r="B140" s="11"/>
-      <c r="C140" s="13"/>
-    </row>
-    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="141" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2"/>
       <c r="B141" s="11"/>
-      <c r="C141" s="13"/>
-    </row>
-    <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="142" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2"/>
       <c r="B142" s="11"/>
-      <c r="C142" s="13"/>
-    </row>
-    <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="143" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2"/>
       <c r="B143" s="11"/>
-      <c r="C143" s="13"/>
-    </row>
-    <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="144" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2"/>
       <c r="B144" s="11"/>
-      <c r="C144" s="13"/>
-    </row>
-    <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="145" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2"/>
       <c r="B145" s="11"/>
-      <c r="C145" s="13"/>
-    </row>
-    <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="146" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2"/>
       <c r="B146" s="11"/>
-      <c r="C146" s="13"/>
-    </row>
-    <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="147" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2"/>
       <c r="B147" s="11"/>
-      <c r="C147" s="13"/>
-    </row>
-    <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="148" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2"/>
       <c r="B148" s="11"/>
-      <c r="C148" s="13"/>
-    </row>
-    <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="149" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2"/>
       <c r="B149" s="11"/>
-      <c r="C149" s="13"/>
-    </row>
-    <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="150" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2"/>
       <c r="B150" s="11"/>
-      <c r="C150" s="13"/>
-    </row>
-    <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="151" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2"/>
       <c r="B151" s="11"/>
-      <c r="C151" s="13"/>
-    </row>
-    <row r="152" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="152" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2"/>
       <c r="B152" s="11"/>
-      <c r="C152" s="13"/>
-    </row>
-    <row r="153" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="153" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2"/>
       <c r="B153" s="11"/>
-      <c r="C153" s="13"/>
-    </row>
-    <row r="154" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="154" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="2"/>
       <c r="B154" s="11"/>
-      <c r="C154" s="13"/>
-    </row>
-    <row r="155" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="155" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="2"/>
       <c r="B155" s="11"/>
-      <c r="C155" s="13"/>
-    </row>
-    <row r="156" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="156" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="2"/>
       <c r="B156" s="11"/>
-      <c r="C156" s="13"/>
-    </row>
-    <row r="157" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="157" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="2"/>
       <c r="B157" s="11"/>
-      <c r="C157" s="13"/>
-    </row>
-    <row r="158" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="158" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="2"/>
       <c r="B158" s="11"/>
-      <c r="C158" s="13"/>
-    </row>
-    <row r="159" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="159" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2"/>
       <c r="B159" s="11"/>
-      <c r="C159" s="13"/>
-    </row>
-    <row r="160" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="160" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="2"/>
       <c r="B160" s="11"/>
-      <c r="C160" s="13"/>
-    </row>
-    <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="161" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="2"/>
       <c r="B161" s="11"/>
-      <c r="C161" s="13"/>
-    </row>
-    <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="162" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="2"/>
       <c r="B162" s="11"/>
-      <c r="C162" s="13"/>
-    </row>
-    <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="163" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="2"/>
       <c r="B163" s="11"/>
-      <c r="C163" s="13"/>
-    </row>
-    <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="164" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="2"/>
       <c r="B164" s="11"/>
-      <c r="C164" s="13"/>
-    </row>
-    <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="165" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="2"/>
       <c r="B165" s="11"/>
-      <c r="C165" s="13"/>
-    </row>
-    <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="166" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="2"/>
       <c r="B166" s="11"/>
-      <c r="C166" s="13"/>
-    </row>
-    <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="167" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="2"/>
       <c r="B167" s="11"/>
-      <c r="C167" s="13"/>
-    </row>
-    <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="168" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="2"/>
       <c r="B168" s="11"/>
-      <c r="C168" s="13"/>
-    </row>
-    <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="169" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="2"/>
       <c r="B169" s="11"/>
-      <c r="C169" s="13"/>
-    </row>
-    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="170" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="2"/>
       <c r="B170" s="11"/>
-      <c r="C170" s="13"/>
-    </row>
-    <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="171" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="2"/>
       <c r="B171" s="11"/>
-      <c r="C171" s="13"/>
-    </row>
-    <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="172" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="2"/>
       <c r="B172" s="11"/>
-      <c r="C172" s="13"/>
-    </row>
-    <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="173" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="2"/>
       <c r="B173" s="11"/>
-      <c r="C173" s="13"/>
-    </row>
-    <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="174" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="2"/>
       <c r="B174" s="11"/>
-      <c r="C174" s="13"/>
-    </row>
-    <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="175" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="2"/>
       <c r="B175" s="11"/>
-      <c r="C175" s="13"/>
-    </row>
-    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="176" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="2"/>
       <c r="B176" s="11"/>
-      <c r="C176" s="13"/>
-    </row>
-    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="177" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="2"/>
       <c r="B177" s="11"/>
-      <c r="C177" s="13"/>
-    </row>
-    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="178" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="2"/>
       <c r="B178" s="11"/>
-      <c r="C178" s="13"/>
-    </row>
-    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="179" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="2"/>
       <c r="B179" s="11"/>
-      <c r="C179" s="13"/>
-    </row>
-    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="180" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="2"/>
       <c r="B180" s="11"/>
-      <c r="C180" s="13"/>
-    </row>
-    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="181" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="2"/>
       <c r="B181" s="11"/>
-      <c r="C181" s="13"/>
-    </row>
-    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="182" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="2"/>
       <c r="B182" s="11"/>
-      <c r="C182" s="13"/>
-    </row>
-    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="183" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="2"/>
       <c r="B183" s="11"/>
-      <c r="C183" s="13"/>
-    </row>
-    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="184" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="2"/>
       <c r="B184" s="11"/>
-      <c r="C184" s="13"/>
-    </row>
-    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="185" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="2"/>
       <c r="B185" s="11"/>
-      <c r="C185" s="13"/>
-    </row>
-    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="186" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="2"/>
       <c r="B186" s="11"/>
-      <c r="C186" s="13"/>
-    </row>
-    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="187" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="2"/>
       <c r="B187" s="11"/>
-      <c r="C187" s="13"/>
-    </row>
-    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="188" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="2"/>
       <c r="B188" s="11"/>
-      <c r="C188" s="13"/>
-    </row>
-    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="189" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="2"/>
       <c r="B189" s="11"/>
-      <c r="C189" s="13"/>
-    </row>
-    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="190" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="2"/>
       <c r="B190" s="11"/>
-      <c r="C190" s="13"/>
-    </row>
-    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="191" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="2"/>
       <c r="B191" s="11"/>
-      <c r="C191" s="13"/>
-    </row>
-    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="192" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="2"/>
       <c r="B192" s="11"/>
-      <c r="C192" s="13"/>
-    </row>
-    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="193" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="2"/>
       <c r="B193" s="11"/>
-      <c r="C193" s="13"/>
-    </row>
-    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="194" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="2"/>
       <c r="B194" s="11"/>
-      <c r="C194" s="13"/>
-    </row>
-    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="195" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="2"/>
       <c r="B195" s="11"/>
-      <c r="C195" s="13"/>
-    </row>
-    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="196" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="2"/>
       <c r="B196" s="11"/>
-      <c r="C196" s="13"/>
-    </row>
-    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="197" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="2"/>
       <c r="B197" s="11"/>
-      <c r="C197" s="13"/>
-    </row>
-    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="198" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="2"/>
       <c r="B198" s="11"/>
-      <c r="C198" s="13"/>
-    </row>
-    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="199" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="2"/>
       <c r="B199" s="11"/>
-      <c r="C199" s="13"/>
-    </row>
-    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="200" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="2"/>
       <c r="B200" s="11"/>
-      <c r="C200" s="13"/>
-    </row>
-    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="201" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="2"/>
       <c r="B201" s="11"/>
-      <c r="C201" s="13"/>
-    </row>
-    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="202" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="2"/>
       <c r="B202" s="11"/>
-      <c r="C202" s="13"/>
-    </row>
-    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="203" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="2"/>
       <c r="B203" s="11"/>
-      <c r="C203" s="13"/>
-    </row>
-    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="204" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="2"/>
       <c r="B204" s="11"/>
-      <c r="C204" s="13"/>
-    </row>
-    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="205" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="2"/>
       <c r="B205" s="11"/>
-      <c r="C205" s="13"/>
-    </row>
-    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="206" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="2"/>
       <c r="B206" s="11"/>
-      <c r="C206" s="13"/>
-    </row>
-    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="207" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="2"/>
       <c r="B207" s="11"/>
-      <c r="C207" s="13"/>
-    </row>
-    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="208" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="2"/>
       <c r="B208" s="11"/>
-      <c r="C208" s="13"/>
-    </row>
-    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="209" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="2"/>
       <c r="B209" s="11"/>
-      <c r="C209" s="13"/>
-    </row>
-    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="210" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="2"/>
       <c r="B210" s="11"/>
-      <c r="C210" s="13"/>
-    </row>
-    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="211" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="2"/>
       <c r="B211" s="11"/>
-      <c r="C211" s="13"/>
-    </row>
-    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="212" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2"/>
       <c r="B212" s="11"/>
-      <c r="C212" s="13"/>
-    </row>
-    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="213" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="2"/>
       <c r="B213" s="11"/>
-      <c r="C213" s="13"/>
-    </row>
-    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="214" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="2"/>
       <c r="B214" s="11"/>
-      <c r="C214" s="13"/>
-    </row>
-    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="215" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="2"/>
       <c r="B215" s="11"/>
-      <c r="C215" s="13"/>
-    </row>
-    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="216" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="2"/>
       <c r="B216" s="11"/>
-      <c r="C216" s="13"/>
-    </row>
-    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="217" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="2"/>
       <c r="B217" s="11"/>
-      <c r="C217" s="13"/>
-    </row>
-    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="218" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="2"/>
       <c r="B218" s="11"/>
-      <c r="C218" s="13"/>
-    </row>
-    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="219" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="2"/>
       <c r="B219" s="11"/>
-      <c r="C219" s="13"/>
-    </row>
-    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="220" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="2"/>
       <c r="B220" s="11"/>
-      <c r="C220" s="13"/>
-    </row>
-    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="221" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="2"/>
       <c r="B221" s="11"/>
-      <c r="C221" s="13"/>
-    </row>
-    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="222" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="2"/>
       <c r="B222" s="11"/>
-      <c r="C222" s="13"/>
-    </row>
-    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="223" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="2"/>
       <c r="B223" s="11"/>
-      <c r="C223" s="13"/>
-    </row>
-    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="224" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="2"/>
       <c r="B224" s="11"/>
-      <c r="C224" s="13"/>
-    </row>
-    <row r="225" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="225" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="2"/>
       <c r="B225" s="11"/>
-      <c r="C225" s="13"/>
-    </row>
-    <row r="226" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="226" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="2"/>
       <c r="B226" s="11"/>
-      <c r="C226" s="13"/>
-    </row>
-    <row r="227" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="227" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="2"/>
       <c r="B227" s="11"/>
-      <c r="C227" s="13"/>
-    </row>
-    <row r="228" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="228" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="2"/>
       <c r="B228" s="11"/>
-      <c r="C228" s="13"/>
-    </row>
-    <row r="229" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="229" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="2"/>
       <c r="B229" s="11"/>
-      <c r="C229" s="13"/>
-    </row>
-    <row r="230" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="230" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="2"/>
       <c r="B230" s="11"/>
-      <c r="C230" s="13"/>
-    </row>
-    <row r="231" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="231" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="2"/>
       <c r="B231" s="11"/>
-      <c r="C231" s="13"/>
-    </row>
-    <row r="232" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="232" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="2"/>
       <c r="B232" s="11"/>
-      <c r="C232" s="13"/>
-    </row>
-    <row r="233" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="233" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="2"/>
       <c r="B233" s="11"/>
-      <c r="C233" s="13"/>
-    </row>
-    <row r="234" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="234" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="2"/>
       <c r="B234" s="11"/>
-      <c r="C234" s="13"/>
-    </row>
-    <row r="235" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="235" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="2"/>
       <c r="B235" s="11"/>
-      <c r="C235" s="13"/>
-    </row>
-    <row r="236" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="236" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="2"/>
       <c r="B236" s="11"/>
-      <c r="C236" s="13"/>
-    </row>
-    <row r="237" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="237" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="2"/>
       <c r="B237" s="11"/>
-      <c r="C237" s="13"/>
-    </row>
-    <row r="238" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="238" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="2"/>
       <c r="B238" s="11"/>
-      <c r="C238" s="13"/>
-    </row>
-    <row r="239" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="239" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="2"/>
       <c r="B239" s="11"/>
-      <c r="C239" s="13"/>
-    </row>
-    <row r="240" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="240" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="2"/>
       <c r="B240" s="11"/>
-      <c r="C240" s="13"/>
-    </row>
-    <row r="241" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="241" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="2"/>
       <c r="B241" s="11"/>
-      <c r="C241" s="13"/>
-    </row>
-    <row r="242" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="242" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="2"/>
       <c r="B242" s="11"/>
-      <c r="C242" s="13"/>
-    </row>
-    <row r="243" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="243" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="2"/>
       <c r="B243" s="11"/>
-      <c r="C243" s="13"/>
-    </row>
-    <row r="244" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="244" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="2"/>
       <c r="B244" s="11"/>
-      <c r="C244" s="13"/>
-    </row>
-    <row r="245" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="245" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="2"/>
       <c r="B245" s="11"/>
-      <c r="C245" s="13"/>
-    </row>
-    <row r="246" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="246" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="2"/>
       <c r="B246" s="11"/>
-      <c r="C246" s="13"/>
-    </row>
-    <row r="247" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="247" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="2"/>
       <c r="B247" s="11"/>
-      <c r="C247" s="13"/>
-    </row>
-    <row r="248" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="248" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="2"/>
       <c r="B248" s="11"/>
-      <c r="C248" s="13"/>
-    </row>
-    <row r="249" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="249" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="2"/>
       <c r="B249" s="11"/>
-      <c r="C249" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Add wire frame id to RTM
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI9M-Testing\Core\QA\WorkShop\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9474CDB8-DF2A-412D-8352-D3AA62D8C964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9627D640-0B6E-44B5-A585-6921748EEA69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="114">
   <si>
     <t>SRS ID</t>
   </si>
@@ -316,6 +316,64 @@
   </si>
   <si>
     <t>TC_Client_018</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_001</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_002</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_003</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_004</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_005</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_006</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_007</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_008</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_009</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_010</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_011</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_012</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_013</t>
+  </si>
+  <si>
+    <t>WireFrame_Client_001</t>
+  </si>
+  <si>
+    <t>WireFrame_Client_002
+WireFrame_Client_003</t>
+  </si>
+  <si>
+    <t>WireFrame_Client_004</t>
+  </si>
+  <si>
+    <t>Wireframe_Checkout_001</t>
+  </si>
+  <si>
+    <t>Wireframe_Checkout_002</t>
+  </si>
+  <si>
+    <t>WireFrame Design ID</t>
   </si>
 </sst>
 </file>
@@ -452,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -475,6 +533,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,1213 +759,1513 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B249"/>
+  <dimension ref="A1:C249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.77734375" customWidth="1"/>
     <col min="2" max="2" width="37.44140625" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="14"/>
+    </row>
+    <row r="23" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="14"/>
+    </row>
+    <row r="24" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="14"/>
+    </row>
+    <row r="25" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="14"/>
+    </row>
+    <row r="26" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="14"/>
+    </row>
+    <row r="27" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="14"/>
+    </row>
+    <row r="28" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="14"/>
+    </row>
+    <row r="29" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="14"/>
+    </row>
+    <row r="30" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="14"/>
+    </row>
+    <row r="31" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="14"/>
+    </row>
+    <row r="32" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>59</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="14"/>
+    </row>
+    <row r="34" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>63</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="14"/>
+    </row>
+    <row r="35" spans="1:3" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>65</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="14"/>
+    </row>
+    <row r="36" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C36" s="14"/>
+    </row>
+    <row r="37" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C37" s="14"/>
+    </row>
+    <row r="38" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C38" s="14"/>
+    </row>
+    <row r="39" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="54" x14ac:dyDescent="0.35">
+      <c r="C39" s="14"/>
+    </row>
+    <row r="40" spans="1:3" ht="54" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C40" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>72</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C41" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="54" x14ac:dyDescent="0.35">
+      <c r="C42" s="14"/>
+    </row>
+    <row r="43" spans="1:3" ht="54" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C43" s="14"/>
+    </row>
+    <row r="44" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C44" s="14"/>
+    </row>
+    <row r="45" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C45" s="14"/>
+    </row>
+    <row r="46" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>77</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="36" x14ac:dyDescent="0.35">
+      <c r="C46" s="14"/>
+    </row>
+    <row r="47" spans="1:3" ht="36" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C47" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C48" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C49" s="14"/>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>81</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C50" s="14"/>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4"/>
       <c r="B51" s="7"/>
-    </row>
-    <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C51" s="14"/>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="4"/>
       <c r="B52" s="7"/>
-    </row>
-    <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C52" s="14"/>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4"/>
       <c r="B53" s="7"/>
-    </row>
-    <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="14"/>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="11"/>
-    </row>
-    <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C54" s="14"/>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" s="11"/>
-    </row>
-    <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C55" s="14"/>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="11"/>
-    </row>
-    <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="14"/>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="11"/>
-    </row>
-    <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="14"/>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="11"/>
-    </row>
-    <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="14"/>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="11"/>
-    </row>
-    <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C59" s="14"/>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="11"/>
-    </row>
-    <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="14"/>
+    </row>
+    <row r="61" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="11"/>
-    </row>
-    <row r="62" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="14"/>
+    </row>
+    <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="11"/>
-    </row>
-    <row r="63" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C62" s="14"/>
+    </row>
+    <row r="63" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="11"/>
-    </row>
-    <row r="64" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C63" s="14"/>
+    </row>
+    <row r="64" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="11"/>
-    </row>
-    <row r="65" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C64" s="14"/>
+    </row>
+    <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="11"/>
-    </row>
-    <row r="66" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C65" s="14"/>
+    </row>
+    <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="11"/>
-    </row>
-    <row r="67" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C66" s="14"/>
+    </row>
+    <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" s="11"/>
-    </row>
-    <row r="68" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C67" s="14"/>
+    </row>
+    <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" s="11"/>
-    </row>
-    <row r="69" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C68" s="14"/>
+    </row>
+    <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="11"/>
-    </row>
-    <row r="70" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C69" s="14"/>
+    </row>
+    <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" s="11"/>
-    </row>
-    <row r="71" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C70" s="14"/>
+    </row>
+    <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="11"/>
-    </row>
-    <row r="72" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C71" s="14"/>
+    </row>
+    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="11"/>
-    </row>
-    <row r="73" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C72" s="14"/>
+    </row>
+    <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="11"/>
-    </row>
-    <row r="74" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C73" s="14"/>
+    </row>
+    <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="11"/>
-    </row>
-    <row r="75" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C74" s="14"/>
+    </row>
+    <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="11"/>
-    </row>
-    <row r="76" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C75" s="14"/>
+    </row>
+    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="11"/>
-    </row>
-    <row r="77" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C76" s="14"/>
+    </row>
+    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" s="11"/>
-    </row>
-    <row r="78" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C77" s="14"/>
+    </row>
+    <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" s="11"/>
-    </row>
-    <row r="79" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C78" s="14"/>
+    </row>
+    <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" s="11"/>
-    </row>
-    <row r="80" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C79" s="14"/>
+    </row>
+    <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" s="11"/>
-    </row>
-    <row r="81" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C80" s="14"/>
+    </row>
+    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="B81" s="11"/>
-    </row>
-    <row r="82" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C81" s="14"/>
+    </row>
+    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
       <c r="B82" s="11"/>
-    </row>
-    <row r="83" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C82" s="14"/>
+    </row>
+    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2"/>
       <c r="B83" s="11"/>
-    </row>
-    <row r="84" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C83" s="14"/>
+    </row>
+    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
       <c r="B84" s="11"/>
-    </row>
-    <row r="85" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C84" s="14"/>
+    </row>
+    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2"/>
       <c r="B85" s="11"/>
-    </row>
-    <row r="86" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C85" s="14"/>
+    </row>
+    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" s="11"/>
-    </row>
-    <row r="87" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C86" s="14"/>
+    </row>
+    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
       <c r="B87" s="11"/>
-    </row>
-    <row r="88" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C87" s="14"/>
+    </row>
+    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
       <c r="B88" s="11"/>
-    </row>
-    <row r="89" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C88" s="14"/>
+    </row>
+    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" s="11"/>
-    </row>
-    <row r="90" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C89" s="14"/>
+    </row>
+    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
       <c r="B90" s="11"/>
-    </row>
-    <row r="91" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C90" s="14"/>
+    </row>
+    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
       <c r="B91" s="11"/>
-    </row>
-    <row r="92" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C91" s="14"/>
+    </row>
+    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
       <c r="B92" s="11"/>
-    </row>
-    <row r="93" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C92" s="14"/>
+    </row>
+    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
       <c r="B93" s="11"/>
-    </row>
-    <row r="94" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C93" s="14"/>
+    </row>
+    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
       <c r="B94" s="11"/>
-    </row>
-    <row r="95" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C94" s="14"/>
+    </row>
+    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2"/>
       <c r="B95" s="11"/>
-    </row>
-    <row r="96" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C95" s="14"/>
+    </row>
+    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
       <c r="B96" s="11"/>
-    </row>
-    <row r="97" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C96" s="14"/>
+    </row>
+    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
       <c r="B97" s="11"/>
-    </row>
-    <row r="98" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C97" s="14"/>
+    </row>
+    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
       <c r="B98" s="11"/>
-    </row>
-    <row r="99" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C98" s="14"/>
+    </row>
+    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
       <c r="B99" s="11"/>
-    </row>
-    <row r="100" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C99" s="14"/>
+    </row>
+    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
       <c r="B100" s="11"/>
-    </row>
-    <row r="101" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C100" s="14"/>
+    </row>
+    <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
       <c r="B101" s="11"/>
-    </row>
-    <row r="102" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C101" s="14"/>
+    </row>
+    <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
       <c r="B102" s="11"/>
-    </row>
-    <row r="103" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C102" s="14"/>
+    </row>
+    <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
       <c r="B103" s="11"/>
-    </row>
-    <row r="104" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C103" s="14"/>
+    </row>
+    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="B104" s="11"/>
-    </row>
-    <row r="105" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C104" s="14"/>
+    </row>
+    <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
       <c r="B105" s="11"/>
-    </row>
-    <row r="106" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C105" s="14"/>
+    </row>
+    <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="B106" s="11"/>
-    </row>
-    <row r="107" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C106" s="14"/>
+    </row>
+    <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" s="11"/>
-    </row>
-    <row r="108" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C107" s="14"/>
+    </row>
+    <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
       <c r="B108" s="11"/>
-    </row>
-    <row r="109" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C108" s="14"/>
+    </row>
+    <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2"/>
       <c r="B109" s="11"/>
-    </row>
-    <row r="110" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C109" s="14"/>
+    </row>
+    <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="B110" s="11"/>
-    </row>
-    <row r="111" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C110" s="14"/>
+    </row>
+    <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2"/>
       <c r="B111" s="11"/>
-    </row>
-    <row r="112" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C111" s="14"/>
+    </row>
+    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
       <c r="B112" s="11"/>
-    </row>
-    <row r="113" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C112" s="14"/>
+    </row>
+    <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
       <c r="B113" s="11"/>
-    </row>
-    <row r="114" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C113" s="14"/>
+    </row>
+    <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="B114" s="11"/>
-    </row>
-    <row r="115" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C114" s="14"/>
+    </row>
+    <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2"/>
       <c r="B115" s="11"/>
-    </row>
-    <row r="116" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C115" s="14"/>
+    </row>
+    <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2"/>
       <c r="B116" s="11"/>
-    </row>
-    <row r="117" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C116" s="14"/>
+    </row>
+    <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2"/>
       <c r="B117" s="11"/>
-    </row>
-    <row r="118" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C117" s="14"/>
+    </row>
+    <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2"/>
       <c r="B118" s="11"/>
-    </row>
-    <row r="119" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C118" s="14"/>
+    </row>
+    <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2"/>
       <c r="B119" s="11"/>
-    </row>
-    <row r="120" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C119" s="14"/>
+    </row>
+    <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2"/>
       <c r="B120" s="11"/>
-    </row>
-    <row r="121" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C120" s="14"/>
+    </row>
+    <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2"/>
       <c r="B121" s="11"/>
-    </row>
-    <row r="122" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C121" s="14"/>
+    </row>
+    <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2"/>
       <c r="B122" s="11"/>
-    </row>
-    <row r="123" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C122" s="14"/>
+    </row>
+    <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2"/>
       <c r="B123" s="11"/>
-    </row>
-    <row r="124" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C123" s="14"/>
+    </row>
+    <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2"/>
       <c r="B124" s="11"/>
-    </row>
-    <row r="125" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C124" s="14"/>
+    </row>
+    <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2"/>
       <c r="B125" s="11"/>
-    </row>
-    <row r="126" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C125" s="14"/>
+    </row>
+    <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2"/>
       <c r="B126" s="11"/>
-    </row>
-    <row r="127" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C126" s="14"/>
+    </row>
+    <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2"/>
       <c r="B127" s="11"/>
-    </row>
-    <row r="128" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C127" s="14"/>
+    </row>
+    <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2"/>
       <c r="B128" s="11"/>
-    </row>
-    <row r="129" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C128" s="14"/>
+    </row>
+    <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2"/>
       <c r="B129" s="11"/>
-    </row>
-    <row r="130" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C129" s="14"/>
+    </row>
+    <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2"/>
       <c r="B130" s="11"/>
-    </row>
-    <row r="131" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C130" s="14"/>
+    </row>
+    <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2"/>
       <c r="B131" s="11"/>
-    </row>
-    <row r="132" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C131" s="14"/>
+    </row>
+    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2"/>
       <c r="B132" s="11"/>
-    </row>
-    <row r="133" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C132" s="14"/>
+    </row>
+    <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2"/>
       <c r="B133" s="11"/>
-    </row>
-    <row r="134" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C133" s="14"/>
+    </row>
+    <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2"/>
       <c r="B134" s="11"/>
-    </row>
-    <row r="135" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C134" s="14"/>
+    </row>
+    <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2"/>
       <c r="B135" s="11"/>
-    </row>
-    <row r="136" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C135" s="14"/>
+    </row>
+    <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2"/>
       <c r="B136" s="11"/>
-    </row>
-    <row r="137" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C136" s="14"/>
+    </row>
+    <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2"/>
       <c r="B137" s="11"/>
-    </row>
-    <row r="138" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C137" s="14"/>
+    </row>
+    <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2"/>
       <c r="B138" s="11"/>
-    </row>
-    <row r="139" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C138" s="14"/>
+    </row>
+    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2"/>
       <c r="B139" s="11"/>
-    </row>
-    <row r="140" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C139" s="14"/>
+    </row>
+    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2"/>
       <c r="B140" s="11"/>
-    </row>
-    <row r="141" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C140" s="14"/>
+    </row>
+    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2"/>
       <c r="B141" s="11"/>
-    </row>
-    <row r="142" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C141" s="14"/>
+    </row>
+    <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2"/>
       <c r="B142" s="11"/>
-    </row>
-    <row r="143" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C142" s="14"/>
+    </row>
+    <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2"/>
       <c r="B143" s="11"/>
-    </row>
-    <row r="144" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C143" s="14"/>
+    </row>
+    <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2"/>
       <c r="B144" s="11"/>
-    </row>
-    <row r="145" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C144" s="14"/>
+    </row>
+    <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2"/>
       <c r="B145" s="11"/>
-    </row>
-    <row r="146" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C145" s="14"/>
+    </row>
+    <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2"/>
       <c r="B146" s="11"/>
-    </row>
-    <row r="147" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C146" s="14"/>
+    </row>
+    <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2"/>
       <c r="B147" s="11"/>
-    </row>
-    <row r="148" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C147" s="14"/>
+    </row>
+    <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2"/>
       <c r="B148" s="11"/>
-    </row>
-    <row r="149" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C148" s="14"/>
+    </row>
+    <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2"/>
       <c r="B149" s="11"/>
-    </row>
-    <row r="150" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C149" s="14"/>
+    </row>
+    <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2"/>
       <c r="B150" s="11"/>
-    </row>
-    <row r="151" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C150" s="14"/>
+    </row>
+    <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2"/>
       <c r="B151" s="11"/>
-    </row>
-    <row r="152" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C151" s="14"/>
+    </row>
+    <row r="152" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2"/>
       <c r="B152" s="11"/>
-    </row>
-    <row r="153" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C152" s="14"/>
+    </row>
+    <row r="153" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2"/>
       <c r="B153" s="11"/>
-    </row>
-    <row r="154" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C153" s="14"/>
+    </row>
+    <row r="154" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="2"/>
       <c r="B154" s="11"/>
-    </row>
-    <row r="155" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C154" s="14"/>
+    </row>
+    <row r="155" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="2"/>
       <c r="B155" s="11"/>
-    </row>
-    <row r="156" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C155" s="14"/>
+    </row>
+    <row r="156" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="2"/>
       <c r="B156" s="11"/>
-    </row>
-    <row r="157" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C156" s="14"/>
+    </row>
+    <row r="157" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="2"/>
       <c r="B157" s="11"/>
-    </row>
-    <row r="158" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C157" s="14"/>
+    </row>
+    <row r="158" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="2"/>
       <c r="B158" s="11"/>
-    </row>
-    <row r="159" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C158" s="14"/>
+    </row>
+    <row r="159" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2"/>
       <c r="B159" s="11"/>
-    </row>
-    <row r="160" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C159" s="14"/>
+    </row>
+    <row r="160" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="2"/>
       <c r="B160" s="11"/>
-    </row>
-    <row r="161" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C160" s="14"/>
+    </row>
+    <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="2"/>
       <c r="B161" s="11"/>
-    </row>
-    <row r="162" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C161" s="14"/>
+    </row>
+    <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="2"/>
       <c r="B162" s="11"/>
-    </row>
-    <row r="163" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C162" s="14"/>
+    </row>
+    <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="2"/>
       <c r="B163" s="11"/>
-    </row>
-    <row r="164" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C163" s="14"/>
+    </row>
+    <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="2"/>
       <c r="B164" s="11"/>
-    </row>
-    <row r="165" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C164" s="14"/>
+    </row>
+    <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="2"/>
       <c r="B165" s="11"/>
-    </row>
-    <row r="166" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C165" s="14"/>
+    </row>
+    <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="2"/>
       <c r="B166" s="11"/>
-    </row>
-    <row r="167" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C166" s="14"/>
+    </row>
+    <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="2"/>
       <c r="B167" s="11"/>
-    </row>
-    <row r="168" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C167" s="14"/>
+    </row>
+    <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="2"/>
       <c r="B168" s="11"/>
-    </row>
-    <row r="169" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C168" s="14"/>
+    </row>
+    <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="2"/>
       <c r="B169" s="11"/>
-    </row>
-    <row r="170" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C169" s="14"/>
+    </row>
+    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="2"/>
       <c r="B170" s="11"/>
-    </row>
-    <row r="171" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C170" s="14"/>
+    </row>
+    <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="2"/>
       <c r="B171" s="11"/>
-    </row>
-    <row r="172" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C171" s="14"/>
+    </row>
+    <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="2"/>
       <c r="B172" s="11"/>
-    </row>
-    <row r="173" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C172" s="14"/>
+    </row>
+    <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="2"/>
       <c r="B173" s="11"/>
-    </row>
-    <row r="174" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C173" s="14"/>
+    </row>
+    <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="2"/>
       <c r="B174" s="11"/>
-    </row>
-    <row r="175" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C174" s="14"/>
+    </row>
+    <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="2"/>
       <c r="B175" s="11"/>
-    </row>
-    <row r="176" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C175" s="14"/>
+    </row>
+    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="2"/>
       <c r="B176" s="11"/>
-    </row>
-    <row r="177" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C176" s="14"/>
+    </row>
+    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="2"/>
       <c r="B177" s="11"/>
-    </row>
-    <row r="178" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C177" s="14"/>
+    </row>
+    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="2"/>
       <c r="B178" s="11"/>
-    </row>
-    <row r="179" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C178" s="14"/>
+    </row>
+    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="2"/>
       <c r="B179" s="11"/>
-    </row>
-    <row r="180" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C179" s="14"/>
+    </row>
+    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="2"/>
       <c r="B180" s="11"/>
-    </row>
-    <row r="181" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C180" s="14"/>
+    </row>
+    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="2"/>
       <c r="B181" s="11"/>
-    </row>
-    <row r="182" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C181" s="14"/>
+    </row>
+    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="2"/>
       <c r="B182" s="11"/>
-    </row>
-    <row r="183" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C182" s="14"/>
+    </row>
+    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="2"/>
       <c r="B183" s="11"/>
-    </row>
-    <row r="184" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C183" s="14"/>
+    </row>
+    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="2"/>
       <c r="B184" s="11"/>
-    </row>
-    <row r="185" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C184" s="14"/>
+    </row>
+    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="2"/>
       <c r="B185" s="11"/>
-    </row>
-    <row r="186" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C185" s="14"/>
+    </row>
+    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="2"/>
       <c r="B186" s="11"/>
-    </row>
-    <row r="187" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C186" s="14"/>
+    </row>
+    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="2"/>
       <c r="B187" s="11"/>
-    </row>
-    <row r="188" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C187" s="14"/>
+    </row>
+    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="2"/>
       <c r="B188" s="11"/>
-    </row>
-    <row r="189" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C188" s="14"/>
+    </row>
+    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="2"/>
       <c r="B189" s="11"/>
-    </row>
-    <row r="190" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C189" s="14"/>
+    </row>
+    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="2"/>
       <c r="B190" s="11"/>
-    </row>
-    <row r="191" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C190" s="14"/>
+    </row>
+    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="2"/>
       <c r="B191" s="11"/>
-    </row>
-    <row r="192" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C191" s="14"/>
+    </row>
+    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="2"/>
       <c r="B192" s="11"/>
-    </row>
-    <row r="193" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C192" s="14"/>
+    </row>
+    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="2"/>
       <c r="B193" s="11"/>
-    </row>
-    <row r="194" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C193" s="14"/>
+    </row>
+    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="2"/>
       <c r="B194" s="11"/>
-    </row>
-    <row r="195" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C194" s="14"/>
+    </row>
+    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="2"/>
       <c r="B195" s="11"/>
-    </row>
-    <row r="196" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C195" s="14"/>
+    </row>
+    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="2"/>
       <c r="B196" s="11"/>
-    </row>
-    <row r="197" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C196" s="14"/>
+    </row>
+    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="2"/>
       <c r="B197" s="11"/>
-    </row>
-    <row r="198" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C197" s="14"/>
+    </row>
+    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="2"/>
       <c r="B198" s="11"/>
-    </row>
-    <row r="199" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C198" s="14"/>
+    </row>
+    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="2"/>
       <c r="B199" s="11"/>
-    </row>
-    <row r="200" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C199" s="14"/>
+    </row>
+    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="2"/>
       <c r="B200" s="11"/>
-    </row>
-    <row r="201" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C200" s="14"/>
+    </row>
+    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="2"/>
       <c r="B201" s="11"/>
-    </row>
-    <row r="202" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C201" s="14"/>
+    </row>
+    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="2"/>
       <c r="B202" s="11"/>
-    </row>
-    <row r="203" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C202" s="14"/>
+    </row>
+    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="2"/>
       <c r="B203" s="11"/>
-    </row>
-    <row r="204" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C203" s="14"/>
+    </row>
+    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="2"/>
       <c r="B204" s="11"/>
-    </row>
-    <row r="205" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C204" s="14"/>
+    </row>
+    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="2"/>
       <c r="B205" s="11"/>
-    </row>
-    <row r="206" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C205" s="14"/>
+    </row>
+    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="2"/>
       <c r="B206" s="11"/>
-    </row>
-    <row r="207" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C206" s="14"/>
+    </row>
+    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="2"/>
       <c r="B207" s="11"/>
-    </row>
-    <row r="208" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C207" s="14"/>
+    </row>
+    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="2"/>
       <c r="B208" s="11"/>
-    </row>
-    <row r="209" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C208" s="14"/>
+    </row>
+    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="2"/>
       <c r="B209" s="11"/>
-    </row>
-    <row r="210" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C209" s="14"/>
+    </row>
+    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="2"/>
       <c r="B210" s="11"/>
-    </row>
-    <row r="211" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C210" s="14"/>
+    </row>
+    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="2"/>
       <c r="B211" s="11"/>
-    </row>
-    <row r="212" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C211" s="14"/>
+    </row>
+    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2"/>
       <c r="B212" s="11"/>
-    </row>
-    <row r="213" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C212" s="14"/>
+    </row>
+    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="2"/>
       <c r="B213" s="11"/>
-    </row>
-    <row r="214" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C213" s="14"/>
+    </row>
+    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="2"/>
       <c r="B214" s="11"/>
-    </row>
-    <row r="215" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C214" s="14"/>
+    </row>
+    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="2"/>
       <c r="B215" s="11"/>
-    </row>
-    <row r="216" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C215" s="14"/>
+    </row>
+    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="2"/>
       <c r="B216" s="11"/>
-    </row>
-    <row r="217" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C216" s="14"/>
+    </row>
+    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="2"/>
       <c r="B217" s="11"/>
-    </row>
-    <row r="218" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C217" s="14"/>
+    </row>
+    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="2"/>
       <c r="B218" s="11"/>
-    </row>
-    <row r="219" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C218" s="14"/>
+    </row>
+    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="2"/>
       <c r="B219" s="11"/>
-    </row>
-    <row r="220" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C219" s="14"/>
+    </row>
+    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="2"/>
       <c r="B220" s="11"/>
-    </row>
-    <row r="221" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C220" s="14"/>
+    </row>
+    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="2"/>
       <c r="B221" s="11"/>
-    </row>
-    <row r="222" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C221" s="14"/>
+    </row>
+    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="2"/>
       <c r="B222" s="11"/>
-    </row>
-    <row r="223" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C222" s="14"/>
+    </row>
+    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="2"/>
       <c r="B223" s="11"/>
-    </row>
-    <row r="224" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C223" s="14"/>
+    </row>
+    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="2"/>
       <c r="B224" s="11"/>
-    </row>
-    <row r="225" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C224" s="14"/>
+    </row>
+    <row r="225" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="2"/>
       <c r="B225" s="11"/>
-    </row>
-    <row r="226" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C225" s="14"/>
+    </row>
+    <row r="226" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="2"/>
       <c r="B226" s="11"/>
-    </row>
-    <row r="227" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C226" s="14"/>
+    </row>
+    <row r="227" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="2"/>
       <c r="B227" s="11"/>
-    </row>
-    <row r="228" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C227" s="14"/>
+    </row>
+    <row r="228" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="2"/>
       <c r="B228" s="11"/>
-    </row>
-    <row r="229" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C228" s="14"/>
+    </row>
+    <row r="229" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="2"/>
       <c r="B229" s="11"/>
-    </row>
-    <row r="230" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C229" s="14"/>
+    </row>
+    <row r="230" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="2"/>
       <c r="B230" s="11"/>
-    </row>
-    <row r="231" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C230" s="14"/>
+    </row>
+    <row r="231" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="2"/>
       <c r="B231" s="11"/>
-    </row>
-    <row r="232" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C231" s="14"/>
+    </row>
+    <row r="232" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="2"/>
       <c r="B232" s="11"/>
-    </row>
-    <row r="233" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C232" s="14"/>
+    </row>
+    <row r="233" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="2"/>
       <c r="B233" s="11"/>
-    </row>
-    <row r="234" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C233" s="14"/>
+    </row>
+    <row r="234" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="2"/>
       <c r="B234" s="11"/>
-    </row>
-    <row r="235" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C234" s="14"/>
+    </row>
+    <row r="235" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="2"/>
       <c r="B235" s="11"/>
-    </row>
-    <row r="236" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C235" s="14"/>
+    </row>
+    <row r="236" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="2"/>
       <c r="B236" s="11"/>
-    </row>
-    <row r="237" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C236" s="14"/>
+    </row>
+    <row r="237" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="2"/>
       <c r="B237" s="11"/>
-    </row>
-    <row r="238" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C237" s="14"/>
+    </row>
+    <row r="238" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="2"/>
       <c r="B238" s="11"/>
-    </row>
-    <row r="239" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C238" s="14"/>
+    </row>
+    <row r="239" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="2"/>
       <c r="B239" s="11"/>
-    </row>
-    <row r="240" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C239" s="14"/>
+    </row>
+    <row r="240" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="2"/>
       <c r="B240" s="11"/>
-    </row>
-    <row r="241" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C240" s="14"/>
+    </row>
+    <row r="241" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="2"/>
       <c r="B241" s="11"/>
-    </row>
-    <row r="242" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C241" s="14"/>
+    </row>
+    <row r="242" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="2"/>
       <c r="B242" s="11"/>
-    </row>
-    <row r="243" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C242" s="14"/>
+    </row>
+    <row r="243" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="2"/>
       <c r="B243" s="11"/>
-    </row>
-    <row r="244" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C243" s="14"/>
+    </row>
+    <row r="244" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="2"/>
       <c r="B244" s="11"/>
-    </row>
-    <row r="245" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C244" s="14"/>
+    </row>
+    <row r="245" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="2"/>
       <c r="B245" s="11"/>
-    </row>
-    <row r="246" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C245" s="14"/>
+    </row>
+    <row r="246" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="2"/>
       <c r="B246" s="11"/>
-    </row>
-    <row r="247" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C246" s="14"/>
+    </row>
+    <row r="247" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="2"/>
       <c r="B247" s="11"/>
-    </row>
-    <row r="248" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C247" s="14"/>
+    </row>
+    <row r="248" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="2"/>
       <c r="B248" s="11"/>
-    </row>
-    <row r="249" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C248" s="14"/>
+    </row>
+    <row r="249" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="2"/>
       <c r="B249" s="11"/>
+      <c r="C249" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Doc: Added Traceability for Order History and shopping cart between TC and WireFrames
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA041DB-BF5C-45E1-9E14-7602F38E0735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5ECBABF-0DDB-41DB-AD6E-1EA43D1D3598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="124">
   <si>
     <t>SRS ID</t>
   </si>
@@ -384,6 +384,24 @@
   </si>
   <si>
     <t>WireFrame_Supplier_009</t>
+  </si>
+  <si>
+    <t>WireFrame_Cart_001</t>
+  </si>
+  <si>
+    <t>WireFrame_OrderHistory_001</t>
+  </si>
+  <si>
+    <t>WireFrame_OrderHistory_002</t>
+  </si>
+  <si>
+    <t>WireFrame_shoppingcart_003</t>
+  </si>
+  <si>
+    <t>WireFrame_shoppingcart_002</t>
+  </si>
+  <si>
+    <t>WireFrame_shoppingcart_004</t>
   </si>
 </sst>
 </file>
@@ -520,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -550,6 +568,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -770,8 +794,8 @@
   </sheetPr>
   <dimension ref="A1:C247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1145,7 +1169,9 @@
       <c r="B34" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="12"/>
+      <c r="C34" s="15" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="35" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
@@ -1154,7 +1180,9 @@
       <c r="B35" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C35" s="12"/>
+      <c r="C35" s="15" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="36" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
@@ -1163,7 +1191,9 @@
       <c r="B36" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="12"/>
+      <c r="C36" s="15" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="37" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
@@ -1172,7 +1202,9 @@
       <c r="B37" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="12"/>
+      <c r="C37" s="15" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="38" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
@@ -1203,7 +1235,9 @@
       <c r="B40" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C40" s="12"/>
+      <c r="C40" s="16" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="41" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
@@ -1212,7 +1246,9 @@
       <c r="B41" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="12"/>
+      <c r="C41" s="17" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="42" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
@@ -1221,7 +1257,9 @@
       <c r="B42" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C42" s="12"/>
+      <c r="C42" s="18" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="43" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
@@ -1230,7 +1268,9 @@
       <c r="B43" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="12"/>
+      <c r="C43" s="19" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="44" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
@@ -1239,7 +1279,9 @@
       <c r="B44" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C44" s="12"/>
+      <c r="C44" s="20" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="45" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
@@ -1259,7 +1301,7 @@
       <c r="B46" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="20" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Doc: Updated Cart Wireframes and Traceability according to Review comments
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5ECBABF-0DDB-41DB-AD6E-1EA43D1D3598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1198D1B3-FAE8-4F86-94F0-8AA3A647E50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="125">
   <si>
     <t>SRS ID</t>
   </si>
@@ -402,6 +402,10 @@
   </si>
   <si>
     <t>WireFrame_shoppingcart_004</t>
+  </si>
+  <si>
+    <t>WireFrame_Cart_001
+WireFrame_Cart_005</t>
   </si>
 </sst>
 </file>
@@ -538,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -568,12 +572,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -794,8 +792,8 @@
   </sheetPr>
   <dimension ref="A1:C247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1169,7 +1167,7 @@
       <c r="B34" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="12" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1180,7 +1178,7 @@
       <c r="B35" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="12" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1191,7 +1189,7 @@
       <c r="B36" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C36" s="12" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1202,7 +1200,7 @@
       <c r="B37" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="12" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1235,7 +1233,7 @@
       <c r="B40" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C40" s="16" t="s">
+      <c r="C40" s="12" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1246,8 +1244,8 @@
       <c r="B41" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="17" t="s">
-        <v>118</v>
+      <c r="C41" s="13" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -1257,7 +1255,7 @@
       <c r="B42" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C42" s="12" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1268,7 +1266,7 @@
       <c r="B43" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C43" s="12" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1279,7 +1277,7 @@
       <c r="B44" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C44" s="20" t="s">
+      <c r="C44" s="12" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1301,7 +1299,7 @@
       <c r="B46" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C46" s="20" t="s">
+      <c r="C46" s="12" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Doc: Updated Traceability for Checkout page between TC and WireFrames
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1198D1B3-FAE8-4F86-94F0-8AA3A647E50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC289CDF-C0DC-4AE3-9459-8C7D56329637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="124">
   <si>
     <t>SRS ID</t>
   </si>
@@ -353,9 +353,6 @@
   </si>
   <si>
     <t>Wireframe_Checkout_001</t>
-  </si>
-  <si>
-    <t>Wireframe_Checkout_002</t>
   </si>
   <si>
     <t>WireFrame Design ID</t>
@@ -793,7 +790,7 @@
   <dimension ref="A1:C247"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -811,7 +808,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1060,7 +1057,7 @@
         <v>8</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.3">
@@ -1080,7 +1077,7 @@
         <v>49</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1091,7 +1088,7 @@
         <v>51</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1102,7 +1099,7 @@
         <v>53</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1113,7 +1110,7 @@
         <v>55</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1124,7 +1121,7 @@
         <v>55</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1135,7 +1132,7 @@
         <v>58</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1146,7 +1143,7 @@
         <v>60</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1157,7 +1154,7 @@
         <v>62</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1168,7 +1165,7 @@
         <v>78</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1179,7 +1176,7 @@
         <v>79</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1190,7 +1187,7 @@
         <v>78</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -1201,7 +1198,7 @@
         <v>85</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
@@ -1234,7 +1231,7 @@
         <v>81</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
@@ -1245,7 +1242,7 @@
         <v>87</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -1256,7 +1253,7 @@
         <v>83</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -1267,7 +1264,7 @@
         <v>84</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -1278,7 +1275,7 @@
         <v>82</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
@@ -1300,7 +1297,7 @@
         <v>89</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -1310,7 +1307,9 @@
       <c r="B47" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C47" s="12"/>
+      <c r="C47" s="12" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
@@ -1319,7 +1318,9 @@
       <c r="B48" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C48" s="12"/>
+      <c r="C48" s="12" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>

</xml_diff>

<commit_message>
Doc: Added Traceability for Login feature between TC and Wireframes
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC289CDF-C0DC-4AE3-9459-8C7D56329637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A33BA9-72C7-425D-B6EF-6402859D1D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="128">
   <si>
     <t>SRS ID</t>
   </si>
@@ -403,6 +403,26 @@
   <si>
     <t>WireFrame_Cart_001
 WireFrame_Cart_005</t>
+  </si>
+  <si>
+    <t>WireFrame_Login_005</t>
+  </si>
+  <si>
+    <t>WireFrame_Login_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_Login_002
+TC_Login_005
+TC_Login_006
+TC_Login_007
+TC_Login_0012
+TC_Login_0013
+</t>
+  </si>
+  <si>
+    <t>WireFrame_Login_003
+WireFrame_Login_004
+WireFrame_Login_005</t>
   </si>
 </sst>
 </file>
@@ -787,10 +807,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C247"/>
+  <dimension ref="A1:C248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1038,7 +1058,9 @@
       <c r="B22" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="12"/>
+      <c r="C22" s="12" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="23" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
@@ -1047,7 +1069,9 @@
       <c r="B23" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="12"/>
+      <c r="C23" s="12" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="24" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
@@ -1067,55 +1091,57 @@
       <c r="B25" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="12"/>
-    </row>
-    <row r="26" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B27" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+    <row r="28" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B28" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C28" s="14" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>55</v>
@@ -1126,175 +1152,175 @@
     </row>
     <row r="31" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>118</v>
+        <v>61</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B37" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>85</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B39" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C39" s="13" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B41" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C41" s="12" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
+    <row r="42" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B42" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C42" s="13" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>84</v>
+        <v>71</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B45" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C45" s="12" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
+    <row r="46" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B46" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>107</v>
@@ -1302,18 +1328,18 @@
     </row>
     <row r="47" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>90</v>
@@ -1323,9 +1349,15 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="4"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="12"/>
+      <c r="A49" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
@@ -1337,9 +1369,9 @@
       <c r="B51" s="7"/>
       <c r="C51" s="12"/>
     </row>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="B52" s="10"/>
+    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="4"/>
+      <c r="B52" s="7"/>
       <c r="C52" s="12"/>
     </row>
     <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2316,6 +2348,11 @@
       <c r="A247" s="2"/>
       <c r="B247" s="10"/>
       <c r="C247" s="12"/>
+    </row>
+    <row r="248" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A248" s="2"/>
+      <c r="B248" s="10"/>
+      <c r="C248" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Doc: Updated Login feature in CRS,SRS and RTM according to assessment comments
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A33BA9-72C7-425D-B6EF-6402859D1D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1C4392-7A57-41D4-9964-43A8331075D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,386 +43,391 @@
     <t>SRS_Login_005</t>
   </si>
   <si>
-    <t xml:space="preserve">TC_Login_001 </t>
-  </si>
-  <si>
     <t>TC_Login_001  
 TC-Login_008</t>
   </si>
   <si>
-    <t xml:space="preserve">TC_Login_001  </t>
+    <t>SRS_Register_001</t>
+  </si>
+  <si>
+    <t>TC_Register_001</t>
+  </si>
+  <si>
+    <t>SRS_Register_002</t>
+  </si>
+  <si>
+    <t>TC_Register_002</t>
+  </si>
+  <si>
+    <t>SRS_Register_003</t>
+  </si>
+  <si>
+    <t>TC_Register_003</t>
+  </si>
+  <si>
+    <t>SRS_Register_004</t>
+  </si>
+  <si>
+    <t>TC_Register_004</t>
+  </si>
+  <si>
+    <t>SRS_Register_005</t>
+  </si>
+  <si>
+    <t>TC_Register_005</t>
+  </si>
+  <si>
+    <t>SRS_Register_006</t>
+  </si>
+  <si>
+    <t>TC_Register_006</t>
+  </si>
+  <si>
+    <t>SRS_Register_007</t>
+  </si>
+  <si>
+    <t>TC_Register_007</t>
+  </si>
+  <si>
+    <t>SRS_Register_008</t>
+  </si>
+  <si>
+    <t>TC_Register_008</t>
+  </si>
+  <si>
+    <t>SRS_Register_009</t>
+  </si>
+  <si>
+    <t>TC_Register_009</t>
+  </si>
+  <si>
+    <t>SRS_Register_010</t>
+  </si>
+  <si>
+    <t>TC_Register_010</t>
+  </si>
+  <si>
+    <t>SRS_Register_011</t>
+  </si>
+  <si>
+    <t>TC_Register_011</t>
+  </si>
+  <si>
+    <t>SRS_Register_012</t>
+  </si>
+  <si>
+    <t>TC_Register_012</t>
+  </si>
+  <si>
+    <t>SRS_Register_013</t>
+  </si>
+  <si>
+    <t>TC_Register_013</t>
+  </si>
+  <si>
+    <t>SRS_Register_014</t>
+  </si>
+  <si>
+    <t>TC_Register_014</t>
+  </si>
+  <si>
+    <t>SRS_Register_015</t>
+  </si>
+  <si>
+    <t>TC_Register_015</t>
+  </si>
+  <si>
+    <t>SRS_Register_016</t>
+  </si>
+  <si>
+    <t>TC_Register_016</t>
+  </si>
+  <si>
+    <t>SRS_Register_017</t>
+  </si>
+  <si>
+    <t>TC_Register_017</t>
+  </si>
+  <si>
+    <t>SRS_Register_018</t>
+  </si>
+  <si>
+    <t>SRS_Register_019</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_001</t>
+  </si>
+  <si>
+    <t>TC_Supplier_001</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_002</t>
+  </si>
+  <si>
+    <t>TC_Supplier_002
+TC_Supplier_003</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_003</t>
+  </si>
+  <si>
+    <t>TC_Supplier_004</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_004</t>
+  </si>
+  <si>
+    <t>TC_Supplier_005</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_005</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_006</t>
+  </si>
+  <si>
+    <t>TC_Supplier_006</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_007</t>
+  </si>
+  <si>
+    <t>TC_Supplier_007</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_008</t>
+  </si>
+  <si>
+    <t>TC_Supplier_008</t>
+  </si>
+  <si>
+    <t>SRS_Client_001</t>
+  </si>
+  <si>
+    <t>SRS_Client_002</t>
+  </si>
+  <si>
+    <t>SRS_Client_003</t>
+  </si>
+  <si>
+    <t>SRS_Client_004</t>
+  </si>
+  <si>
+    <t>SRS_Client_005</t>
+  </si>
+  <si>
+    <t>SRS_Client_006</t>
+  </si>
+  <si>
+    <t>SRS_Client_007</t>
+  </si>
+  <si>
+    <t>SRS_Client_008</t>
+  </si>
+  <si>
+    <t>SRS_Client_009</t>
+  </si>
+  <si>
+    <t>SRS_Client_0010</t>
+  </si>
+  <si>
+    <t>SRS_Client_011</t>
+  </si>
+  <si>
+    <t>SRS_Client_012</t>
+  </si>
+  <si>
+    <t>SRS_Client_013</t>
+  </si>
+  <si>
+    <t>SRS_Client_014</t>
+  </si>
+  <si>
+    <t>SRS_Client_015</t>
+  </si>
+  <si>
+    <t>TC_Client_001</t>
+  </si>
+  <si>
+    <t>TC_Client_002</t>
+  </si>
+  <si>
+    <t>TC_Client_007</t>
+  </si>
+  <si>
+    <t>TC_Client_008</t>
+  </si>
+  <si>
+    <t>TC_Client_009</t>
+  </si>
+  <si>
+    <t>TC_Client_013</t>
+  </si>
+  <si>
+    <t>TC_Client_014</t>
+  </si>
+  <si>
+    <t>TC_Client_003</t>
+  </si>
+  <si>
+    <t>TC_Client_004                            TC_Client_005                             TC_Client_006</t>
+  </si>
+  <si>
+    <t>TC_Client_010                               TC_Client_011                       TC_Client_012</t>
+  </si>
+  <si>
+    <t>TC_Client_015                             TC_Client_016</t>
+  </si>
+  <si>
+    <t>TC_Client_017</t>
+  </si>
+  <si>
+    <t>TC_Client_018</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_001</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_002</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_003</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_004</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_005</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_006</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_007</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_008</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_009</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_010</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_011</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_012</t>
+  </si>
+  <si>
+    <t>WireFrame_Reg_013</t>
+  </si>
+  <si>
+    <t>WireFrame_Client_001</t>
+  </si>
+  <si>
+    <t>WireFrame_Client_002
+WireFrame_Client_003</t>
+  </si>
+  <si>
+    <t>WireFrame_Client_004</t>
+  </si>
+  <si>
+    <t>Wireframe_Checkout_001</t>
+  </si>
+  <si>
+    <t>WireFrame Design ID</t>
+  </si>
+  <si>
+    <t>WireFrame_Supplier_001</t>
+  </si>
+  <si>
+    <t>WireFrame_Supplier_002</t>
+  </si>
+  <si>
+    <t>WireFrame_Supplier_003
+WireFrame_Supplier_004</t>
+  </si>
+  <si>
+    <t>WireFrame_Supplier_005</t>
+  </si>
+  <si>
+    <t>WireFrame_Supplier_006</t>
+  </si>
+  <si>
+    <t>WireFrame_Supplier_007</t>
+  </si>
+  <si>
+    <t>WireFrame_Supplier_008</t>
+  </si>
+  <si>
+    <t>WireFrame_Supplier_009</t>
+  </si>
+  <si>
+    <t>WireFrame_Cart_001</t>
+  </si>
+  <si>
+    <t>WireFrame_OrderHistory_001</t>
+  </si>
+  <si>
+    <t>WireFrame_OrderHistory_002</t>
+  </si>
+  <si>
+    <t>WireFrame_shoppingcart_003</t>
+  </si>
+  <si>
+    <t>WireFrame_shoppingcart_002</t>
+  </si>
+  <si>
+    <t>WireFrame_shoppingcart_004</t>
+  </si>
+  <si>
+    <t>WireFrame_Cart_001
+WireFrame_Cart_005</t>
+  </si>
+  <si>
+    <t>WireFrame_Login_005</t>
+  </si>
+  <si>
+    <t>WireFrame_Login_002</t>
+  </si>
+  <si>
+    <t>WireFrame_Login_003
+WireFrame_Login_004
+WireFrame_Login_005</t>
   </si>
   <si>
     <t xml:space="preserve">TC_Login_002
 TC_Login_003
 TC_Login_004
 TC_Login_009
-TC_Login_0010
+TC_Login_010
 TC_Login_0011
 </t>
   </si>
   <si>
-    <t>TC_Login_014</t>
-  </si>
-  <si>
-    <t>SRS_Register_001</t>
-  </si>
-  <si>
-    <t>TC_Register_001</t>
-  </si>
-  <si>
-    <t>SRS_Register_002</t>
-  </si>
-  <si>
-    <t>TC_Register_002</t>
-  </si>
-  <si>
-    <t>SRS_Register_003</t>
-  </si>
-  <si>
-    <t>TC_Register_003</t>
-  </si>
-  <si>
-    <t>SRS_Register_004</t>
-  </si>
-  <si>
-    <t>TC_Register_004</t>
-  </si>
-  <si>
-    <t>SRS_Register_005</t>
-  </si>
-  <si>
-    <t>TC_Register_005</t>
-  </si>
-  <si>
-    <t>SRS_Register_006</t>
-  </si>
-  <si>
-    <t>TC_Register_006</t>
-  </si>
-  <si>
-    <t>SRS_Register_007</t>
-  </si>
-  <si>
-    <t>TC_Register_007</t>
-  </si>
-  <si>
-    <t>SRS_Register_008</t>
-  </si>
-  <si>
-    <t>TC_Register_008</t>
-  </si>
-  <si>
-    <t>SRS_Register_009</t>
-  </si>
-  <si>
-    <t>TC_Register_009</t>
-  </si>
-  <si>
-    <t>SRS_Register_010</t>
-  </si>
-  <si>
-    <t>TC_Register_010</t>
-  </si>
-  <si>
-    <t>SRS_Register_011</t>
-  </si>
-  <si>
-    <t>TC_Register_011</t>
-  </si>
-  <si>
-    <t>SRS_Register_012</t>
-  </si>
-  <si>
-    <t>TC_Register_012</t>
-  </si>
-  <si>
-    <t>SRS_Register_013</t>
-  </si>
-  <si>
-    <t>TC_Register_013</t>
-  </si>
-  <si>
-    <t>SRS_Register_014</t>
-  </si>
-  <si>
-    <t>TC_Register_014</t>
-  </si>
-  <si>
-    <t>SRS_Register_015</t>
-  </si>
-  <si>
-    <t>TC_Register_015</t>
-  </si>
-  <si>
-    <t>SRS_Register_016</t>
-  </si>
-  <si>
-    <t>TC_Register_016</t>
-  </si>
-  <si>
-    <t>SRS_Register_017</t>
-  </si>
-  <si>
-    <t>TC_Register_017</t>
-  </si>
-  <si>
-    <t>SRS_Register_018</t>
-  </si>
-  <si>
-    <t>SRS_Register_019</t>
-  </si>
-  <si>
-    <t>SRS_Supplier_001</t>
-  </si>
-  <si>
-    <t>TC_Supplier_001</t>
-  </si>
-  <si>
-    <t>SRS_Supplier_002</t>
-  </si>
-  <si>
-    <t>TC_Supplier_002
-TC_Supplier_003</t>
-  </si>
-  <si>
-    <t>SRS_Supplier_003</t>
-  </si>
-  <si>
-    <t>TC_Supplier_004</t>
-  </si>
-  <si>
-    <t>SRS_Supplier_004</t>
-  </si>
-  <si>
-    <t>TC_Supplier_005</t>
-  </si>
-  <si>
-    <t>SRS_Supplier_005</t>
-  </si>
-  <si>
-    <t>SRS_Supplier_006</t>
-  </si>
-  <si>
-    <t>TC_Supplier_006</t>
-  </si>
-  <si>
-    <t>SRS_Supplier_007</t>
-  </si>
-  <si>
-    <t>TC_Supplier_007</t>
-  </si>
-  <si>
-    <t>SRS_Supplier_008</t>
-  </si>
-  <si>
-    <t>TC_Supplier_008</t>
-  </si>
-  <si>
-    <t>SRS_Client_001</t>
-  </si>
-  <si>
-    <t>SRS_Client_002</t>
-  </si>
-  <si>
-    <t>SRS_Client_003</t>
-  </si>
-  <si>
-    <t>SRS_Client_004</t>
-  </si>
-  <si>
-    <t>SRS_Client_005</t>
-  </si>
-  <si>
-    <t>SRS_Client_006</t>
-  </si>
-  <si>
-    <t>SRS_Client_007</t>
-  </si>
-  <si>
-    <t>SRS_Client_008</t>
-  </si>
-  <si>
-    <t>SRS_Client_009</t>
-  </si>
-  <si>
-    <t>SRS_Client_0010</t>
-  </si>
-  <si>
-    <t>SRS_Client_011</t>
-  </si>
-  <si>
-    <t>SRS_Client_012</t>
-  </si>
-  <si>
-    <t>SRS_Client_013</t>
-  </si>
-  <si>
-    <t>SRS_Client_014</t>
-  </si>
-  <si>
-    <t>SRS_Client_015</t>
-  </si>
-  <si>
-    <t>TC_Client_001</t>
-  </si>
-  <si>
-    <t>TC_Client_002</t>
-  </si>
-  <si>
-    <t>TC_Client_007</t>
-  </si>
-  <si>
-    <t>TC_Client_008</t>
-  </si>
-  <si>
-    <t>TC_Client_009</t>
-  </si>
-  <si>
-    <t>TC_Client_013</t>
-  </si>
-  <si>
-    <t>TC_Client_014</t>
-  </si>
-  <si>
-    <t>TC_Client_003</t>
-  </si>
-  <si>
-    <t>TC_Client_004                            TC_Client_005                             TC_Client_006</t>
-  </si>
-  <si>
-    <t>TC_Client_010                               TC_Client_011                       TC_Client_012</t>
-  </si>
-  <si>
-    <t>TC_Client_015                             TC_Client_016</t>
-  </si>
-  <si>
-    <t>TC_Client_017</t>
-  </si>
-  <si>
-    <t>TC_Client_018</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_001</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_002</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_003</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_004</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_005</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_006</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_007</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_008</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_009</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_010</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_011</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_012</t>
-  </si>
-  <si>
-    <t>WireFrame_Reg_013</t>
-  </si>
-  <si>
-    <t>WireFrame_Client_001</t>
-  </si>
-  <si>
-    <t>WireFrame_Client_002
-WireFrame_Client_003</t>
-  </si>
-  <si>
-    <t>WireFrame_Client_004</t>
-  </si>
-  <si>
-    <t>Wireframe_Checkout_001</t>
-  </si>
-  <si>
-    <t>WireFrame Design ID</t>
-  </si>
-  <si>
-    <t>WireFrame_Supplier_001</t>
-  </si>
-  <si>
-    <t>WireFrame_Supplier_002</t>
-  </si>
-  <si>
-    <t>WireFrame_Supplier_003
-WireFrame_Supplier_004</t>
-  </si>
-  <si>
-    <t>WireFrame_Supplier_005</t>
-  </si>
-  <si>
-    <t>WireFrame_Supplier_006</t>
-  </si>
-  <si>
-    <t>WireFrame_Supplier_007</t>
-  </si>
-  <si>
-    <t>WireFrame_Supplier_008</t>
-  </si>
-  <si>
-    <t>WireFrame_Supplier_009</t>
-  </si>
-  <si>
-    <t>WireFrame_Cart_001</t>
-  </si>
-  <si>
-    <t>WireFrame_OrderHistory_001</t>
-  </si>
-  <si>
-    <t>WireFrame_OrderHistory_002</t>
-  </si>
-  <si>
-    <t>WireFrame_shoppingcart_003</t>
-  </si>
-  <si>
-    <t>WireFrame_shoppingcart_002</t>
-  </si>
-  <si>
-    <t>WireFrame_shoppingcart_004</t>
-  </si>
-  <si>
-    <t>WireFrame_Cart_001
-WireFrame_Cart_005</t>
-  </si>
-  <si>
-    <t>WireFrame_Login_005</t>
-  </si>
-  <si>
-    <t>WireFrame_Login_002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_Login_002
-TC_Login_005
+    <t>SRS_Login_006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_Login_001 
+TC_Login_008 </t>
+  </si>
+  <si>
+    <t>TC_Login_005
 TC_Login_006
 TC_Login_007
-TC_Login_0012
-TC_Login_0013
-</t>
-  </si>
-  <si>
-    <t>WireFrame_Login_003
-WireFrame_Login_004
-WireFrame_Login_005</t>
+TC_Login_012
+TC_Login_013</t>
+  </si>
+  <si>
+    <t>TC_Login_001
+TC_Login_002
+TC_Login_003
+TC_Login_008
+TC_Login_009
+TC_Login_010
+TC_Login_014</t>
   </si>
 </sst>
 </file>
@@ -559,7 +564,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -587,6 +592,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -809,8 +817,8 @@
   </sheetPr>
   <dimension ref="A1:C248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -828,249 +836,249 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>7</v>
+      <c r="B21" s="8" t="s">
+        <v>125</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>9</v>
+        <v>125</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>11</v>
+      <c r="B23" s="15" t="s">
+        <v>127</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1078,285 +1086,285 @@
         <v>5</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>10</v>
+      <c r="B25" s="15" t="s">
+        <v>123</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="15" t="s">
         <v>126</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2357,5 +2365,6 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Doc: updated Traceability between Wireframes and system design for add_new_product Feature
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E3CA75-686D-4180-BBA2-948695923666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E3DC1E-4796-4763-985D-AD14D2D7856A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="148">
   <si>
     <t>SRS ID</t>
   </si>
@@ -476,6 +476,46 @@
   <si>
     <t xml:space="preserve">                                                   
 TC_Supplier_017</t>
+  </si>
+  <si>
+    <t>System Design ID</t>
+  </si>
+  <si>
+    <t>CD_AddNewProduct_page
+FC_AddNewProduct_page
+SD_AddNewProduct_002</t>
+  </si>
+  <si>
+    <t>CD_AddNewProduct_page
+FC_AddNewProduct_page
+SD_AddNewProduct_001
+SD_AddNewProduct_003
+UI_AddNewProduct_001</t>
+  </si>
+  <si>
+    <t>CD_AddNewProduct_page
+FC_AddNewProduct_page
+SD_AddNewProduct_002
+UI_AddNewProduct_002
+UI_AddNewProduct_003</t>
+  </si>
+  <si>
+    <t>CD_AddNewProduct_page
+FC_AddNewProduct_page
+SD_AddNewProduct_002
+UI_AddNewProduct_004</t>
+  </si>
+  <si>
+    <t>CD_AddNewProduct_page
+FC_AddNewProduct_page
+SD_AddNewProduct_002
+UI_AddNewProduct_005</t>
+  </si>
+  <si>
+    <t>CD_AddNewProduct_page
+FC_AddNewProduct_page
+SD_AddNewProduct_002
+UI_AddNewProduct_006</t>
   </si>
 </sst>
 </file>
@@ -612,7 +652,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -646,6 +686,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -864,10 +905,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C249"/>
+  <dimension ref="A1:D249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -875,9 +916,10 @@
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="37.42578125" customWidth="1"/>
     <col min="3" max="3" width="42.28515625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -887,8 +929,11 @@
       <c r="C1" s="13" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -898,8 +943,9 @@
       <c r="C2" s="10" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="15"/>
+    </row>
+    <row r="3" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -909,8 +955,9 @@
       <c r="C3" s="10" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -920,8 +967,9 @@
       <c r="C4" s="10" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="15"/>
+    </row>
+    <row r="5" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -931,8 +979,9 @@
       <c r="C5" s="10" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="15"/>
+    </row>
+    <row r="6" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -942,8 +991,9 @@
       <c r="C6" s="10" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="15"/>
+    </row>
+    <row r="7" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -953,8 +1003,9 @@
       <c r="C7" s="10" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="15"/>
+    </row>
+    <row r="8" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -964,8 +1015,9 @@
       <c r="C8" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="15"/>
+    </row>
+    <row r="9" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -975,8 +1027,9 @@
       <c r="C9" s="10" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="15"/>
+    </row>
+    <row r="10" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -986,8 +1039,9 @@
       <c r="C10" s="10" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="15"/>
+    </row>
+    <row r="11" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -997,8 +1051,9 @@
       <c r="C11" s="10" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -1008,8 +1063,9 @@
       <c r="C12" s="10" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1019,8 +1075,9 @@
       <c r="C13" s="10" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="15"/>
+    </row>
+    <row r="14" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1030,8 +1087,9 @@
       <c r="C14" s="10" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="15"/>
+    </row>
+    <row r="15" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
@@ -1041,8 +1099,9 @@
       <c r="C15" s="10" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="15"/>
+    </row>
+    <row r="16" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
@@ -1052,8 +1111,9 @@
       <c r="C16" s="10" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="15"/>
+    </row>
+    <row r="17" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
@@ -1063,8 +1123,9 @@
       <c r="C17" s="10" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="15"/>
+    </row>
+    <row r="18" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
@@ -1074,8 +1135,9 @@
       <c r="C18" s="10" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="15"/>
+    </row>
+    <row r="19" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
@@ -1085,8 +1147,9 @@
       <c r="C19" s="10" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>2</v>
       </c>
@@ -1096,8 +1159,9 @@
       <c r="C20" s="10" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="15"/>
+    </row>
+    <row r="21" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>3</v>
       </c>
@@ -1107,8 +1171,9 @@
       <c r="C21" s="10" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="154.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="15"/>
+    </row>
+    <row r="22" spans="1:4" ht="154.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>4</v>
       </c>
@@ -1118,8 +1183,9 @@
       <c r="C22" s="10" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="15"/>
+    </row>
+    <row r="23" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>5</v>
       </c>
@@ -1129,8 +1195,9 @@
       <c r="C23" s="10" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="15"/>
+    </row>
+    <row r="24" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
@@ -1140,8 +1207,9 @@
       <c r="C24" s="10" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="15"/>
+    </row>
+    <row r="25" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>98</v>
       </c>
@@ -1151,8 +1219,9 @@
       <c r="C25" s="10" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="15"/>
+    </row>
+    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>34</v>
       </c>
@@ -1162,8 +1231,11 @@
       <c r="C26" s="11" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>35</v>
       </c>
@@ -1173,8 +1245,11 @@
       <c r="C27" s="11" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>36</v>
       </c>
@@ -1184,8 +1259,11 @@
       <c r="C28" s="11" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>37</v>
       </c>
@@ -1195,8 +1273,11 @@
       <c r="C29" s="11" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
@@ -1206,8 +1287,11 @@
       <c r="C30" s="11" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>39</v>
       </c>
@@ -1215,10 +1299,13 @@
         <v>136</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>40</v>
       </c>
@@ -1226,10 +1313,13 @@
         <v>137</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>42</v>
       </c>
@@ -1237,28 +1327,37 @@
         <v>41</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="D33" s="15"/>
+    </row>
+    <row r="34" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>138</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="11"/>
-    </row>
-    <row r="35" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="15"/>
+    </row>
+    <row r="35" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>139</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="C35" s="11"/>
-    </row>
-    <row r="36" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>44</v>
       </c>
@@ -1268,8 +1367,9 @@
       <c r="C36" s="10" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="15"/>
+    </row>
+    <row r="37" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>45</v>
       </c>
@@ -1279,8 +1379,9 @@
       <c r="C37" s="10" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="15"/>
+    </row>
+    <row r="38" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>46</v>
       </c>
@@ -1290,8 +1391,9 @@
       <c r="C38" s="10" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D38" s="15"/>
+    </row>
+    <row r="39" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>47</v>
       </c>
@@ -1301,8 +1403,9 @@
       <c r="C39" s="10" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D39" s="15"/>
+    </row>
+    <row r="40" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>48</v>
       </c>
@@ -1312,8 +1415,9 @@
       <c r="C40" s="10" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D40" s="15"/>
+    </row>
+    <row r="41" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>49</v>
       </c>
@@ -1323,8 +1427,9 @@
       <c r="C41" s="10" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D41" s="15"/>
+    </row>
+    <row r="42" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>50</v>
       </c>
@@ -1334,8 +1439,9 @@
       <c r="C42" s="10" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D42" s="15"/>
+    </row>
+    <row r="43" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>51</v>
       </c>
@@ -1345,8 +1451,9 @@
       <c r="C43" s="10" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+      <c r="D43" s="15"/>
+    </row>
+    <row r="44" spans="1:4" ht="27" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>52</v>
       </c>
@@ -1356,8 +1463,9 @@
       <c r="C44" s="10" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D44" s="15"/>
+    </row>
+    <row r="45" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>102</v>
       </c>
@@ -1367,8 +1475,9 @@
       <c r="C45" s="10" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D45" s="15"/>
+    </row>
+    <row r="46" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>53</v>
       </c>
@@ -1378,8 +1487,9 @@
       <c r="C46" s="10" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D46" s="15"/>
+    </row>
+    <row r="47" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>54</v>
       </c>
@@ -1389,8 +1499,9 @@
       <c r="C47" s="10" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D47" s="15"/>
+    </row>
+    <row r="48" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>55</v>
       </c>
@@ -1400,8 +1511,9 @@
       <c r="C48" s="10" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D48" s="15"/>
+    </row>
+    <row r="49" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>56</v>
       </c>
@@ -1411,8 +1523,9 @@
       <c r="C49" s="10" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D49" s="15"/>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>57</v>
       </c>
@@ -1422,8 +1535,9 @@
       <c r="C50" s="10" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D50" s="15"/>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>103</v>
       </c>
@@ -1433,8 +1547,9 @@
       <c r="C51" s="10" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D51" s="15"/>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>104</v>
       </c>
@@ -1444,8 +1559,9 @@
       <c r="C52" s="10" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D52" s="15"/>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>105</v>
       </c>
@@ -1455,8 +1571,9 @@
       <c r="C53" s="10" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D53" s="15"/>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>106</v>
       </c>
@@ -1466,8 +1583,9 @@
       <c r="C54" s="10" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D54" s="15"/>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>107</v>
       </c>
@@ -1477,608 +1595,717 @@
       <c r="C55" s="10" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D55" s="15"/>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="10"/>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D56" s="15"/>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="10"/>
-    </row>
-    <row r="58" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D57" s="15"/>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="10"/>
-    </row>
-    <row r="59" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D58" s="15"/>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="9"/>
       <c r="C59" s="10"/>
-    </row>
-    <row r="60" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D59" s="15"/>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="9"/>
       <c r="C60" s="10"/>
-    </row>
-    <row r="61" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D60" s="15"/>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="9"/>
       <c r="C61" s="10"/>
-    </row>
-    <row r="62" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D61" s="15"/>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="9"/>
       <c r="C62" s="10"/>
-    </row>
-    <row r="63" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D62" s="15"/>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="9"/>
       <c r="C63" s="10"/>
-    </row>
-    <row r="64" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D63" s="15"/>
+    </row>
+    <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="9"/>
       <c r="C64" s="10"/>
-    </row>
-    <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D64" s="15"/>
+    </row>
+    <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="9"/>
       <c r="C65" s="10"/>
-    </row>
-    <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D65" s="15"/>
+    </row>
+    <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="9"/>
       <c r="C66" s="10"/>
-    </row>
-    <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D66" s="15"/>
+    </row>
+    <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="9"/>
       <c r="C67" s="10"/>
-    </row>
-    <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D67" s="15"/>
+    </row>
+    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="9"/>
       <c r="C68" s="10"/>
-    </row>
-    <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D68" s="15"/>
+    </row>
+    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="9"/>
       <c r="C69" s="10"/>
-    </row>
-    <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D69" s="15"/>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="9"/>
       <c r="C70" s="10"/>
-    </row>
-    <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D70" s="15"/>
+    </row>
+    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="9"/>
       <c r="C71" s="10"/>
-    </row>
-    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D71" s="15"/>
+    </row>
+    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="9"/>
       <c r="C72" s="10"/>
-    </row>
-    <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D72" s="15"/>
+    </row>
+    <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="9"/>
       <c r="C73" s="10"/>
-    </row>
-    <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D73" s="15"/>
+    </row>
+    <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="9"/>
       <c r="C74" s="10"/>
-    </row>
-    <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D74" s="15"/>
+    </row>
+    <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="9"/>
       <c r="C75" s="10"/>
-    </row>
-    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D75" s="15"/>
+    </row>
+    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="9"/>
       <c r="C76" s="10"/>
-    </row>
-    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D76" s="15"/>
+    </row>
+    <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="9"/>
       <c r="C77" s="10"/>
-    </row>
-    <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D77" s="15"/>
+    </row>
+    <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="9"/>
       <c r="C78" s="10"/>
-    </row>
-    <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D78" s="15"/>
+    </row>
+    <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="9"/>
       <c r="C79" s="10"/>
-    </row>
-    <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D79" s="15"/>
+    </row>
+    <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="9"/>
       <c r="C80" s="10"/>
-    </row>
-    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D80" s="15"/>
+    </row>
+    <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="9"/>
       <c r="C81" s="10"/>
-    </row>
-    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D81" s="15"/>
+    </row>
+    <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="9"/>
       <c r="C82" s="10"/>
-    </row>
-    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D82" s="15"/>
+    </row>
+    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="9"/>
       <c r="C83" s="10"/>
-    </row>
-    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D83" s="15"/>
+    </row>
+    <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="9"/>
       <c r="C84" s="10"/>
-    </row>
-    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D84" s="15"/>
+    </row>
+    <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="9"/>
       <c r="C85" s="10"/>
-    </row>
-    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D85" s="15"/>
+    </row>
+    <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="9"/>
       <c r="C86" s="10"/>
-    </row>
-    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D86" s="15"/>
+    </row>
+    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="9"/>
       <c r="C87" s="10"/>
-    </row>
-    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D87" s="15"/>
+    </row>
+    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="9"/>
       <c r="C88" s="10"/>
-    </row>
-    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D88" s="15"/>
+    </row>
+    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="9"/>
       <c r="C89" s="10"/>
-    </row>
-    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D89" s="15"/>
+    </row>
+    <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="9"/>
       <c r="C90" s="10"/>
-    </row>
-    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D90" s="15"/>
+    </row>
+    <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="9"/>
       <c r="C91" s="10"/>
-    </row>
-    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D91" s="15"/>
+    </row>
+    <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="9"/>
       <c r="C92" s="10"/>
-    </row>
-    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D92" s="15"/>
+    </row>
+    <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="9"/>
       <c r="C93" s="10"/>
-    </row>
-    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D93" s="15"/>
+    </row>
+    <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="9"/>
       <c r="C94" s="10"/>
-    </row>
-    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D94" s="15"/>
+    </row>
+    <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="9"/>
       <c r="C95" s="10"/>
-    </row>
-    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D95" s="15"/>
+    </row>
+    <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="9"/>
       <c r="C96" s="10"/>
-    </row>
-    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D96" s="15"/>
+    </row>
+    <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="9"/>
       <c r="C97" s="10"/>
-    </row>
-    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D97" s="15"/>
+    </row>
+    <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="9"/>
       <c r="C98" s="10"/>
-    </row>
-    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D98" s="15"/>
+    </row>
+    <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="9"/>
       <c r="C99" s="10"/>
-    </row>
-    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D99" s="15"/>
+    </row>
+    <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="9"/>
       <c r="C100" s="10"/>
-    </row>
-    <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D100" s="15"/>
+    </row>
+    <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="9"/>
       <c r="C101" s="10"/>
-    </row>
-    <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D101" s="15"/>
+    </row>
+    <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="9"/>
       <c r="C102" s="10"/>
-    </row>
-    <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D102" s="15"/>
+    </row>
+    <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="9"/>
       <c r="C103" s="10"/>
-    </row>
-    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D103" s="15"/>
+    </row>
+    <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="9"/>
       <c r="C104" s="10"/>
-    </row>
-    <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D104" s="15"/>
+    </row>
+    <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="9"/>
       <c r="C105" s="10"/>
-    </row>
-    <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D105" s="15"/>
+    </row>
+    <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="9"/>
       <c r="C106" s="10"/>
-    </row>
-    <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D106" s="15"/>
+    </row>
+    <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="9"/>
       <c r="C107" s="10"/>
-    </row>
-    <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D107" s="15"/>
+    </row>
+    <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="9"/>
       <c r="C108" s="10"/>
-    </row>
-    <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D108" s="15"/>
+    </row>
+    <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="9"/>
       <c r="C109" s="10"/>
-    </row>
-    <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D109" s="15"/>
+    </row>
+    <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="9"/>
       <c r="C110" s="10"/>
-    </row>
-    <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D110" s="15"/>
+    </row>
+    <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="9"/>
       <c r="C111" s="10"/>
-    </row>
-    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D111" s="15"/>
+    </row>
+    <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="9"/>
       <c r="C112" s="10"/>
-    </row>
-    <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D112" s="15"/>
+    </row>
+    <row r="113" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="9"/>
       <c r="C113" s="10"/>
-    </row>
-    <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D113" s="15"/>
+    </row>
+    <row r="114" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="9"/>
       <c r="C114" s="10"/>
-    </row>
-    <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D114" s="15"/>
+    </row>
+    <row r="115" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="9"/>
       <c r="C115" s="10"/>
-    </row>
-    <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D115" s="15"/>
+    </row>
+    <row r="116" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="9"/>
       <c r="C116" s="10"/>
-    </row>
-    <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D116" s="15"/>
+    </row>
+    <row r="117" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="9"/>
       <c r="C117" s="10"/>
-    </row>
-    <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D117" s="15"/>
+    </row>
+    <row r="118" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="9"/>
       <c r="C118" s="10"/>
-    </row>
-    <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D118" s="15"/>
+    </row>
+    <row r="119" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="9"/>
       <c r="C119" s="10"/>
-    </row>
-    <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D119" s="15"/>
+    </row>
+    <row r="120" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="9"/>
       <c r="C120" s="10"/>
-    </row>
-    <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D120" s="15"/>
+    </row>
+    <row r="121" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="9"/>
       <c r="C121" s="10"/>
-    </row>
-    <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D121" s="15"/>
+    </row>
+    <row r="122" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="9"/>
       <c r="C122" s="10"/>
-    </row>
-    <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D122" s="15"/>
+    </row>
+    <row r="123" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="9"/>
       <c r="C123" s="10"/>
-    </row>
-    <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D123" s="15"/>
+    </row>
+    <row r="124" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="9"/>
       <c r="C124" s="10"/>
-    </row>
-    <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D124" s="15"/>
+    </row>
+    <row r="125" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="9"/>
       <c r="C125" s="10"/>
-    </row>
-    <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D125" s="15"/>
+    </row>
+    <row r="126" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="9"/>
       <c r="C126" s="10"/>
-    </row>
-    <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D126" s="15"/>
+    </row>
+    <row r="127" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="9"/>
       <c r="C127" s="10"/>
-    </row>
-    <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D127" s="15"/>
+    </row>
+    <row r="128" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="9"/>
       <c r="C128" s="10"/>
-    </row>
-    <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D128" s="15"/>
+    </row>
+    <row r="129" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="9"/>
       <c r="C129" s="10"/>
-    </row>
-    <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D129" s="15"/>
+    </row>
+    <row r="130" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="9"/>
       <c r="C130" s="10"/>
-    </row>
-    <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D130" s="15"/>
+    </row>
+    <row r="131" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="9"/>
       <c r="C131" s="10"/>
-    </row>
-    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D131" s="15"/>
+    </row>
+    <row r="132" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="9"/>
       <c r="C132" s="10"/>
-    </row>
-    <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D132" s="15"/>
+    </row>
+    <row r="133" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="9"/>
       <c r="C133" s="10"/>
-    </row>
-    <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D133" s="15"/>
+    </row>
+    <row r="134" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="9"/>
       <c r="C134" s="10"/>
-    </row>
-    <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D134" s="15"/>
+    </row>
+    <row r="135" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="9"/>
       <c r="C135" s="10"/>
-    </row>
-    <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D135" s="15"/>
+    </row>
+    <row r="136" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="9"/>
       <c r="C136" s="10"/>
-    </row>
-    <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D136" s="15"/>
+    </row>
+    <row r="137" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="B137" s="9"/>
       <c r="C137" s="10"/>
-    </row>
-    <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D137" s="15"/>
+    </row>
+    <row r="138" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
       <c r="B138" s="9"/>
       <c r="C138" s="10"/>
-    </row>
-    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D138" s="15"/>
+    </row>
+    <row r="139" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
       <c r="B139" s="9"/>
       <c r="C139" s="10"/>
-    </row>
-    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D139" s="15"/>
+    </row>
+    <row r="140" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140" s="9"/>
       <c r="C140" s="10"/>
-    </row>
-    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D140" s="15"/>
+    </row>
+    <row r="141" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141" s="9"/>
       <c r="C141" s="10"/>
-    </row>
-    <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D141" s="15"/>
+    </row>
+    <row r="142" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142" s="9"/>
       <c r="C142" s="10"/>
-    </row>
-    <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D142" s="15"/>
+    </row>
+    <row r="143" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
       <c r="B143" s="9"/>
       <c r="C143" s="10"/>
-    </row>
-    <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D143" s="15"/>
+    </row>
+    <row r="144" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
       <c r="B144" s="9"/>
       <c r="C144" s="10"/>
-    </row>
-    <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D144" s="15"/>
+    </row>
+    <row r="145" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
       <c r="B145" s="9"/>
       <c r="C145" s="10"/>
-    </row>
-    <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D145" s="15"/>
+    </row>
+    <row r="146" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
       <c r="B146" s="9"/>
       <c r="C146" s="10"/>
-    </row>
-    <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D146" s="15"/>
+    </row>
+    <row r="147" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
       <c r="B147" s="9"/>
       <c r="C147" s="10"/>
-    </row>
-    <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D147" s="15"/>
+    </row>
+    <row r="148" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
       <c r="B148" s="9"/>
       <c r="C148" s="10"/>
-    </row>
-    <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D148" s="15"/>
+    </row>
+    <row r="149" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
       <c r="B149" s="9"/>
       <c r="C149" s="10"/>
-    </row>
-    <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D149" s="15"/>
+    </row>
+    <row r="150" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
       <c r="B150" s="9"/>
       <c r="C150" s="10"/>
-    </row>
-    <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D150" s="15"/>
+    </row>
+    <row r="151" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2"/>
       <c r="B151" s="9"/>
       <c r="C151" s="10"/>
-    </row>
-    <row r="152" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D151" s="15"/>
+    </row>
+    <row r="152" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2"/>
       <c r="B152" s="9"/>
       <c r="C152" s="10"/>
-    </row>
-    <row r="153" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D152" s="15"/>
+    </row>
+    <row r="153" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2"/>
       <c r="B153" s="9"/>
       <c r="C153" s="10"/>
-    </row>
-    <row r="154" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D153" s="15"/>
+    </row>
+    <row r="154" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2"/>
       <c r="B154" s="9"/>
       <c r="C154" s="10"/>
-    </row>
-    <row r="155" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D154" s="15"/>
+    </row>
+    <row r="155" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2"/>
       <c r="B155" s="9"/>
       <c r="C155" s="10"/>
-    </row>
-    <row r="156" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D155" s="15"/>
+    </row>
+    <row r="156" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2"/>
       <c r="B156" s="9"/>
       <c r="C156" s="10"/>
-    </row>
-    <row r="157" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D156" s="15"/>
+    </row>
+    <row r="157" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2"/>
       <c r="B157" s="9"/>
       <c r="C157" s="10"/>
-    </row>
-    <row r="158" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D157" s="15"/>
+    </row>
+    <row r="158" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2"/>
       <c r="B158" s="9"/>
       <c r="C158" s="10"/>
-    </row>
-    <row r="159" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D158" s="15"/>
+    </row>
+    <row r="159" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2"/>
       <c r="B159" s="9"/>
       <c r="C159" s="10"/>
-    </row>
-    <row r="160" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D159" s="15"/>
+    </row>
+    <row r="160" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2"/>
       <c r="B160" s="9"/>
       <c r="C160" s="10"/>
-    </row>
-    <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D160" s="15"/>
+    </row>
+    <row r="161" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2"/>
       <c r="B161" s="9"/>
       <c r="C161" s="10"/>
-    </row>
-    <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D161" s="15"/>
+    </row>
+    <row r="162" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2"/>
       <c r="B162" s="9"/>
       <c r="C162" s="10"/>
-    </row>
-    <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D162" s="15"/>
+    </row>
+    <row r="163" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
       <c r="B163" s="9"/>
       <c r="C163" s="10"/>
-    </row>
-    <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D163" s="15"/>
+    </row>
+    <row r="164" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2"/>
       <c r="B164" s="9"/>
       <c r="C164" s="10"/>
     </row>
-    <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2"/>
       <c r="B165" s="9"/>
       <c r="C165" s="10"/>
     </row>
-    <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2"/>
       <c r="B166" s="9"/>
       <c r="C166" s="10"/>
     </row>
-    <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2"/>
       <c r="B167" s="9"/>
       <c r="C167" s="10"/>
     </row>
-    <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2"/>
       <c r="B168" s="9"/>
       <c r="C168" s="10"/>
     </row>
-    <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2"/>
       <c r="B169" s="9"/>
       <c r="C169" s="10"/>
     </row>
-    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2"/>
       <c r="B170" s="9"/>
       <c r="C170" s="10"/>
     </row>
-    <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2"/>
       <c r="B171" s="9"/>
       <c r="C171" s="10"/>
     </row>
-    <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2"/>
       <c r="B172" s="9"/>
       <c r="C172" s="10"/>
     </row>
-    <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2"/>
       <c r="B173" s="9"/>
       <c r="C173" s="10"/>
     </row>
-    <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2"/>
       <c r="B174" s="9"/>
       <c r="C174" s="10"/>
     </row>
-    <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2"/>
       <c r="B175" s="9"/>
       <c r="C175" s="10"/>
     </row>
-    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2"/>
       <c r="B176" s="9"/>
       <c r="C176" s="10"/>

</xml_diff>

<commit_message>
update RTM for register & login System design and UI design
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\RTM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI9M-Testing\Core\QA\WorkShop\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E3DC1E-4796-4763-985D-AD14D2D7856A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048AEA25-6BB5-4420-912F-776DE1F1457A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="171">
   <si>
     <t>SRS ID</t>
   </si>
@@ -516,6 +516,75 @@
 FC_AddNewProduct_page
 SD_AddNewProduct_002
 UI_AddNewProduct_006</t>
+  </si>
+  <si>
+    <t>CD_Register.png                 SD_Register_001.png                  UI_Register_001.png</t>
+  </si>
+  <si>
+    <t>CD_Register.png                 SD_Register_001.png                   UI_Register_001.png</t>
+  </si>
+  <si>
+    <t>CD_Register.png                 SD_Register_002.png                    FD_Register_007.png                 UI_Register_002.png</t>
+  </si>
+  <si>
+    <t>CD_Register.png                 SD_Register_002.png                    FD_Register_007.png                 UI_Register_003.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD_Register.png                 SD_Register_002.png                    FD_Register_007.png         UI_Register_004.png     </t>
+  </si>
+  <si>
+    <t>CD_Register.png                 SD_Register_002.png                    FD_Register_002.png            UI_Register_005.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD_Register.png                 SD_Register_001.png            UI_Register_001.png                        </t>
+  </si>
+  <si>
+    <t>CD_Register.png                 SD_Register_002.png                 FD_Register_005.png           UI_Register_006.png</t>
+  </si>
+  <si>
+    <t>CD_Register.png                 SD_Register_002.png                          FD_Register_001.png            UI_Register_007.png</t>
+  </si>
+  <si>
+    <t>CD_Register.png                 SD_Register_002.png                  UI_Register_008.png</t>
+  </si>
+  <si>
+    <t>CD_Register.png                 SD_Register_002.png                     FD_Register_002.png            UI_Register_009.png</t>
+  </si>
+  <si>
+    <t>CD_Register.png                 SD_Register_002.png                   FD_Register_006.png         UI_Register_010.png</t>
+  </si>
+  <si>
+    <t>CD_Register.png                 SD_Register_002.png                          FD_Register_006.png                         UI_Register_011.png</t>
+  </si>
+  <si>
+    <t>CD_Register.png                 SD_Register_001.png              UI_Register_001.png</t>
+  </si>
+  <si>
+    <t>CD_Register.png                 SD_Register_002.png                   UI_Register_012.png</t>
+  </si>
+  <si>
+    <t>CD_Register.png                   SD_Register_002.png                     FD_Register_004.png             UI_Register_013.png</t>
+  </si>
+  <si>
+    <t>CD_Register.png                  SD_Register_002.png              FD_Register_004.png             UI_Register_013.png</t>
+  </si>
+  <si>
+    <t>UI_Login_001.png                            CD_Login.png                                    SD_Login_001.png</t>
+  </si>
+  <si>
+    <t>UI_Login_002.png                                CD_Login.png                                 SD_Login_002.png                                    FD_Login_001.png</t>
+  </si>
+  <si>
+    <t>UI_Login_003.png                            CD_Login.png                                     SD_Login_002.png                                     FD_Login_001.png</t>
+  </si>
+  <si>
+    <t>UI_Login_004.png                                        CD_Login.png                        SD_Login_002.png                     FD_Login_002.png</t>
+  </si>
+  <si>
+    <t>UI_Login_005.png                          CD_Login.png                                 SD_Login_002.png                        FD_Login_002.png</t>
+  </si>
+  <si>
+    <t>UI_Login_006.png                            CD_Login.png                                     SD_Login_002.png                            FD_Login_001.png                                   FD_Login_002.png</t>
   </si>
 </sst>
 </file>
@@ -652,7 +721,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -686,7 +755,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -907,19 +975,19 @@
   </sheetPr>
   <dimension ref="A1:D249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="37.44140625" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="38.44140625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -933,7 +1001,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="59.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -943,9 +1011,11 @@
       <c r="C2" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="15"/>
-    </row>
-    <row r="3" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="99" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -955,9 +1025,11 @@
       <c r="C3" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="15"/>
-    </row>
-    <row r="4" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -967,9 +1039,11 @@
       <c r="C4" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="15"/>
-    </row>
-    <row r="5" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="73.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -979,9 +1053,11 @@
       <c r="C5" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="15"/>
-    </row>
-    <row r="6" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -991,9 +1067,11 @@
       <c r="C6" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="15"/>
-    </row>
-    <row r="7" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1003,9 +1081,11 @@
       <c r="C7" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="15"/>
-    </row>
-    <row r="8" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1015,9 +1095,11 @@
       <c r="C8" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="15"/>
-    </row>
-    <row r="9" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1027,9 +1109,11 @@
       <c r="C9" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="15"/>
-    </row>
-    <row r="10" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -1039,9 +1123,11 @@
       <c r="C10" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="15"/>
-    </row>
-    <row r="11" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="109.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -1051,9 +1137,11 @@
       <c r="C11" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="15"/>
-    </row>
-    <row r="12" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="90.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -1063,9 +1151,11 @@
       <c r="C12" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="15"/>
-    </row>
-    <row r="13" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="81" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1075,9 +1165,11 @@
       <c r="C13" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="15"/>
-    </row>
-    <row r="14" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1087,9 +1179,11 @@
       <c r="C14" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D14" s="15"/>
-    </row>
-    <row r="15" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
@@ -1099,9 +1193,11 @@
       <c r="C15" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="15"/>
-    </row>
-    <row r="16" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
@@ -1111,9 +1207,11 @@
       <c r="C16" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="15"/>
-    </row>
-    <row r="17" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="55.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
@@ -1123,9 +1221,11 @@
       <c r="C17" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="15"/>
-    </row>
-    <row r="18" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
@@ -1135,9 +1235,11 @@
       <c r="C18" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="15"/>
-    </row>
-    <row r="19" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="88.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
@@ -1147,9 +1249,11 @@
       <c r="C19" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="15"/>
-    </row>
-    <row r="20" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="55.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>2</v>
       </c>
@@ -1159,9 +1263,11 @@
       <c r="C20" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="15"/>
-    </row>
-    <row r="21" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>3</v>
       </c>
@@ -1171,9 +1277,11 @@
       <c r="C21" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D21" s="15"/>
-    </row>
-    <row r="22" spans="1:4" ht="154.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="102" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>4</v>
       </c>
@@ -1183,9 +1291,11 @@
       <c r="C22" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="15"/>
-    </row>
-    <row r="23" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>5</v>
       </c>
@@ -1195,9 +1305,11 @@
       <c r="C23" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D23" s="15"/>
-    </row>
-    <row r="24" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
@@ -1207,9 +1319,11 @@
       <c r="C24" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="15"/>
-    </row>
-    <row r="25" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>98</v>
       </c>
@@ -1219,9 +1333,11 @@
       <c r="C25" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="15"/>
-    </row>
-    <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="64.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>34</v>
       </c>
@@ -1235,7 +1351,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>35</v>
       </c>
@@ -1249,7 +1365,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>36</v>
       </c>
@@ -1263,7 +1379,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>37</v>
       </c>
@@ -1277,7 +1393,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
@@ -1291,7 +1407,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>39</v>
       </c>
@@ -1305,7 +1421,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>40</v>
       </c>
@@ -1319,7 +1435,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>42</v>
       </c>
@@ -1329,9 +1445,9 @@
       <c r="C33" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D33" s="15"/>
-    </row>
-    <row r="34" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="10"/>
+    </row>
+    <row r="34" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>138</v>
       </c>
@@ -1341,9 +1457,9 @@
       <c r="C34" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D34" s="15"/>
-    </row>
-    <row r="35" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D34" s="10"/>
+    </row>
+    <row r="35" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>139</v>
       </c>
@@ -1357,7 +1473,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>44</v>
       </c>
@@ -1367,9 +1483,9 @@
       <c r="C36" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="15"/>
-    </row>
-    <row r="37" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="10"/>
+    </row>
+    <row r="37" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>45</v>
       </c>
@@ -1379,9 +1495,9 @@
       <c r="C37" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D37" s="15"/>
-    </row>
-    <row r="38" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="10"/>
+    </row>
+    <row r="38" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>46</v>
       </c>
@@ -1391,9 +1507,9 @@
       <c r="C38" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D38" s="15"/>
-    </row>
-    <row r="39" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D38" s="10"/>
+    </row>
+    <row r="39" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>47</v>
       </c>
@@ -1403,9 +1519,9 @@
       <c r="C39" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D39" s="15"/>
-    </row>
-    <row r="40" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D39" s="10"/>
+    </row>
+    <row r="40" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>48</v>
       </c>
@@ -1415,9 +1531,9 @@
       <c r="C40" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D40" s="15"/>
-    </row>
-    <row r="41" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D40" s="10"/>
+    </row>
+    <row r="41" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>49</v>
       </c>
@@ -1427,9 +1543,9 @@
       <c r="C41" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D41" s="15"/>
-    </row>
-    <row r="42" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D41" s="10"/>
+    </row>
+    <row r="42" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>50</v>
       </c>
@@ -1439,9 +1555,9 @@
       <c r="C42" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D42" s="15"/>
-    </row>
-    <row r="43" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D42" s="10"/>
+    </row>
+    <row r="43" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>51</v>
       </c>
@@ -1451,9 +1567,9 @@
       <c r="C43" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D43" s="15"/>
-    </row>
-    <row r="44" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="D43" s="10"/>
+    </row>
+    <row r="44" spans="1:4" ht="27.6" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>52</v>
       </c>
@@ -1463,9 +1579,9 @@
       <c r="C44" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="D44" s="15"/>
-    </row>
-    <row r="45" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D44" s="10"/>
+    </row>
+    <row r="45" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>102</v>
       </c>
@@ -1475,9 +1591,9 @@
       <c r="C45" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D45" s="15"/>
-    </row>
-    <row r="46" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D45" s="10"/>
+    </row>
+    <row r="46" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>53</v>
       </c>
@@ -1487,9 +1603,9 @@
       <c r="C46" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D46" s="15"/>
-    </row>
-    <row r="47" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D46" s="10"/>
+    </row>
+    <row r="47" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>54</v>
       </c>
@@ -1499,9 +1615,9 @@
       <c r="C47" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D47" s="15"/>
-    </row>
-    <row r="48" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D47" s="10"/>
+    </row>
+    <row r="48" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>55</v>
       </c>
@@ -1511,9 +1627,9 @@
       <c r="C48" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D48" s="15"/>
-    </row>
-    <row r="49" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D48" s="10"/>
+    </row>
+    <row r="49" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>56</v>
       </c>
@@ -1523,9 +1639,9 @@
       <c r="C49" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="15"/>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D49" s="10"/>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>57</v>
       </c>
@@ -1535,9 +1651,9 @@
       <c r="C50" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D50" s="15"/>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D50" s="10"/>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>103</v>
       </c>
@@ -1547,9 +1663,9 @@
       <c r="C51" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="D51" s="15"/>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D51" s="10"/>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>104</v>
       </c>
@@ -1559,9 +1675,9 @@
       <c r="C52" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D52" s="15"/>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D52" s="10"/>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>105</v>
       </c>
@@ -1571,9 +1687,9 @@
       <c r="C53" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D53" s="15"/>
-    </row>
-    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D53" s="10"/>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>106</v>
       </c>
@@ -1583,9 +1699,9 @@
       <c r="C54" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D54" s="15"/>
-    </row>
-    <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D54" s="10"/>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>107</v>
       </c>
@@ -1595,1082 +1711,1082 @@
       <c r="C55" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D55" s="15"/>
-    </row>
-    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D55" s="10"/>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="10"/>
-      <c r="D56" s="15"/>
-    </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D56" s="10"/>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="10"/>
-      <c r="D57" s="15"/>
-    </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D57" s="10"/>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="10"/>
-      <c r="D58" s="15"/>
-    </row>
-    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D58" s="10"/>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="9"/>
       <c r="C59" s="10"/>
-      <c r="D59" s="15"/>
-    </row>
-    <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D59" s="10"/>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="9"/>
       <c r="C60" s="10"/>
-      <c r="D60" s="15"/>
-    </row>
-    <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D60" s="10"/>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="9"/>
       <c r="C61" s="10"/>
-      <c r="D61" s="15"/>
-    </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D61" s="10"/>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="9"/>
       <c r="C62" s="10"/>
-      <c r="D62" s="15"/>
-    </row>
-    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D62" s="10"/>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="9"/>
       <c r="C63" s="10"/>
-      <c r="D63" s="15"/>
-    </row>
-    <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D63" s="10"/>
+    </row>
+    <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="9"/>
       <c r="C64" s="10"/>
-      <c r="D64" s="15"/>
-    </row>
-    <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D64" s="10"/>
+    </row>
+    <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="9"/>
       <c r="C65" s="10"/>
-      <c r="D65" s="15"/>
-    </row>
-    <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D65" s="10"/>
+    </row>
+    <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="9"/>
       <c r="C66" s="10"/>
-      <c r="D66" s="15"/>
-    </row>
-    <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D66" s="10"/>
+    </row>
+    <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" s="9"/>
       <c r="C67" s="10"/>
-      <c r="D67" s="15"/>
-    </row>
-    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D67" s="10"/>
+    </row>
+    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" s="9"/>
       <c r="C68" s="10"/>
-      <c r="D68" s="15"/>
-    </row>
-    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D68" s="10"/>
+    </row>
+    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="9"/>
       <c r="C69" s="10"/>
-      <c r="D69" s="15"/>
-    </row>
-    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D69" s="10"/>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" s="9"/>
       <c r="C70" s="10"/>
-      <c r="D70" s="15"/>
-    </row>
-    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D70" s="10"/>
+    </row>
+    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="9"/>
       <c r="C71" s="10"/>
-      <c r="D71" s="15"/>
-    </row>
-    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D71" s="10"/>
+    </row>
+    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="9"/>
       <c r="C72" s="10"/>
-      <c r="D72" s="15"/>
-    </row>
-    <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D72" s="10"/>
+    </row>
+    <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="9"/>
       <c r="C73" s="10"/>
-      <c r="D73" s="15"/>
-    </row>
-    <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D73" s="10"/>
+    </row>
+    <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="9"/>
       <c r="C74" s="10"/>
-      <c r="D74" s="15"/>
-    </row>
-    <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D74" s="10"/>
+    </row>
+    <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="9"/>
       <c r="C75" s="10"/>
-      <c r="D75" s="15"/>
-    </row>
-    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D75" s="10"/>
+    </row>
+    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="9"/>
       <c r="C76" s="10"/>
-      <c r="D76" s="15"/>
-    </row>
-    <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D76" s="10"/>
+    </row>
+    <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" s="9"/>
       <c r="C77" s="10"/>
-      <c r="D77" s="15"/>
-    </row>
-    <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D77" s="10"/>
+    </row>
+    <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" s="9"/>
       <c r="C78" s="10"/>
-      <c r="D78" s="15"/>
-    </row>
-    <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D78" s="10"/>
+    </row>
+    <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" s="9"/>
       <c r="C79" s="10"/>
-      <c r="D79" s="15"/>
-    </row>
-    <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D79" s="10"/>
+    </row>
+    <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" s="9"/>
       <c r="C80" s="10"/>
-      <c r="D80" s="15"/>
-    </row>
-    <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D80" s="10"/>
+    </row>
+    <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="B81" s="9"/>
       <c r="C81" s="10"/>
-      <c r="D81" s="15"/>
-    </row>
-    <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D81" s="10"/>
+    </row>
+    <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
       <c r="B82" s="9"/>
       <c r="C82" s="10"/>
-      <c r="D82" s="15"/>
-    </row>
-    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D82" s="10"/>
+    </row>
+    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2"/>
       <c r="B83" s="9"/>
       <c r="C83" s="10"/>
-      <c r="D83" s="15"/>
-    </row>
-    <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D83" s="10"/>
+    </row>
+    <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
       <c r="B84" s="9"/>
       <c r="C84" s="10"/>
-      <c r="D84" s="15"/>
-    </row>
-    <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D84" s="10"/>
+    </row>
+    <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2"/>
       <c r="B85" s="9"/>
       <c r="C85" s="10"/>
-      <c r="D85" s="15"/>
-    </row>
-    <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D85" s="10"/>
+    </row>
+    <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" s="9"/>
       <c r="C86" s="10"/>
-      <c r="D86" s="15"/>
-    </row>
-    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D86" s="10"/>
+    </row>
+    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
       <c r="B87" s="9"/>
       <c r="C87" s="10"/>
-      <c r="D87" s="15"/>
-    </row>
-    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D87" s="10"/>
+    </row>
+    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
       <c r="B88" s="9"/>
       <c r="C88" s="10"/>
-      <c r="D88" s="15"/>
-    </row>
-    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D88" s="10"/>
+    </row>
+    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" s="9"/>
       <c r="C89" s="10"/>
-      <c r="D89" s="15"/>
-    </row>
-    <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D89" s="10"/>
+    </row>
+    <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
       <c r="B90" s="9"/>
       <c r="C90" s="10"/>
-      <c r="D90" s="15"/>
-    </row>
-    <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D90" s="10"/>
+    </row>
+    <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
       <c r="B91" s="9"/>
       <c r="C91" s="10"/>
-      <c r="D91" s="15"/>
-    </row>
-    <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D91" s="10"/>
+    </row>
+    <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
       <c r="B92" s="9"/>
       <c r="C92" s="10"/>
-      <c r="D92" s="15"/>
-    </row>
-    <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D92" s="10"/>
+    </row>
+    <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
       <c r="B93" s="9"/>
       <c r="C93" s="10"/>
-      <c r="D93" s="15"/>
-    </row>
-    <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D93" s="10"/>
+    </row>
+    <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
       <c r="B94" s="9"/>
       <c r="C94" s="10"/>
-      <c r="D94" s="15"/>
-    </row>
-    <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D94" s="10"/>
+    </row>
+    <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2"/>
       <c r="B95" s="9"/>
       <c r="C95" s="10"/>
-      <c r="D95" s="15"/>
-    </row>
-    <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D95" s="10"/>
+    </row>
+    <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
       <c r="B96" s="9"/>
       <c r="C96" s="10"/>
-      <c r="D96" s="15"/>
-    </row>
-    <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D96" s="10"/>
+    </row>
+    <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
       <c r="B97" s="9"/>
       <c r="C97" s="10"/>
-      <c r="D97" s="15"/>
-    </row>
-    <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D97" s="10"/>
+    </row>
+    <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
       <c r="B98" s="9"/>
       <c r="C98" s="10"/>
-      <c r="D98" s="15"/>
-    </row>
-    <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D98" s="10"/>
+    </row>
+    <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
       <c r="B99" s="9"/>
       <c r="C99" s="10"/>
-      <c r="D99" s="15"/>
-    </row>
-    <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D99" s="10"/>
+    </row>
+    <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
       <c r="B100" s="9"/>
       <c r="C100" s="10"/>
-      <c r="D100" s="15"/>
-    </row>
-    <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D100" s="10"/>
+    </row>
+    <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
       <c r="B101" s="9"/>
       <c r="C101" s="10"/>
-      <c r="D101" s="15"/>
-    </row>
-    <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D101" s="10"/>
+    </row>
+    <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
       <c r="B102" s="9"/>
       <c r="C102" s="10"/>
-      <c r="D102" s="15"/>
-    </row>
-    <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D102" s="10"/>
+    </row>
+    <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
       <c r="B103" s="9"/>
       <c r="C103" s="10"/>
-      <c r="D103" s="15"/>
-    </row>
-    <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D103" s="10"/>
+    </row>
+    <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="B104" s="9"/>
       <c r="C104" s="10"/>
-      <c r="D104" s="15"/>
-    </row>
-    <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D104" s="10"/>
+    </row>
+    <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
       <c r="B105" s="9"/>
       <c r="C105" s="10"/>
-      <c r="D105" s="15"/>
-    </row>
-    <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D105" s="10"/>
+    </row>
+    <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="B106" s="9"/>
       <c r="C106" s="10"/>
-      <c r="D106" s="15"/>
-    </row>
-    <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D106" s="10"/>
+    </row>
+    <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" s="9"/>
       <c r="C107" s="10"/>
-      <c r="D107" s="15"/>
-    </row>
-    <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D107" s="10"/>
+    </row>
+    <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
       <c r="B108" s="9"/>
       <c r="C108" s="10"/>
-      <c r="D108" s="15"/>
-    </row>
-    <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D108" s="10"/>
+    </row>
+    <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2"/>
       <c r="B109" s="9"/>
       <c r="C109" s="10"/>
-      <c r="D109" s="15"/>
-    </row>
-    <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D109" s="10"/>
+    </row>
+    <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="B110" s="9"/>
       <c r="C110" s="10"/>
-      <c r="D110" s="15"/>
-    </row>
-    <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D110" s="10"/>
+    </row>
+    <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2"/>
       <c r="B111" s="9"/>
       <c r="C111" s="10"/>
-      <c r="D111" s="15"/>
-    </row>
-    <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D111" s="10"/>
+    </row>
+    <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
       <c r="B112" s="9"/>
       <c r="C112" s="10"/>
-      <c r="D112" s="15"/>
-    </row>
-    <row r="113" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D112" s="10"/>
+    </row>
+    <row r="113" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
       <c r="B113" s="9"/>
       <c r="C113" s="10"/>
-      <c r="D113" s="15"/>
-    </row>
-    <row r="114" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D113" s="10"/>
+    </row>
+    <row r="114" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="B114" s="9"/>
       <c r="C114" s="10"/>
-      <c r="D114" s="15"/>
-    </row>
-    <row r="115" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D114" s="10"/>
+    </row>
+    <row r="115" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2"/>
       <c r="B115" s="9"/>
       <c r="C115" s="10"/>
-      <c r="D115" s="15"/>
-    </row>
-    <row r="116" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D115" s="10"/>
+    </row>
+    <row r="116" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2"/>
       <c r="B116" s="9"/>
       <c r="C116" s="10"/>
-      <c r="D116" s="15"/>
-    </row>
-    <row r="117" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D116" s="10"/>
+    </row>
+    <row r="117" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2"/>
       <c r="B117" s="9"/>
       <c r="C117" s="10"/>
-      <c r="D117" s="15"/>
-    </row>
-    <row r="118" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D117" s="10"/>
+    </row>
+    <row r="118" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2"/>
       <c r="B118" s="9"/>
       <c r="C118" s="10"/>
-      <c r="D118" s="15"/>
-    </row>
-    <row r="119" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D118" s="10"/>
+    </row>
+    <row r="119" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2"/>
       <c r="B119" s="9"/>
       <c r="C119" s="10"/>
-      <c r="D119" s="15"/>
-    </row>
-    <row r="120" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D119" s="10"/>
+    </row>
+    <row r="120" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2"/>
       <c r="B120" s="9"/>
       <c r="C120" s="10"/>
-      <c r="D120" s="15"/>
-    </row>
-    <row r="121" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D120" s="10"/>
+    </row>
+    <row r="121" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2"/>
       <c r="B121" s="9"/>
       <c r="C121" s="10"/>
-      <c r="D121" s="15"/>
-    </row>
-    <row r="122" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D121" s="10"/>
+    </row>
+    <row r="122" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2"/>
       <c r="B122" s="9"/>
       <c r="C122" s="10"/>
-      <c r="D122" s="15"/>
-    </row>
-    <row r="123" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D122" s="10"/>
+    </row>
+    <row r="123" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2"/>
       <c r="B123" s="9"/>
       <c r="C123" s="10"/>
-      <c r="D123" s="15"/>
-    </row>
-    <row r="124" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D123" s="10"/>
+    </row>
+    <row r="124" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2"/>
       <c r="B124" s="9"/>
       <c r="C124" s="10"/>
-      <c r="D124" s="15"/>
-    </row>
-    <row r="125" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D124" s="10"/>
+    </row>
+    <row r="125" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2"/>
       <c r="B125" s="9"/>
       <c r="C125" s="10"/>
-      <c r="D125" s="15"/>
-    </row>
-    <row r="126" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D125" s="10"/>
+    </row>
+    <row r="126" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2"/>
       <c r="B126" s="9"/>
       <c r="C126" s="10"/>
-      <c r="D126" s="15"/>
-    </row>
-    <row r="127" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D126" s="10"/>
+    </row>
+    <row r="127" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2"/>
       <c r="B127" s="9"/>
       <c r="C127" s="10"/>
-      <c r="D127" s="15"/>
-    </row>
-    <row r="128" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D127" s="10"/>
+    </row>
+    <row r="128" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2"/>
       <c r="B128" s="9"/>
       <c r="C128" s="10"/>
-      <c r="D128" s="15"/>
-    </row>
-    <row r="129" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D128" s="10"/>
+    </row>
+    <row r="129" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2"/>
       <c r="B129" s="9"/>
       <c r="C129" s="10"/>
-      <c r="D129" s="15"/>
-    </row>
-    <row r="130" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D129" s="10"/>
+    </row>
+    <row r="130" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2"/>
       <c r="B130" s="9"/>
       <c r="C130" s="10"/>
-      <c r="D130" s="15"/>
-    </row>
-    <row r="131" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D130" s="10"/>
+    </row>
+    <row r="131" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2"/>
       <c r="B131" s="9"/>
       <c r="C131" s="10"/>
-      <c r="D131" s="15"/>
-    </row>
-    <row r="132" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D131" s="10"/>
+    </row>
+    <row r="132" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2"/>
       <c r="B132" s="9"/>
       <c r="C132" s="10"/>
-      <c r="D132" s="15"/>
-    </row>
-    <row r="133" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D132" s="10"/>
+    </row>
+    <row r="133" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2"/>
       <c r="B133" s="9"/>
       <c r="C133" s="10"/>
-      <c r="D133" s="15"/>
-    </row>
-    <row r="134" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D133" s="10"/>
+    </row>
+    <row r="134" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2"/>
       <c r="B134" s="9"/>
       <c r="C134" s="10"/>
-      <c r="D134" s="15"/>
-    </row>
-    <row r="135" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D134" s="10"/>
+    </row>
+    <row r="135" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2"/>
       <c r="B135" s="9"/>
       <c r="C135" s="10"/>
-      <c r="D135" s="15"/>
-    </row>
-    <row r="136" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D135" s="10"/>
+    </row>
+    <row r="136" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2"/>
       <c r="B136" s="9"/>
       <c r="C136" s="10"/>
-      <c r="D136" s="15"/>
-    </row>
-    <row r="137" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D136" s="10"/>
+    </row>
+    <row r="137" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2"/>
       <c r="B137" s="9"/>
       <c r="C137" s="10"/>
-      <c r="D137" s="15"/>
-    </row>
-    <row r="138" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D137" s="10"/>
+    </row>
+    <row r="138" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2"/>
       <c r="B138" s="9"/>
       <c r="C138" s="10"/>
-      <c r="D138" s="15"/>
-    </row>
-    <row r="139" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D138" s="10"/>
+    </row>
+    <row r="139" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2"/>
       <c r="B139" s="9"/>
       <c r="C139" s="10"/>
-      <c r="D139" s="15"/>
-    </row>
-    <row r="140" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D139" s="10"/>
+    </row>
+    <row r="140" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2"/>
       <c r="B140" s="9"/>
       <c r="C140" s="10"/>
-      <c r="D140" s="15"/>
-    </row>
-    <row r="141" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D140" s="10"/>
+    </row>
+    <row r="141" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2"/>
       <c r="B141" s="9"/>
       <c r="C141" s="10"/>
-      <c r="D141" s="15"/>
-    </row>
-    <row r="142" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D141" s="10"/>
+    </row>
+    <row r="142" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2"/>
       <c r="B142" s="9"/>
       <c r="C142" s="10"/>
-      <c r="D142" s="15"/>
-    </row>
-    <row r="143" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D142" s="10"/>
+    </row>
+    <row r="143" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2"/>
       <c r="B143" s="9"/>
       <c r="C143" s="10"/>
-      <c r="D143" s="15"/>
-    </row>
-    <row r="144" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D143" s="10"/>
+    </row>
+    <row r="144" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2"/>
       <c r="B144" s="9"/>
       <c r="C144" s="10"/>
-      <c r="D144" s="15"/>
-    </row>
-    <row r="145" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D144" s="10"/>
+    </row>
+    <row r="145" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2"/>
       <c r="B145" s="9"/>
       <c r="C145" s="10"/>
-      <c r="D145" s="15"/>
-    </row>
-    <row r="146" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D145" s="10"/>
+    </row>
+    <row r="146" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2"/>
       <c r="B146" s="9"/>
       <c r="C146" s="10"/>
-      <c r="D146" s="15"/>
-    </row>
-    <row r="147" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D146" s="10"/>
+    </row>
+    <row r="147" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2"/>
       <c r="B147" s="9"/>
       <c r="C147" s="10"/>
-      <c r="D147" s="15"/>
-    </row>
-    <row r="148" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D147" s="10"/>
+    </row>
+    <row r="148" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2"/>
       <c r="B148" s="9"/>
       <c r="C148" s="10"/>
-      <c r="D148" s="15"/>
-    </row>
-    <row r="149" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D148" s="10"/>
+    </row>
+    <row r="149" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2"/>
       <c r="B149" s="9"/>
       <c r="C149" s="10"/>
-      <c r="D149" s="15"/>
-    </row>
-    <row r="150" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D149" s="10"/>
+    </row>
+    <row r="150" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2"/>
       <c r="B150" s="9"/>
       <c r="C150" s="10"/>
-      <c r="D150" s="15"/>
-    </row>
-    <row r="151" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D150" s="10"/>
+    </row>
+    <row r="151" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2"/>
       <c r="B151" s="9"/>
       <c r="C151" s="10"/>
-      <c r="D151" s="15"/>
-    </row>
-    <row r="152" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D151" s="10"/>
+    </row>
+    <row r="152" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2"/>
       <c r="B152" s="9"/>
       <c r="C152" s="10"/>
-      <c r="D152" s="15"/>
-    </row>
-    <row r="153" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D152" s="10"/>
+    </row>
+    <row r="153" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2"/>
       <c r="B153" s="9"/>
       <c r="C153" s="10"/>
-      <c r="D153" s="15"/>
-    </row>
-    <row r="154" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D153" s="10"/>
+    </row>
+    <row r="154" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="2"/>
       <c r="B154" s="9"/>
       <c r="C154" s="10"/>
-      <c r="D154" s="15"/>
-    </row>
-    <row r="155" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D154" s="10"/>
+    </row>
+    <row r="155" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="2"/>
       <c r="B155" s="9"/>
       <c r="C155" s="10"/>
-      <c r="D155" s="15"/>
-    </row>
-    <row r="156" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D155" s="10"/>
+    </row>
+    <row r="156" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="2"/>
       <c r="B156" s="9"/>
       <c r="C156" s="10"/>
-      <c r="D156" s="15"/>
-    </row>
-    <row r="157" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D156" s="10"/>
+    </row>
+    <row r="157" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="2"/>
       <c r="B157" s="9"/>
       <c r="C157" s="10"/>
-      <c r="D157" s="15"/>
-    </row>
-    <row r="158" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D157" s="10"/>
+    </row>
+    <row r="158" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="2"/>
       <c r="B158" s="9"/>
       <c r="C158" s="10"/>
-      <c r="D158" s="15"/>
-    </row>
-    <row r="159" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D158" s="10"/>
+    </row>
+    <row r="159" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2"/>
       <c r="B159" s="9"/>
       <c r="C159" s="10"/>
-      <c r="D159" s="15"/>
-    </row>
-    <row r="160" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D159" s="10"/>
+    </row>
+    <row r="160" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="2"/>
       <c r="B160" s="9"/>
       <c r="C160" s="10"/>
-      <c r="D160" s="15"/>
-    </row>
-    <row r="161" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D160" s="10"/>
+    </row>
+    <row r="161" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="2"/>
       <c r="B161" s="9"/>
       <c r="C161" s="10"/>
-      <c r="D161" s="15"/>
-    </row>
-    <row r="162" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D161" s="10"/>
+    </row>
+    <row r="162" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="2"/>
       <c r="B162" s="9"/>
       <c r="C162" s="10"/>
-      <c r="D162" s="15"/>
-    </row>
-    <row r="163" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D162" s="10"/>
+    </row>
+    <row r="163" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="2"/>
       <c r="B163" s="9"/>
       <c r="C163" s="10"/>
-      <c r="D163" s="15"/>
-    </row>
-    <row r="164" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D163" s="10"/>
+    </row>
+    <row r="164" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="2"/>
       <c r="B164" s="9"/>
       <c r="C164" s="10"/>
     </row>
-    <row r="165" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="2"/>
       <c r="B165" s="9"/>
       <c r="C165" s="10"/>
     </row>
-    <row r="166" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="2"/>
       <c r="B166" s="9"/>
       <c r="C166" s="10"/>
     </row>
-    <row r="167" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="2"/>
       <c r="B167" s="9"/>
       <c r="C167" s="10"/>
     </row>
-    <row r="168" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="2"/>
       <c r="B168" s="9"/>
       <c r="C168" s="10"/>
     </row>
-    <row r="169" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="2"/>
       <c r="B169" s="9"/>
       <c r="C169" s="10"/>
     </row>
-    <row r="170" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="2"/>
       <c r="B170" s="9"/>
       <c r="C170" s="10"/>
     </row>
-    <row r="171" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="2"/>
       <c r="B171" s="9"/>
       <c r="C171" s="10"/>
     </row>
-    <row r="172" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="2"/>
       <c r="B172" s="9"/>
       <c r="C172" s="10"/>
     </row>
-    <row r="173" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="2"/>
       <c r="B173" s="9"/>
       <c r="C173" s="10"/>
     </row>
-    <row r="174" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="2"/>
       <c r="B174" s="9"/>
       <c r="C174" s="10"/>
     </row>
-    <row r="175" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="2"/>
       <c r="B175" s="9"/>
       <c r="C175" s="10"/>
     </row>
-    <row r="176" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="2"/>
       <c r="B176" s="9"/>
       <c r="C176" s="10"/>
     </row>
-    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="2"/>
       <c r="B177" s="9"/>
       <c r="C177" s="10"/>
     </row>
-    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="2"/>
       <c r="B178" s="9"/>
       <c r="C178" s="10"/>
     </row>
-    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="2"/>
       <c r="B179" s="9"/>
       <c r="C179" s="10"/>
     </row>
-    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="2"/>
       <c r="B180" s="9"/>
       <c r="C180" s="10"/>
     </row>
-    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="2"/>
       <c r="B181" s="9"/>
       <c r="C181" s="10"/>
     </row>
-    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="2"/>
       <c r="B182" s="9"/>
       <c r="C182" s="10"/>
     </row>
-    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="2"/>
       <c r="B183" s="9"/>
       <c r="C183" s="10"/>
     </row>
-    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="2"/>
       <c r="B184" s="9"/>
       <c r="C184" s="10"/>
     </row>
-    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="2"/>
       <c r="B185" s="9"/>
       <c r="C185" s="10"/>
     </row>
-    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="2"/>
       <c r="B186" s="9"/>
       <c r="C186" s="10"/>
     </row>
-    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="2"/>
       <c r="B187" s="9"/>
       <c r="C187" s="10"/>
     </row>
-    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="2"/>
       <c r="B188" s="9"/>
       <c r="C188" s="10"/>
     </row>
-    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="2"/>
       <c r="B189" s="9"/>
       <c r="C189" s="10"/>
     </row>
-    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="2"/>
       <c r="B190" s="9"/>
       <c r="C190" s="10"/>
     </row>
-    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="2"/>
       <c r="B191" s="9"/>
       <c r="C191" s="10"/>
     </row>
-    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="2"/>
       <c r="B192" s="9"/>
       <c r="C192" s="10"/>
     </row>
-    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="2"/>
       <c r="B193" s="9"/>
       <c r="C193" s="10"/>
     </row>
-    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="2"/>
       <c r="B194" s="9"/>
       <c r="C194" s="10"/>
     </row>
-    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="2"/>
       <c r="B195" s="9"/>
       <c r="C195" s="10"/>
     </row>
-    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="2"/>
       <c r="B196" s="9"/>
       <c r="C196" s="10"/>
     </row>
-    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="2"/>
       <c r="B197" s="9"/>
       <c r="C197" s="10"/>
     </row>
-    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="2"/>
       <c r="B198" s="9"/>
       <c r="C198" s="10"/>
     </row>
-    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="2"/>
       <c r="B199" s="9"/>
       <c r="C199" s="10"/>
     </row>
-    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="2"/>
       <c r="B200" s="9"/>
       <c r="C200" s="10"/>
     </row>
-    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="2"/>
       <c r="B201" s="9"/>
       <c r="C201" s="10"/>
     </row>
-    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="2"/>
       <c r="B202" s="9"/>
       <c r="C202" s="10"/>
     </row>
-    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="2"/>
       <c r="B203" s="9"/>
       <c r="C203" s="10"/>
     </row>
-    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="2"/>
       <c r="B204" s="9"/>
       <c r="C204" s="10"/>
     </row>
-    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="2"/>
       <c r="B205" s="9"/>
       <c r="C205" s="10"/>
     </row>
-    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="2"/>
       <c r="B206" s="9"/>
       <c r="C206" s="10"/>
     </row>
-    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="2"/>
       <c r="B207" s="9"/>
       <c r="C207" s="10"/>
     </row>
-    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="2"/>
       <c r="B208" s="9"/>
       <c r="C208" s="10"/>
     </row>
-    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="2"/>
       <c r="B209" s="9"/>
       <c r="C209" s="10"/>
     </row>
-    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="2"/>
       <c r="B210" s="9"/>
       <c r="C210" s="10"/>
     </row>
-    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="2"/>
       <c r="B211" s="9"/>
       <c r="C211" s="10"/>
     </row>
-    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2"/>
       <c r="B212" s="9"/>
       <c r="C212" s="10"/>
     </row>
-    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="2"/>
       <c r="B213" s="9"/>
       <c r="C213" s="10"/>
     </row>
-    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="2"/>
       <c r="B214" s="9"/>
       <c r="C214" s="10"/>
     </row>
-    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="2"/>
       <c r="B215" s="9"/>
       <c r="C215" s="10"/>
     </row>
-    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="2"/>
       <c r="B216" s="9"/>
       <c r="C216" s="10"/>
     </row>
-    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="2"/>
       <c r="B217" s="9"/>
       <c r="C217" s="10"/>
     </row>
-    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="2"/>
       <c r="B218" s="9"/>
       <c r="C218" s="10"/>
     </row>
-    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="2"/>
       <c r="B219" s="9"/>
       <c r="C219" s="10"/>
     </row>
-    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="2"/>
       <c r="B220" s="9"/>
       <c r="C220" s="10"/>
     </row>
-    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="2"/>
       <c r="B221" s="9"/>
       <c r="C221" s="10"/>
     </row>
-    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="2"/>
       <c r="B222" s="9"/>
       <c r="C222" s="10"/>
     </row>
-    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="2"/>
       <c r="B223" s="9"/>
       <c r="C223" s="10"/>
     </row>
-    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="2"/>
       <c r="B224" s="9"/>
       <c r="C224" s="10"/>
     </row>
-    <row r="225" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="2"/>
       <c r="B225" s="9"/>
       <c r="C225" s="10"/>
     </row>
-    <row r="226" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="2"/>
       <c r="B226" s="9"/>
       <c r="C226" s="10"/>
     </row>
-    <row r="227" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="2"/>
       <c r="B227" s="9"/>
       <c r="C227" s="10"/>
     </row>
-    <row r="228" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="2"/>
       <c r="B228" s="9"/>
       <c r="C228" s="10"/>
     </row>
-    <row r="229" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="2"/>
       <c r="B229" s="9"/>
       <c r="C229" s="10"/>
     </row>
-    <row r="230" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="2"/>
       <c r="B230" s="9"/>
       <c r="C230" s="10"/>
     </row>
-    <row r="231" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="2"/>
       <c r="B231" s="9"/>
       <c r="C231" s="10"/>
     </row>
-    <row r="232" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="2"/>
       <c r="B232" s="9"/>
       <c r="C232" s="10"/>
     </row>
-    <row r="233" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="2"/>
       <c r="B233" s="9"/>
       <c r="C233" s="10"/>
     </row>
-    <row r="234" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="2"/>
       <c r="B234" s="9"/>
       <c r="C234" s="10"/>
     </row>
-    <row r="235" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="2"/>
       <c r="B235" s="9"/>
       <c r="C235" s="10"/>
     </row>
-    <row r="236" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="2"/>
       <c r="B236" s="9"/>
       <c r="C236" s="10"/>
     </row>
-    <row r="237" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="2"/>
       <c r="B237" s="9"/>
       <c r="C237" s="10"/>
     </row>
-    <row r="238" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="2"/>
       <c r="B238" s="9"/>
       <c r="C238" s="10"/>
     </row>
-    <row r="239" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="2"/>
       <c r="B239" s="9"/>
       <c r="C239" s="10"/>
     </row>
-    <row r="240" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="2"/>
       <c r="B240" s="9"/>
       <c r="C240" s="10"/>
     </row>
-    <row r="241" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="2"/>
       <c r="B241" s="9"/>
       <c r="C241" s="10"/>
     </row>
-    <row r="242" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="2"/>
       <c r="B242" s="9"/>
       <c r="C242" s="10"/>
     </row>
-    <row r="243" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="2"/>
       <c r="B243" s="9"/>
       <c r="C243" s="10"/>
     </row>
-    <row r="244" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="2"/>
       <c r="B244" s="9"/>
       <c r="C244" s="10"/>
     </row>
-    <row r="245" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="2"/>
       <c r="B245" s="9"/>
       <c r="C245" s="10"/>
     </row>
-    <row r="246" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="2"/>
       <c r="B246" s="9"/>
       <c r="C246" s="10"/>
     </row>
-    <row r="247" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="2"/>
       <c r="B247" s="9"/>
       <c r="C247" s="10"/>
     </row>
-    <row r="248" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="2"/>
       <c r="B248" s="9"/>
       <c r="C248" s="10"/>
     </row>
-    <row r="249" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="2"/>
       <c r="B249" s="9"/>
       <c r="C249" s="10"/>

</xml_diff>

<commit_message>
updating RTM adding register & login development IDs
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI9M-Testing\Core\QA\WorkShop\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048AEA25-6BB5-4420-912F-776DE1F1457A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8DACC2-DF29-4975-80F0-E76B3FA8951A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="174">
   <si>
     <t>SRS ID</t>
   </si>
@@ -585,6 +585,15 @@
   </si>
   <si>
     <t>UI_Login_006.png                            CD_Login.png                                     SD_Login_002.png                            FD_Login_001.png                                   FD_Login_002.png</t>
+  </si>
+  <si>
+    <t>Development ID</t>
+  </si>
+  <si>
+    <t>signup.html                                               signup.js</t>
+  </si>
+  <si>
+    <t>index.html                                                           index.js</t>
   </si>
 </sst>
 </file>
@@ -973,10 +982,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D249"/>
+  <dimension ref="A1:E249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -985,9 +994,10 @@
     <col min="2" max="2" width="37.44140625" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" style="14" customWidth="1"/>
     <col min="4" max="4" width="38.44140625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="37.6640625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1000,8 +1010,11 @@
       <c r="D1" s="13" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="59.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E1" s="13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="59.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1014,8 +1027,11 @@
       <c r="D2" s="10" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="99" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E2" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1028,8 +1044,11 @@
       <c r="D3" s="10" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E3" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -1042,8 +1061,11 @@
       <c r="D4" s="10" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="73.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E4" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="73.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1056,8 +1078,11 @@
       <c r="D5" s="10" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E5" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1070,8 +1095,11 @@
       <c r="D6" s="10" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E6" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="82.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1084,8 +1112,11 @@
       <c r="D7" s="10" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E7" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1098,8 +1129,11 @@
       <c r="D8" s="10" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E8" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1112,8 +1146,11 @@
       <c r="D9" s="10" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E9" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -1126,8 +1163,11 @@
       <c r="D10" s="10" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="109.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E10" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="109.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -1140,8 +1180,11 @@
       <c r="D11" s="10" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="90.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E11" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="90.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -1154,8 +1197,11 @@
       <c r="D12" s="10" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="81" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E12" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1168,8 +1214,11 @@
       <c r="D13" s="10" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E13" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="61.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1182,8 +1231,11 @@
       <c r="D14" s="10" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E14" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
@@ -1196,8 +1248,11 @@
       <c r="D15" s="10" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E15" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
@@ -1210,8 +1265,11 @@
       <c r="D16" s="10" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="55.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E16" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="55.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
@@ -1224,8 +1282,11 @@
       <c r="D17" s="10" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E17" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
@@ -1238,8 +1299,11 @@
       <c r="D18" s="10" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="88.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E18" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="88.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
@@ -1252,8 +1316,11 @@
       <c r="D19" s="10" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="55.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E19" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="55.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>2</v>
       </c>
@@ -1266,8 +1333,11 @@
       <c r="D20" s="10" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="88.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E20" s="14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="88.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>3</v>
       </c>
@@ -1280,8 +1350,11 @@
       <c r="D21" s="10" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="102" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E21" s="14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>4</v>
       </c>
@@ -1294,8 +1367,11 @@
       <c r="D22" s="10" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E22" s="14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>5</v>
       </c>
@@ -1308,8 +1384,11 @@
       <c r="D23" s="10" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E23" s="14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
@@ -1322,8 +1401,11 @@
       <c r="D24" s="10" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E24" s="14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>98</v>
       </c>
@@ -1336,8 +1418,11 @@
       <c r="D25" s="10" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="64.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E25" s="14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="64.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>34</v>
       </c>
@@ -1351,7 +1436,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>35</v>
       </c>
@@ -1365,7 +1450,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>36</v>
       </c>
@@ -1379,7 +1464,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>37</v>
       </c>
@@ -1393,7 +1478,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
@@ -1407,7 +1492,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>39</v>
       </c>
@@ -1421,7 +1506,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
DOc: Updated Traceability for checkout and client home
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\RTM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI material\QA\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC2A154-A8AE-416E-B6DF-9547A66B15A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F0E9CF-3EF4-4394-89E2-F5FC0CD69298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="184">
   <si>
     <t>SRS ID</t>
   </si>
@@ -635,6 +635,26 @@
   </si>
   <si>
     <t>client_home.html                                                           client_home.js</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI_Client_Home_Page_001.jpeg
+CD__Client_Home_Page.jpeg
+FD_Client_Home_Page.jpeg
+SD_Client_Home_Page001.png
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD_Checkout.jpeg
+FD_Checkout.jpeg
+SD_Checkout.png
+UI_Checkout.jpeg
+</t>
+  </si>
+  <si>
+    <t>CD_Checkout.jpeg
+FD_Checkout.jpeg
+SD_Checkout.png
+UI_Checkout.jpeg</t>
   </si>
 </sst>
 </file>
@@ -680,7 +700,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -691,6 +711,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF4A86E8"/>
         <bgColor rgb="FF4A86E8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -808,10 +834,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1035,20 +1061,20 @@
   <dimension ref="A1:E249"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="37.7109375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="37.44140625" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="38.44140625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="37.6640625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1065,7 +1091,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="59.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="59.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1082,7 +1108,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1099,7 +1125,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -1116,7 +1142,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="73.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1133,7 +1159,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1150,7 +1176,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="82.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="82.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1167,7 +1193,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1184,7 +1210,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1201,7 +1227,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -1218,7 +1244,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="109.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="109.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -1235,7 +1261,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="90.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -1252,7 +1278,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1269,7 +1295,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="61.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="61.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1286,7 +1312,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
@@ -1303,7 +1329,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
@@ -1320,7 +1346,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="55.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="55.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
@@ -1337,7 +1363,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
@@ -1354,7 +1380,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="88.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="88.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
@@ -1371,7 +1397,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="55.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="55.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>2</v>
       </c>
@@ -1384,11 +1410,11 @@
       <c r="D20" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="10" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="88.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="88.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>3</v>
       </c>
@@ -1401,11 +1427,11 @@
       <c r="D21" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="10" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>4</v>
       </c>
@@ -1422,7 +1448,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>5</v>
       </c>
@@ -1439,7 +1465,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
@@ -1456,7 +1482,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>97</v>
       </c>
@@ -1473,14 +1499,14 @@
         <v>171</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="16" t="s">
         <v>85</v>
       </c>
       <c r="D26" s="15" t="s">
@@ -1490,160 +1516,160 @@
         <v>174</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="16" t="s">
         <v>172</v>
       </c>
       <c r="D27" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="10" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="16" t="s">
         <v>173</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="10" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="16" t="s">
         <v>86</v>
       </c>
       <c r="D29" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="E29" s="10" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="16" t="s">
         <v>87</v>
       </c>
       <c r="D30" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="10" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="16" t="s">
         <v>87</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E31" s="10" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="16" t="s">
         <v>88</v>
       </c>
       <c r="D32" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="E32" s="10" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="16" t="s">
         <v>89</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="10" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>137</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="16" t="s">
         <v>90</v>
       </c>
       <c r="D34" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="E34" s="16" t="s">
+      <c r="E34" s="10" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>138</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="16" t="s">
         <v>172</v>
       </c>
       <c r="D35" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="E35" s="16" t="s">
+      <c r="E35" s="10" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>44</v>
       </c>
@@ -1655,7 +1681,7 @@
       </c>
       <c r="D36" s="15"/>
     </row>
-    <row r="37" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>45</v>
       </c>
@@ -1667,7 +1693,7 @@
       </c>
       <c r="D37" s="15"/>
     </row>
-    <row r="38" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>46</v>
       </c>
@@ -1679,7 +1705,7 @@
       </c>
       <c r="D38" s="15"/>
     </row>
-    <row r="39" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>47</v>
       </c>
@@ -1691,7 +1717,7 @@
       </c>
       <c r="D39" s="15"/>
     </row>
-    <row r="40" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>48</v>
       </c>
@@ -1703,7 +1729,7 @@
       </c>
       <c r="D40" s="15"/>
     </row>
-    <row r="41" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>49</v>
       </c>
@@ -1715,7 +1741,7 @@
       </c>
       <c r="D41" s="15"/>
     </row>
-    <row r="42" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>50</v>
       </c>
@@ -1727,7 +1753,7 @@
       </c>
       <c r="D42" s="15"/>
     </row>
-    <row r="43" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>51</v>
       </c>
@@ -1739,7 +1765,7 @@
       </c>
       <c r="D43" s="15"/>
     </row>
-    <row r="44" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="67.2" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>52</v>
       </c>
@@ -1750,8 +1776,11 @@
         <v>118</v>
       </c>
       <c r="D44" s="15"/>
-    </row>
-    <row r="45" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E44" s="17" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>101</v>
       </c>
@@ -1763,7 +1792,7 @@
       </c>
       <c r="D45" s="15"/>
     </row>
-    <row r="46" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>53</v>
       </c>
@@ -1775,7 +1804,7 @@
       </c>
       <c r="D46" s="15"/>
     </row>
-    <row r="47" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>54</v>
       </c>
@@ -1787,7 +1816,7 @@
       </c>
       <c r="D47" s="15"/>
     </row>
-    <row r="48" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>55</v>
       </c>
@@ -1799,7 +1828,7 @@
       </c>
       <c r="D48" s="15"/>
     </row>
-    <row r="49" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>56</v>
       </c>
@@ -1811,7 +1840,7 @@
       </c>
       <c r="D49" s="15"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>57</v>
       </c>
@@ -1823,7 +1852,7 @@
       </c>
       <c r="D50" s="15"/>
     </row>
-    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>102</v>
       </c>
@@ -1835,7 +1864,7 @@
       </c>
       <c r="D51" s="15"/>
     </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>103</v>
       </c>
@@ -1847,7 +1876,7 @@
       </c>
       <c r="D52" s="15"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>104</v>
       </c>
@@ -1858,8 +1887,11 @@
         <v>82</v>
       </c>
       <c r="D53" s="15"/>
-    </row>
-    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E53" s="17" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>105</v>
       </c>
@@ -1870,8 +1902,11 @@
         <v>82</v>
       </c>
       <c r="D54" s="15"/>
-    </row>
-    <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E54" s="17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>106</v>
       </c>
@@ -1882,1081 +1917,1084 @@
         <v>82</v>
       </c>
       <c r="D55" s="15"/>
-    </row>
-    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E55" s="17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="10"/>
       <c r="D56" s="15"/>
     </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="10"/>
       <c r="D57" s="15"/>
     </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="10"/>
       <c r="D58" s="15"/>
     </row>
-    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="9"/>
       <c r="C59" s="10"/>
       <c r="D59" s="15"/>
     </row>
-    <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="9"/>
       <c r="C60" s="10"/>
       <c r="D60" s="15"/>
     </row>
-    <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="9"/>
       <c r="C61" s="10"/>
       <c r="D61" s="15"/>
     </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="9"/>
       <c r="C62" s="10"/>
       <c r="D62" s="15"/>
     </row>
-    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="9"/>
       <c r="C63" s="10"/>
       <c r="D63" s="15"/>
     </row>
-    <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="9"/>
       <c r="C64" s="10"/>
       <c r="D64" s="15"/>
     </row>
-    <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="9"/>
       <c r="C65" s="10"/>
       <c r="D65" s="15"/>
     </row>
-    <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="9"/>
       <c r="C66" s="10"/>
       <c r="D66" s="15"/>
     </row>
-    <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" s="9"/>
       <c r="C67" s="10"/>
       <c r="D67" s="15"/>
     </row>
-    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" s="9"/>
       <c r="C68" s="10"/>
       <c r="D68" s="15"/>
     </row>
-    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="9"/>
       <c r="C69" s="10"/>
       <c r="D69" s="15"/>
     </row>
-    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" s="9"/>
       <c r="C70" s="10"/>
       <c r="D70" s="15"/>
     </row>
-    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="9"/>
       <c r="C71" s="10"/>
       <c r="D71" s="15"/>
     </row>
-    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="9"/>
       <c r="C72" s="10"/>
       <c r="D72" s="15"/>
     </row>
-    <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="9"/>
       <c r="C73" s="10"/>
       <c r="D73" s="15"/>
     </row>
-    <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="9"/>
       <c r="C74" s="10"/>
       <c r="D74" s="15"/>
     </row>
-    <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="9"/>
       <c r="C75" s="10"/>
       <c r="D75" s="15"/>
     </row>
-    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="9"/>
       <c r="C76" s="10"/>
       <c r="D76" s="15"/>
     </row>
-    <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" s="9"/>
       <c r="C77" s="10"/>
       <c r="D77" s="15"/>
     </row>
-    <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" s="9"/>
       <c r="C78" s="10"/>
       <c r="D78" s="15"/>
     </row>
-    <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" s="9"/>
       <c r="C79" s="10"/>
       <c r="D79" s="15"/>
     </row>
-    <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" s="9"/>
       <c r="C80" s="10"/>
       <c r="D80" s="15"/>
     </row>
-    <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="B81" s="9"/>
       <c r="C81" s="10"/>
       <c r="D81" s="15"/>
     </row>
-    <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
       <c r="B82" s="9"/>
       <c r="C82" s="10"/>
       <c r="D82" s="15"/>
     </row>
-    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2"/>
       <c r="B83" s="9"/>
       <c r="C83" s="10"/>
       <c r="D83" s="15"/>
     </row>
-    <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
       <c r="B84" s="9"/>
       <c r="C84" s="10"/>
       <c r="D84" s="15"/>
     </row>
-    <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2"/>
       <c r="B85" s="9"/>
       <c r="C85" s="10"/>
       <c r="D85" s="15"/>
     </row>
-    <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" s="9"/>
       <c r="C86" s="10"/>
       <c r="D86" s="15"/>
     </row>
-    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
       <c r="B87" s="9"/>
       <c r="C87" s="10"/>
       <c r="D87" s="15"/>
     </row>
-    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
       <c r="B88" s="9"/>
       <c r="C88" s="10"/>
       <c r="D88" s="15"/>
     </row>
-    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" s="9"/>
       <c r="C89" s="10"/>
       <c r="D89" s="15"/>
     </row>
-    <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
       <c r="B90" s="9"/>
       <c r="C90" s="10"/>
       <c r="D90" s="15"/>
     </row>
-    <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
       <c r="B91" s="9"/>
       <c r="C91" s="10"/>
       <c r="D91" s="15"/>
     </row>
-    <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
       <c r="B92" s="9"/>
       <c r="C92" s="10"/>
       <c r="D92" s="15"/>
     </row>
-    <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
       <c r="B93" s="9"/>
       <c r="C93" s="10"/>
       <c r="D93" s="15"/>
     </row>
-    <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
       <c r="B94" s="9"/>
       <c r="C94" s="10"/>
       <c r="D94" s="15"/>
     </row>
-    <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2"/>
       <c r="B95" s="9"/>
       <c r="C95" s="10"/>
       <c r="D95" s="15"/>
     </row>
-    <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
       <c r="B96" s="9"/>
       <c r="C96" s="10"/>
       <c r="D96" s="15"/>
     </row>
-    <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
       <c r="B97" s="9"/>
       <c r="C97" s="10"/>
       <c r="D97" s="15"/>
     </row>
-    <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
       <c r="B98" s="9"/>
       <c r="C98" s="10"/>
       <c r="D98" s="15"/>
     </row>
-    <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
       <c r="B99" s="9"/>
       <c r="C99" s="10"/>
       <c r="D99" s="15"/>
     </row>
-    <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
       <c r="B100" s="9"/>
       <c r="C100" s="10"/>
       <c r="D100" s="15"/>
     </row>
-    <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
       <c r="B101" s="9"/>
       <c r="C101" s="10"/>
       <c r="D101" s="15"/>
     </row>
-    <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
       <c r="B102" s="9"/>
       <c r="C102" s="10"/>
       <c r="D102" s="15"/>
     </row>
-    <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
       <c r="B103" s="9"/>
       <c r="C103" s="10"/>
       <c r="D103" s="15"/>
     </row>
-    <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="B104" s="9"/>
       <c r="C104" s="10"/>
       <c r="D104" s="15"/>
     </row>
-    <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
       <c r="B105" s="9"/>
       <c r="C105" s="10"/>
       <c r="D105" s="15"/>
     </row>
-    <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="B106" s="9"/>
       <c r="C106" s="10"/>
       <c r="D106" s="15"/>
     </row>
-    <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" s="9"/>
       <c r="C107" s="10"/>
       <c r="D107" s="15"/>
     </row>
-    <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
       <c r="B108" s="9"/>
       <c r="C108" s="10"/>
       <c r="D108" s="15"/>
     </row>
-    <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2"/>
       <c r="B109" s="9"/>
       <c r="C109" s="10"/>
       <c r="D109" s="15"/>
     </row>
-    <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="B110" s="9"/>
       <c r="C110" s="10"/>
       <c r="D110" s="15"/>
     </row>
-    <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2"/>
       <c r="B111" s="9"/>
       <c r="C111" s="10"/>
       <c r="D111" s="15"/>
     </row>
-    <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
       <c r="B112" s="9"/>
       <c r="C112" s="10"/>
       <c r="D112" s="15"/>
     </row>
-    <row r="113" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
       <c r="B113" s="9"/>
       <c r="C113" s="10"/>
       <c r="D113" s="15"/>
     </row>
-    <row r="114" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="B114" s="9"/>
       <c r="C114" s="10"/>
       <c r="D114" s="15"/>
     </row>
-    <row r="115" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2"/>
       <c r="B115" s="9"/>
       <c r="C115" s="10"/>
       <c r="D115" s="15"/>
     </row>
-    <row r="116" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2"/>
       <c r="B116" s="9"/>
       <c r="C116" s="10"/>
       <c r="D116" s="15"/>
     </row>
-    <row r="117" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2"/>
       <c r="B117" s="9"/>
       <c r="C117" s="10"/>
       <c r="D117" s="15"/>
     </row>
-    <row r="118" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2"/>
       <c r="B118" s="9"/>
       <c r="C118" s="10"/>
       <c r="D118" s="15"/>
     </row>
-    <row r="119" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2"/>
       <c r="B119" s="9"/>
       <c r="C119" s="10"/>
       <c r="D119" s="15"/>
     </row>
-    <row r="120" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2"/>
       <c r="B120" s="9"/>
       <c r="C120" s="10"/>
       <c r="D120" s="15"/>
     </row>
-    <row r="121" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2"/>
       <c r="B121" s="9"/>
       <c r="C121" s="10"/>
       <c r="D121" s="15"/>
     </row>
-    <row r="122" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2"/>
       <c r="B122" s="9"/>
       <c r="C122" s="10"/>
       <c r="D122" s="15"/>
     </row>
-    <row r="123" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2"/>
       <c r="B123" s="9"/>
       <c r="C123" s="10"/>
       <c r="D123" s="15"/>
     </row>
-    <row r="124" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2"/>
       <c r="B124" s="9"/>
       <c r="C124" s="10"/>
       <c r="D124" s="15"/>
     </row>
-    <row r="125" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2"/>
       <c r="B125" s="9"/>
       <c r="C125" s="10"/>
       <c r="D125" s="15"/>
     </row>
-    <row r="126" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2"/>
       <c r="B126" s="9"/>
       <c r="C126" s="10"/>
       <c r="D126" s="15"/>
     </row>
-    <row r="127" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2"/>
       <c r="B127" s="9"/>
       <c r="C127" s="10"/>
       <c r="D127" s="15"/>
     </row>
-    <row r="128" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2"/>
       <c r="B128" s="9"/>
       <c r="C128" s="10"/>
       <c r="D128" s="15"/>
     </row>
-    <row r="129" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2"/>
       <c r="B129" s="9"/>
       <c r="C129" s="10"/>
       <c r="D129" s="15"/>
     </row>
-    <row r="130" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2"/>
       <c r="B130" s="9"/>
       <c r="C130" s="10"/>
       <c r="D130" s="15"/>
     </row>
-    <row r="131" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2"/>
       <c r="B131" s="9"/>
       <c r="C131" s="10"/>
       <c r="D131" s="15"/>
     </row>
-    <row r="132" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2"/>
       <c r="B132" s="9"/>
       <c r="C132" s="10"/>
       <c r="D132" s="15"/>
     </row>
-    <row r="133" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2"/>
       <c r="B133" s="9"/>
       <c r="C133" s="10"/>
       <c r="D133" s="15"/>
     </row>
-    <row r="134" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2"/>
       <c r="B134" s="9"/>
       <c r="C134" s="10"/>
       <c r="D134" s="15"/>
     </row>
-    <row r="135" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2"/>
       <c r="B135" s="9"/>
       <c r="C135" s="10"/>
       <c r="D135" s="15"/>
     </row>
-    <row r="136" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2"/>
       <c r="B136" s="9"/>
       <c r="C136" s="10"/>
       <c r="D136" s="15"/>
     </row>
-    <row r="137" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2"/>
       <c r="B137" s="9"/>
       <c r="C137" s="10"/>
       <c r="D137" s="15"/>
     </row>
-    <row r="138" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2"/>
       <c r="B138" s="9"/>
       <c r="C138" s="10"/>
       <c r="D138" s="15"/>
     </row>
-    <row r="139" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2"/>
       <c r="B139" s="9"/>
       <c r="C139" s="10"/>
       <c r="D139" s="15"/>
     </row>
-    <row r="140" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2"/>
       <c r="B140" s="9"/>
       <c r="C140" s="10"/>
       <c r="D140" s="15"/>
     </row>
-    <row r="141" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2"/>
       <c r="B141" s="9"/>
       <c r="C141" s="10"/>
       <c r="D141" s="15"/>
     </row>
-    <row r="142" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2"/>
       <c r="B142" s="9"/>
       <c r="C142" s="10"/>
       <c r="D142" s="15"/>
     </row>
-    <row r="143" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2"/>
       <c r="B143" s="9"/>
       <c r="C143" s="10"/>
       <c r="D143" s="15"/>
     </row>
-    <row r="144" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2"/>
       <c r="B144" s="9"/>
       <c r="C144" s="10"/>
       <c r="D144" s="15"/>
     </row>
-    <row r="145" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2"/>
       <c r="B145" s="9"/>
       <c r="C145" s="10"/>
       <c r="D145" s="15"/>
     </row>
-    <row r="146" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2"/>
       <c r="B146" s="9"/>
       <c r="C146" s="10"/>
       <c r="D146" s="15"/>
     </row>
-    <row r="147" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2"/>
       <c r="B147" s="9"/>
       <c r="C147" s="10"/>
       <c r="D147" s="15"/>
     </row>
-    <row r="148" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2"/>
       <c r="B148" s="9"/>
       <c r="C148" s="10"/>
       <c r="D148" s="15"/>
     </row>
-    <row r="149" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2"/>
       <c r="B149" s="9"/>
       <c r="C149" s="10"/>
       <c r="D149" s="15"/>
     </row>
-    <row r="150" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2"/>
       <c r="B150" s="9"/>
       <c r="C150" s="10"/>
       <c r="D150" s="15"/>
     </row>
-    <row r="151" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2"/>
       <c r="B151" s="9"/>
       <c r="C151" s="10"/>
       <c r="D151" s="15"/>
     </row>
-    <row r="152" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2"/>
       <c r="B152" s="9"/>
       <c r="C152" s="10"/>
       <c r="D152" s="15"/>
     </row>
-    <row r="153" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2"/>
       <c r="B153" s="9"/>
       <c r="C153" s="10"/>
       <c r="D153" s="15"/>
     </row>
-    <row r="154" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="2"/>
       <c r="B154" s="9"/>
       <c r="C154" s="10"/>
       <c r="D154" s="15"/>
     </row>
-    <row r="155" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="2"/>
       <c r="B155" s="9"/>
       <c r="C155" s="10"/>
       <c r="D155" s="15"/>
     </row>
-    <row r="156" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="2"/>
       <c r="B156" s="9"/>
       <c r="C156" s="10"/>
       <c r="D156" s="15"/>
     </row>
-    <row r="157" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="2"/>
       <c r="B157" s="9"/>
       <c r="C157" s="10"/>
       <c r="D157" s="15"/>
     </row>
-    <row r="158" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="2"/>
       <c r="B158" s="9"/>
       <c r="C158" s="10"/>
       <c r="D158" s="15"/>
     </row>
-    <row r="159" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2"/>
       <c r="B159" s="9"/>
       <c r="C159" s="10"/>
       <c r="D159" s="15"/>
     </row>
-    <row r="160" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="2"/>
       <c r="B160" s="9"/>
       <c r="C160" s="10"/>
       <c r="D160" s="15"/>
     </row>
-    <row r="161" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="2"/>
       <c r="B161" s="9"/>
       <c r="C161" s="10"/>
       <c r="D161" s="15"/>
     </row>
-    <row r="162" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="2"/>
       <c r="B162" s="9"/>
       <c r="C162" s="10"/>
       <c r="D162" s="15"/>
     </row>
-    <row r="163" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="2"/>
       <c r="B163" s="9"/>
       <c r="C163" s="10"/>
       <c r="D163" s="15"/>
     </row>
-    <row r="164" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="2"/>
       <c r="B164" s="9"/>
       <c r="C164" s="10"/>
     </row>
-    <row r="165" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="2"/>
       <c r="B165" s="9"/>
       <c r="C165" s="10"/>
     </row>
-    <row r="166" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="2"/>
       <c r="B166" s="9"/>
       <c r="C166" s="10"/>
     </row>
-    <row r="167" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="2"/>
       <c r="B167" s="9"/>
       <c r="C167" s="10"/>
     </row>
-    <row r="168" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="2"/>
       <c r="B168" s="9"/>
       <c r="C168" s="10"/>
     </row>
-    <row r="169" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="2"/>
       <c r="B169" s="9"/>
       <c r="C169" s="10"/>
     </row>
-    <row r="170" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="2"/>
       <c r="B170" s="9"/>
       <c r="C170" s="10"/>
     </row>
-    <row r="171" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="2"/>
       <c r="B171" s="9"/>
       <c r="C171" s="10"/>
     </row>
-    <row r="172" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="2"/>
       <c r="B172" s="9"/>
       <c r="C172" s="10"/>
     </row>
-    <row r="173" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="2"/>
       <c r="B173" s="9"/>
       <c r="C173" s="10"/>
     </row>
-    <row r="174" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="2"/>
       <c r="B174" s="9"/>
       <c r="C174" s="10"/>
     </row>
-    <row r="175" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="2"/>
       <c r="B175" s="9"/>
       <c r="C175" s="10"/>
     </row>
-    <row r="176" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="2"/>
       <c r="B176" s="9"/>
       <c r="C176" s="10"/>
     </row>
-    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="2"/>
       <c r="B177" s="9"/>
       <c r="C177" s="10"/>
     </row>
-    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="2"/>
       <c r="B178" s="9"/>
       <c r="C178" s="10"/>
     </row>
-    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="2"/>
       <c r="B179" s="9"/>
       <c r="C179" s="10"/>
     </row>
-    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="2"/>
       <c r="B180" s="9"/>
       <c r="C180" s="10"/>
     </row>
-    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="2"/>
       <c r="B181" s="9"/>
       <c r="C181" s="10"/>
     </row>
-    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="2"/>
       <c r="B182" s="9"/>
       <c r="C182" s="10"/>
     </row>
-    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="2"/>
       <c r="B183" s="9"/>
       <c r="C183" s="10"/>
     </row>
-    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="2"/>
       <c r="B184" s="9"/>
       <c r="C184" s="10"/>
     </row>
-    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="2"/>
       <c r="B185" s="9"/>
       <c r="C185" s="10"/>
     </row>
-    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="2"/>
       <c r="B186" s="9"/>
       <c r="C186" s="10"/>
     </row>
-    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="2"/>
       <c r="B187" s="9"/>
       <c r="C187" s="10"/>
     </row>
-    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="2"/>
       <c r="B188" s="9"/>
       <c r="C188" s="10"/>
     </row>
-    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="2"/>
       <c r="B189" s="9"/>
       <c r="C189" s="10"/>
     </row>
-    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="2"/>
       <c r="B190" s="9"/>
       <c r="C190" s="10"/>
     </row>
-    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="2"/>
       <c r="B191" s="9"/>
       <c r="C191" s="10"/>
     </row>
-    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="2"/>
       <c r="B192" s="9"/>
       <c r="C192" s="10"/>
     </row>
-    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="2"/>
       <c r="B193" s="9"/>
       <c r="C193" s="10"/>
     </row>
-    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="2"/>
       <c r="B194" s="9"/>
       <c r="C194" s="10"/>
     </row>
-    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="2"/>
       <c r="B195" s="9"/>
       <c r="C195" s="10"/>
     </row>
-    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="2"/>
       <c r="B196" s="9"/>
       <c r="C196" s="10"/>
     </row>
-    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="2"/>
       <c r="B197" s="9"/>
       <c r="C197" s="10"/>
     </row>
-    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="2"/>
       <c r="B198" s="9"/>
       <c r="C198" s="10"/>
     </row>
-    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="2"/>
       <c r="B199" s="9"/>
       <c r="C199" s="10"/>
     </row>
-    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="2"/>
       <c r="B200" s="9"/>
       <c r="C200" s="10"/>
     </row>
-    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="2"/>
       <c r="B201" s="9"/>
       <c r="C201" s="10"/>
     </row>
-    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="2"/>
       <c r="B202" s="9"/>
       <c r="C202" s="10"/>
     </row>
-    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="2"/>
       <c r="B203" s="9"/>
       <c r="C203" s="10"/>
     </row>
-    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="2"/>
       <c r="B204" s="9"/>
       <c r="C204" s="10"/>
     </row>
-    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="2"/>
       <c r="B205" s="9"/>
       <c r="C205" s="10"/>
     </row>
-    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="2"/>
       <c r="B206" s="9"/>
       <c r="C206" s="10"/>
     </row>
-    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="2"/>
       <c r="B207" s="9"/>
       <c r="C207" s="10"/>
     </row>
-    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="2"/>
       <c r="B208" s="9"/>
       <c r="C208" s="10"/>
     </row>
-    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="2"/>
       <c r="B209" s="9"/>
       <c r="C209" s="10"/>
     </row>
-    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="2"/>
       <c r="B210" s="9"/>
       <c r="C210" s="10"/>
     </row>
-    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="2"/>
       <c r="B211" s="9"/>
       <c r="C211" s="10"/>
     </row>
-    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2"/>
       <c r="B212" s="9"/>
       <c r="C212" s="10"/>
     </row>
-    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="2"/>
       <c r="B213" s="9"/>
       <c r="C213" s="10"/>
     </row>
-    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="2"/>
       <c r="B214" s="9"/>
       <c r="C214" s="10"/>
     </row>
-    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="2"/>
       <c r="B215" s="9"/>
       <c r="C215" s="10"/>
     </row>
-    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="2"/>
       <c r="B216" s="9"/>
       <c r="C216" s="10"/>
     </row>
-    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="2"/>
       <c r="B217" s="9"/>
       <c r="C217" s="10"/>
     </row>
-    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="2"/>
       <c r="B218" s="9"/>
       <c r="C218" s="10"/>
     </row>
-    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="2"/>
       <c r="B219" s="9"/>
       <c r="C219" s="10"/>
     </row>
-    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="2"/>
       <c r="B220" s="9"/>
       <c r="C220" s="10"/>
     </row>
-    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="2"/>
       <c r="B221" s="9"/>
       <c r="C221" s="10"/>
     </row>
-    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="2"/>
       <c r="B222" s="9"/>
       <c r="C222" s="10"/>
     </row>
-    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="2"/>
       <c r="B223" s="9"/>
       <c r="C223" s="10"/>
     </row>
-    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="2"/>
       <c r="B224" s="9"/>
       <c r="C224" s="10"/>
     </row>
-    <row r="225" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="2"/>
       <c r="B225" s="9"/>
       <c r="C225" s="10"/>
     </row>
-    <row r="226" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="2"/>
       <c r="B226" s="9"/>
       <c r="C226" s="10"/>
     </row>
-    <row r="227" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="2"/>
       <c r="B227" s="9"/>
       <c r="C227" s="10"/>
     </row>
-    <row r="228" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="2"/>
       <c r="B228" s="9"/>
       <c r="C228" s="10"/>
     </row>
-    <row r="229" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="2"/>
       <c r="B229" s="9"/>
       <c r="C229" s="10"/>
     </row>
-    <row r="230" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="2"/>
       <c r="B230" s="9"/>
       <c r="C230" s="10"/>
     </row>
-    <row r="231" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="2"/>
       <c r="B231" s="9"/>
       <c r="C231" s="10"/>
     </row>
-    <row r="232" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="2"/>
       <c r="B232" s="9"/>
       <c r="C232" s="10"/>
     </row>
-    <row r="233" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="2"/>
       <c r="B233" s="9"/>
       <c r="C233" s="10"/>
     </row>
-    <row r="234" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="2"/>
       <c r="B234" s="9"/>
       <c r="C234" s="10"/>
     </row>
-    <row r="235" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="2"/>
       <c r="B235" s="9"/>
       <c r="C235" s="10"/>
     </row>
-    <row r="236" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="2"/>
       <c r="B236" s="9"/>
       <c r="C236" s="10"/>
     </row>
-    <row r="237" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="2"/>
       <c r="B237" s="9"/>
       <c r="C237" s="10"/>
     </row>
-    <row r="238" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="2"/>
       <c r="B238" s="9"/>
       <c r="C238" s="10"/>
     </row>
-    <row r="239" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="2"/>
       <c r="B239" s="9"/>
       <c r="C239" s="10"/>
     </row>
-    <row r="240" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="2"/>
       <c r="B240" s="9"/>
       <c r="C240" s="10"/>
     </row>
-    <row r="241" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="2"/>
       <c r="B241" s="9"/>
       <c r="C241" s="10"/>
     </row>
-    <row r="242" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="2"/>
       <c r="B242" s="9"/>
       <c r="C242" s="10"/>
     </row>
-    <row r="243" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="2"/>
       <c r="B243" s="9"/>
       <c r="C243" s="10"/>
     </row>
-    <row r="244" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="2"/>
       <c r="B244" s="9"/>
       <c r="C244" s="10"/>
     </row>
-    <row r="245" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="2"/>
       <c r="B245" s="9"/>
       <c r="C245" s="10"/>
     </row>
-    <row r="246" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="2"/>
       <c r="B246" s="9"/>
       <c r="C246" s="10"/>
     </row>
-    <row r="247" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="2"/>
       <c r="B247" s="9"/>
       <c r="C247" s="10"/>
     </row>
-    <row r="248" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="2"/>
       <c r="B248" s="9"/>
       <c r="C248" s="10"/>
     </row>
-    <row r="249" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="2"/>
       <c r="B249" s="9"/>
       <c r="C249" s="10"/>

</xml_diff>

<commit_message>
Update RTM add development id for login & register features
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI material\QA\Online-Mobile-Store-WebSite\RTM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI9M-Testing\Core\QA\WorkShop\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F0E9CF-3EF4-4394-89E2-F5FC0CD69298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C933E1E-4136-4F32-9575-9FE6DA3E1D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="181">
   <si>
     <t>SRS ID</t>
   </si>
@@ -279,16 +279,10 @@
     <t>WireFrame_Reg_013</t>
   </si>
   <si>
-    <t>WireFrame_Client_001</t>
-  </si>
-  <si>
     <t>Wireframe_Checkout_001</t>
   </si>
   <si>
     <t>WireFrame Design ID</t>
-  </si>
-  <si>
-    <t>WireFrame_Supplier_001</t>
   </si>
   <si>
     <t>WireFrame_Supplier_002</t>
@@ -631,12 +625,6 @@
 edit.js</t>
   </si>
   <si>
-    <t>supplier_home.html                                                           supplier_home.js</t>
-  </si>
-  <si>
-    <t>client_home.html                                                           client_home.js</t>
-  </si>
-  <si>
     <t xml:space="preserve">UI_Client_Home_Page_001.jpeg
 CD__Client_Home_Page.jpeg
 FD_Client_Home_Page.jpeg
@@ -655,6 +643,9 @@
 FD_Checkout.jpeg
 SD_Checkout.png
 UI_Checkout.jpeg</t>
+  </si>
+  <si>
+    <t>WireFrame_Login_001</t>
   </si>
 </sst>
 </file>
@@ -1061,8 +1052,8 @@
   <dimension ref="A1:E249"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1082,13 +1073,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="59.4" customHeight="1" x14ac:dyDescent="0.35">
@@ -1096,16 +1087,16 @@
         <v>8</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>68</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.35">
@@ -1113,16 +1104,16 @@
         <v>9</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>69</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.35">
@@ -1130,16 +1121,16 @@
         <v>10</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>70</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="73.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -1153,10 +1144,10 @@
         <v>71</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.35">
@@ -1164,16 +1155,16 @@
         <v>13</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>72</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="82.2" customHeight="1" x14ac:dyDescent="0.35">
@@ -1187,10 +1178,10 @@
         <v>68</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
@@ -1198,16 +1189,16 @@
         <v>16</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>73</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1221,10 +1212,10 @@
         <v>68</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1232,16 +1223,16 @@
         <v>18</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>74</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="109.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -1255,10 +1246,10 @@
         <v>75</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="90.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -1272,10 +1263,10 @@
         <v>76</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.35">
@@ -1289,10 +1280,10 @@
         <v>77</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="61.2" customHeight="1" x14ac:dyDescent="0.35">
@@ -1306,10 +1297,10 @@
         <v>78</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
@@ -1323,10 +1314,10 @@
         <v>68</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.35">
@@ -1334,16 +1325,16 @@
         <v>29</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>79</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="55.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -1351,16 +1342,16 @@
         <v>31</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>80</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.35">
@@ -1368,16 +1359,16 @@
         <v>32</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>80</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="88.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -1385,16 +1376,16 @@
         <v>33</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>68</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="55.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -1402,16 +1393,16 @@
         <v>2</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>81</v>
+        <v>180</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="88.2" customHeight="1" x14ac:dyDescent="0.35">
@@ -1419,16 +1410,16 @@
         <v>3</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>81</v>
+        <v>180</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.35">
@@ -1436,16 +1427,16 @@
         <v>4</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.35">
@@ -1456,13 +1447,13 @@
         <v>7</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>84</v>
+        <v>180</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
@@ -1470,33 +1461,33 @@
         <v>6</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>99</v>
-      </c>
       <c r="C25" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
@@ -1504,16 +1495,16 @@
         <v>34</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
@@ -1521,16 +1512,16 @@
         <v>35</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C27" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="E27" s="10" t="s">
         <v>172</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
@@ -1538,16 +1529,16 @@
         <v>36</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
@@ -1555,16 +1546,16 @@
         <v>37</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
@@ -1572,16 +1563,16 @@
         <v>38</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
@@ -1589,16 +1580,16 @@
         <v>39</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
@@ -1606,16 +1597,16 @@
         <v>40</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
@@ -1626,47 +1617,47 @@
         <v>41</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D35" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="E35" s="10" t="s">
         <v>176</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1677,7 +1668,7 @@
         <v>58</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D36" s="15"/>
     </row>
@@ -1689,7 +1680,7 @@
         <v>59</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D37" s="15"/>
     </row>
@@ -1701,7 +1692,7 @@
         <v>65</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D38" s="15"/>
     </row>
@@ -1710,10 +1701,10 @@
         <v>47</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D39" s="15"/>
     </row>
@@ -1722,10 +1713,10 @@
         <v>48</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D40" s="15"/>
     </row>
@@ -1734,10 +1725,10 @@
         <v>49</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D41" s="15"/>
     </row>
@@ -1749,7 +1740,7 @@
         <v>60</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D42" s="15"/>
     </row>
@@ -1761,7 +1752,7 @@
         <v>61</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D43" s="15"/>
     </row>
@@ -1773,22 +1764,21 @@
         <v>62</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="D44" s="15"/>
-      <c r="E44" s="17" t="s">
-        <v>181</v>
+        <v>116</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D45" s="15"/>
     </row>
@@ -1797,10 +1787,10 @@
         <v>53</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D46" s="15"/>
     </row>
@@ -1809,10 +1799,10 @@
         <v>54</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D47" s="15"/>
     </row>
@@ -1824,11 +1814,11 @@
         <v>63</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D48" s="15"/>
     </row>
-    <row r="49" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>56</v>
       </c>
@@ -1836,140 +1826,137 @@
         <v>64</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D49" s="15"/>
     </row>
-    <row r="50" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D50" s="15"/>
     </row>
-    <row r="51" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D51" s="15"/>
     </row>
-    <row r="52" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D52" s="15"/>
     </row>
-    <row r="53" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D53" s="15"/>
-      <c r="E53" s="17" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D54" s="15"/>
-      <c r="E54" s="17" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D55" s="15"/>
-      <c r="E55" s="17" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="10"/>
       <c r="D56" s="15"/>
     </row>
-    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="10"/>
       <c r="D57" s="15"/>
     </row>
-    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="10"/>
       <c r="D58" s="15"/>
     </row>
-    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="9"/>
       <c r="C59" s="10"/>
       <c r="D59" s="15"/>
     </row>
-    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="9"/>
       <c r="C60" s="10"/>
       <c r="D60" s="15"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="9"/>
       <c r="C61" s="10"/>
       <c r="D61" s="15"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="9"/>
       <c r="C62" s="10"/>
       <c r="D62" s="15"/>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="9"/>
       <c r="C63" s="10"/>
       <c r="D63" s="15"/>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="9"/>
       <c r="C64" s="10"/>

</xml_diff>

<commit_message>
update TC and RTM
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI9M-Testing\Core\QA\WorkShop\Online-Mobile-Store-WebSite\RTM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ITI\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8DACC2-DF29-4975-80F0-E76B3FA8951A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DE6C81-0E0F-49E5-B4DC-174D9AA8938B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="179">
   <si>
     <t>SRS ID</t>
   </si>
@@ -397,13 +408,7 @@
     <t>TC_Client_020</t>
   </si>
   <si>
-    <t>WireFrame_Cart_004</t>
-  </si>
-  <si>
     <t>Wireframe_Client_002                        Wireframe_Client_003.jpg</t>
-  </si>
-  <si>
-    <t>WireFrame_Cart_005</t>
   </si>
   <si>
     <t>TC_Register_001         TC_Register_020         TC_Register_021        TC_Register_022        TC_Register_023         TC_Register_024        TC_Register_025         TC_Register_026</t>
@@ -594,6 +599,27 @@
   </si>
   <si>
     <t>index.html                                                           index.js</t>
+  </si>
+  <si>
+    <t>CD_OrderHistory                                           SD_OrderHistory                                                 UI_OrderHistory_001</t>
+  </si>
+  <si>
+    <t>CD_OrderHistory                                           SD_OrderHistory                                               UI_OrderHistory_001</t>
+  </si>
+  <si>
+    <t>CD_Cart                                                                FC_Cart                                                                                         SD_Cart_001                                                       UI_Cart_001</t>
+  </si>
+  <si>
+    <t>WireFrame_Cart_002</t>
+  </si>
+  <si>
+    <t>CD_Cart                                                                FC_Cart                                                                                         SD_Cart_001                                                       UI_Cart_002</t>
+  </si>
+  <si>
+    <t>cart.html                                                            cart.js</t>
+  </si>
+  <si>
+    <t>History.html                                                            History.js</t>
   </si>
 </sst>
 </file>
@@ -984,20 +1010,20 @@
   </sheetPr>
   <dimension ref="A1:E249"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="121" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="37.44140625" customWidth="1"/>
-    <col min="3" max="3" width="42.33203125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="38.44140625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="37.6640625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="37.7109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1008,64 +1034,64 @@
         <v>83</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="59.4" customHeight="1" x14ac:dyDescent="0.35">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="59.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>68</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>69</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>70</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="73.8" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1076,30 +1102,30 @@
         <v>71</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>72</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="82.2" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="82.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1110,30 +1136,30 @@
         <v>68</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>73</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1144,30 +1170,30 @@
         <v>68</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>74</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="109.8" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="109.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -1178,13 +1204,13 @@
         <v>75</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="90.6" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -1195,13 +1221,13 @@
         <v>76</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1212,13 +1238,13 @@
         <v>77</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="61.2" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="61.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1229,13 +1255,13 @@
         <v>78</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
@@ -1246,81 +1272,81 @@
         <v>68</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>79</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="55.8" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="55.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>80</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>80</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="88.8" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="88.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>68</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="55.8" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="55.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>2</v>
       </c>
@@ -1331,13 +1357,13 @@
         <v>81</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="88.2" customHeight="1" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="88.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>3</v>
       </c>
@@ -1348,13 +1374,13 @@
         <v>81</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>4</v>
       </c>
@@ -1365,13 +1391,13 @@
         <v>94</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>5</v>
       </c>
@@ -1382,13 +1408,13 @@
         <v>84</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
@@ -1399,13 +1425,13 @@
         <v>95</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>98</v>
       </c>
@@ -1416,111 +1442,111 @@
         <v>96</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="64.8" customHeight="1" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>85</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>86</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>87</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>88</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>88</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>88</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>89</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>42</v>
       </c>
@@ -1532,9 +1558,9 @@
       </c>
       <c r="D33" s="10"/>
     </row>
-    <row r="34" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>43</v>
@@ -1544,21 +1570,21 @@
       </c>
       <c r="D34" s="10"/>
     </row>
-    <row r="35" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>89</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>44</v>
       </c>
@@ -1568,9 +1594,14 @@
       <c r="C36" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="10"/>
-    </row>
-    <row r="37" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D36" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>45</v>
       </c>
@@ -1580,9 +1611,14 @@
       <c r="C37" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D37" s="10"/>
-    </row>
-    <row r="38" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D37" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>46</v>
       </c>
@@ -1592,9 +1628,14 @@
       <c r="C38" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D38" s="10"/>
-    </row>
-    <row r="39" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="D38" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>47</v>
       </c>
@@ -1604,9 +1645,14 @@
       <c r="C39" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D39" s="10"/>
-    </row>
-    <row r="40" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="D39" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>48</v>
       </c>
@@ -1616,9 +1662,14 @@
       <c r="C40" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D40" s="10"/>
-    </row>
-    <row r="41" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="D40" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>49</v>
       </c>
@@ -1628,9 +1679,14 @@
       <c r="C41" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D41" s="10"/>
-    </row>
-    <row r="42" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="D41" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>50</v>
       </c>
@@ -1640,9 +1696,14 @@
       <c r="C42" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D42" s="10"/>
-    </row>
-    <row r="43" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="D42" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="93" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>51</v>
       </c>
@@ -1652,9 +1713,14 @@
       <c r="C43" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D43" s="10"/>
-    </row>
-    <row r="44" spans="1:4" ht="27.6" x14ac:dyDescent="0.35">
+      <c r="D43" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>52</v>
       </c>
@@ -1662,11 +1728,11 @@
         <v>62</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D44" s="10"/>
     </row>
-    <row r="45" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>102</v>
       </c>
@@ -1676,9 +1742,14 @@
       <c r="C45" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D45" s="10"/>
-    </row>
-    <row r="46" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="D45" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>53</v>
       </c>
@@ -1688,9 +1759,14 @@
       <c r="C46" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D46" s="10"/>
-    </row>
-    <row r="47" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="D46" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="88.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>54</v>
       </c>
@@ -1700,9 +1776,14 @@
       <c r="C47" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D47" s="10"/>
-    </row>
-    <row r="48" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="D47" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="91.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>55</v>
       </c>
@@ -1712,9 +1793,14 @@
       <c r="C48" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D48" s="10"/>
-    </row>
-    <row r="49" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="D48" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>56</v>
       </c>
@@ -1724,9 +1810,14 @@
       <c r="C49" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="10"/>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D49" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>57</v>
       </c>
@@ -1736,9 +1827,14 @@
       <c r="C50" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D50" s="10"/>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D50" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>103</v>
       </c>
@@ -1746,11 +1842,16 @@
         <v>115</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D51" s="10"/>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>104</v>
       </c>
@@ -1758,11 +1859,16 @@
         <v>66</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="D52" s="10"/>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>105</v>
       </c>
@@ -1774,7 +1880,7 @@
       </c>
       <c r="D53" s="10"/>
     </row>
-    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>106</v>
       </c>
@@ -1786,7 +1892,7 @@
       </c>
       <c r="D54" s="10"/>
     </row>
-    <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>107</v>
       </c>
@@ -1798,1080 +1904,1080 @@
       </c>
       <c r="D55" s="10"/>
     </row>
-    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
     </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
     </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
     </row>
-    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="9"/>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
     </row>
-    <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="9"/>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
     </row>
-    <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="9"/>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
     </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="9"/>
       <c r="C62" s="10"/>
       <c r="D62" s="10"/>
     </row>
-    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="9"/>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
     </row>
-    <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="9"/>
       <c r="C64" s="10"/>
       <c r="D64" s="10"/>
     </row>
-    <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="9"/>
       <c r="C65" s="10"/>
       <c r="D65" s="10"/>
     </row>
-    <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="9"/>
       <c r="C66" s="10"/>
       <c r="D66" s="10"/>
     </row>
-    <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="9"/>
       <c r="C67" s="10"/>
       <c r="D67" s="10"/>
     </row>
-    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="9"/>
       <c r="C68" s="10"/>
       <c r="D68" s="10"/>
     </row>
-    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="9"/>
       <c r="C69" s="10"/>
       <c r="D69" s="10"/>
     </row>
-    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="9"/>
       <c r="C70" s="10"/>
       <c r="D70" s="10"/>
     </row>
-    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="9"/>
       <c r="C71" s="10"/>
       <c r="D71" s="10"/>
     </row>
-    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="9"/>
       <c r="C72" s="10"/>
       <c r="D72" s="10"/>
     </row>
-    <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="9"/>
       <c r="C73" s="10"/>
       <c r="D73" s="10"/>
     </row>
-    <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="9"/>
       <c r="C74" s="10"/>
       <c r="D74" s="10"/>
     </row>
-    <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="9"/>
       <c r="C75" s="10"/>
       <c r="D75" s="10"/>
     </row>
-    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="9"/>
       <c r="C76" s="10"/>
       <c r="D76" s="10"/>
     </row>
-    <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="9"/>
       <c r="C77" s="10"/>
       <c r="D77" s="10"/>
     </row>
-    <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="9"/>
       <c r="C78" s="10"/>
       <c r="D78" s="10"/>
     </row>
-    <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="9"/>
       <c r="C79" s="10"/>
       <c r="D79" s="10"/>
     </row>
-    <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="9"/>
       <c r="C80" s="10"/>
       <c r="D80" s="10"/>
     </row>
-    <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="9"/>
       <c r="C81" s="10"/>
       <c r="D81" s="10"/>
     </row>
-    <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="9"/>
       <c r="C82" s="10"/>
       <c r="D82" s="10"/>
     </row>
-    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="9"/>
       <c r="C83" s="10"/>
       <c r="D83" s="10"/>
     </row>
-    <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="9"/>
       <c r="C84" s="10"/>
       <c r="D84" s="10"/>
     </row>
-    <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="9"/>
       <c r="C85" s="10"/>
       <c r="D85" s="10"/>
     </row>
-    <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="9"/>
       <c r="C86" s="10"/>
       <c r="D86" s="10"/>
     </row>
-    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="9"/>
       <c r="C87" s="10"/>
       <c r="D87" s="10"/>
     </row>
-    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="9"/>
       <c r="C88" s="10"/>
       <c r="D88" s="10"/>
     </row>
-    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="9"/>
       <c r="C89" s="10"/>
       <c r="D89" s="10"/>
     </row>
-    <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="9"/>
       <c r="C90" s="10"/>
       <c r="D90" s="10"/>
     </row>
-    <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="9"/>
       <c r="C91" s="10"/>
       <c r="D91" s="10"/>
     </row>
-    <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="9"/>
       <c r="C92" s="10"/>
       <c r="D92" s="10"/>
     </row>
-    <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="9"/>
       <c r="C93" s="10"/>
       <c r="D93" s="10"/>
     </row>
-    <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="9"/>
       <c r="C94" s="10"/>
       <c r="D94" s="10"/>
     </row>
-    <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="9"/>
       <c r="C95" s="10"/>
       <c r="D95" s="10"/>
     </row>
-    <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="9"/>
       <c r="C96" s="10"/>
       <c r="D96" s="10"/>
     </row>
-    <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="9"/>
       <c r="C97" s="10"/>
       <c r="D97" s="10"/>
     </row>
-    <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="9"/>
       <c r="C98" s="10"/>
       <c r="D98" s="10"/>
     </row>
-    <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="9"/>
       <c r="C99" s="10"/>
       <c r="D99" s="10"/>
     </row>
-    <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="9"/>
       <c r="C100" s="10"/>
       <c r="D100" s="10"/>
     </row>
-    <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="9"/>
       <c r="C101" s="10"/>
       <c r="D101" s="10"/>
     </row>
-    <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="9"/>
       <c r="C102" s="10"/>
       <c r="D102" s="10"/>
     </row>
-    <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="9"/>
       <c r="C103" s="10"/>
       <c r="D103" s="10"/>
     </row>
-    <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="9"/>
       <c r="C104" s="10"/>
       <c r="D104" s="10"/>
     </row>
-    <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="9"/>
       <c r="C105" s="10"/>
       <c r="D105" s="10"/>
     </row>
-    <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="9"/>
       <c r="C106" s="10"/>
       <c r="D106" s="10"/>
     </row>
-    <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="9"/>
       <c r="C107" s="10"/>
       <c r="D107" s="10"/>
     </row>
-    <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="9"/>
       <c r="C108" s="10"/>
       <c r="D108" s="10"/>
     </row>
-    <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="9"/>
       <c r="C109" s="10"/>
       <c r="D109" s="10"/>
     </row>
-    <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="9"/>
       <c r="C110" s="10"/>
       <c r="D110" s="10"/>
     </row>
-    <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="9"/>
       <c r="C111" s="10"/>
       <c r="D111" s="10"/>
     </row>
-    <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="9"/>
       <c r="C112" s="10"/>
       <c r="D112" s="10"/>
     </row>
-    <row r="113" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="9"/>
       <c r="C113" s="10"/>
       <c r="D113" s="10"/>
     </row>
-    <row r="114" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="9"/>
       <c r="C114" s="10"/>
       <c r="D114" s="10"/>
     </row>
-    <row r="115" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="9"/>
       <c r="C115" s="10"/>
       <c r="D115" s="10"/>
     </row>
-    <row r="116" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="9"/>
       <c r="C116" s="10"/>
       <c r="D116" s="10"/>
     </row>
-    <row r="117" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="9"/>
       <c r="C117" s="10"/>
       <c r="D117" s="10"/>
     </row>
-    <row r="118" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="9"/>
       <c r="C118" s="10"/>
       <c r="D118" s="10"/>
     </row>
-    <row r="119" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="9"/>
       <c r="C119" s="10"/>
       <c r="D119" s="10"/>
     </row>
-    <row r="120" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="9"/>
       <c r="C120" s="10"/>
       <c r="D120" s="10"/>
     </row>
-    <row r="121" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="9"/>
       <c r="C121" s="10"/>
       <c r="D121" s="10"/>
     </row>
-    <row r="122" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="9"/>
       <c r="C122" s="10"/>
       <c r="D122" s="10"/>
     </row>
-    <row r="123" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="9"/>
       <c r="C123" s="10"/>
       <c r="D123" s="10"/>
     </row>
-    <row r="124" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="9"/>
       <c r="C124" s="10"/>
       <c r="D124" s="10"/>
     </row>
-    <row r="125" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="9"/>
       <c r="C125" s="10"/>
       <c r="D125" s="10"/>
     </row>
-    <row r="126" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="9"/>
       <c r="C126" s="10"/>
       <c r="D126" s="10"/>
     </row>
-    <row r="127" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="9"/>
       <c r="C127" s="10"/>
       <c r="D127" s="10"/>
     </row>
-    <row r="128" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="9"/>
       <c r="C128" s="10"/>
       <c r="D128" s="10"/>
     </row>
-    <row r="129" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="9"/>
       <c r="C129" s="10"/>
       <c r="D129" s="10"/>
     </row>
-    <row r="130" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="9"/>
       <c r="C130" s="10"/>
       <c r="D130" s="10"/>
     </row>
-    <row r="131" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="9"/>
       <c r="C131" s="10"/>
       <c r="D131" s="10"/>
     </row>
-    <row r="132" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="9"/>
       <c r="C132" s="10"/>
       <c r="D132" s="10"/>
     </row>
-    <row r="133" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="9"/>
       <c r="C133" s="10"/>
       <c r="D133" s="10"/>
     </row>
-    <row r="134" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="9"/>
       <c r="C134" s="10"/>
       <c r="D134" s="10"/>
     </row>
-    <row r="135" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="9"/>
       <c r="C135" s="10"/>
       <c r="D135" s="10"/>
     </row>
-    <row r="136" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="9"/>
       <c r="C136" s="10"/>
       <c r="D136" s="10"/>
     </row>
-    <row r="137" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="B137" s="9"/>
       <c r="C137" s="10"/>
       <c r="D137" s="10"/>
     </row>
-    <row r="138" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
       <c r="B138" s="9"/>
       <c r="C138" s="10"/>
       <c r="D138" s="10"/>
     </row>
-    <row r="139" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
       <c r="B139" s="9"/>
       <c r="C139" s="10"/>
       <c r="D139" s="10"/>
     </row>
-    <row r="140" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140" s="9"/>
       <c r="C140" s="10"/>
       <c r="D140" s="10"/>
     </row>
-    <row r="141" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141" s="9"/>
       <c r="C141" s="10"/>
       <c r="D141" s="10"/>
     </row>
-    <row r="142" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142" s="9"/>
       <c r="C142" s="10"/>
       <c r="D142" s="10"/>
     </row>
-    <row r="143" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
       <c r="B143" s="9"/>
       <c r="C143" s="10"/>
       <c r="D143" s="10"/>
     </row>
-    <row r="144" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
       <c r="B144" s="9"/>
       <c r="C144" s="10"/>
       <c r="D144" s="10"/>
     </row>
-    <row r="145" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
       <c r="B145" s="9"/>
       <c r="C145" s="10"/>
       <c r="D145" s="10"/>
     </row>
-    <row r="146" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
       <c r="B146" s="9"/>
       <c r="C146" s="10"/>
       <c r="D146" s="10"/>
     </row>
-    <row r="147" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
       <c r="B147" s="9"/>
       <c r="C147" s="10"/>
       <c r="D147" s="10"/>
     </row>
-    <row r="148" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
       <c r="B148" s="9"/>
       <c r="C148" s="10"/>
       <c r="D148" s="10"/>
     </row>
-    <row r="149" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
       <c r="B149" s="9"/>
       <c r="C149" s="10"/>
       <c r="D149" s="10"/>
     </row>
-    <row r="150" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
       <c r="B150" s="9"/>
       <c r="C150" s="10"/>
       <c r="D150" s="10"/>
     </row>
-    <row r="151" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2"/>
       <c r="B151" s="9"/>
       <c r="C151" s="10"/>
       <c r="D151" s="10"/>
     </row>
-    <row r="152" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2"/>
       <c r="B152" s="9"/>
       <c r="C152" s="10"/>
       <c r="D152" s="10"/>
     </row>
-    <row r="153" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2"/>
       <c r="B153" s="9"/>
       <c r="C153" s="10"/>
       <c r="D153" s="10"/>
     </row>
-    <row r="154" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2"/>
       <c r="B154" s="9"/>
       <c r="C154" s="10"/>
       <c r="D154" s="10"/>
     </row>
-    <row r="155" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2"/>
       <c r="B155" s="9"/>
       <c r="C155" s="10"/>
       <c r="D155" s="10"/>
     </row>
-    <row r="156" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2"/>
       <c r="B156" s="9"/>
       <c r="C156" s="10"/>
       <c r="D156" s="10"/>
     </row>
-    <row r="157" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2"/>
       <c r="B157" s="9"/>
       <c r="C157" s="10"/>
       <c r="D157" s="10"/>
     </row>
-    <row r="158" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2"/>
       <c r="B158" s="9"/>
       <c r="C158" s="10"/>
       <c r="D158" s="10"/>
     </row>
-    <row r="159" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2"/>
       <c r="B159" s="9"/>
       <c r="C159" s="10"/>
       <c r="D159" s="10"/>
     </row>
-    <row r="160" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2"/>
       <c r="B160" s="9"/>
       <c r="C160" s="10"/>
       <c r="D160" s="10"/>
     </row>
-    <row r="161" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2"/>
       <c r="B161" s="9"/>
       <c r="C161" s="10"/>
       <c r="D161" s="10"/>
     </row>
-    <row r="162" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2"/>
       <c r="B162" s="9"/>
       <c r="C162" s="10"/>
       <c r="D162" s="10"/>
     </row>
-    <row r="163" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
       <c r="B163" s="9"/>
       <c r="C163" s="10"/>
       <c r="D163" s="10"/>
     </row>
-    <row r="164" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2"/>
       <c r="B164" s="9"/>
       <c r="C164" s="10"/>
     </row>
-    <row r="165" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2"/>
       <c r="B165" s="9"/>
       <c r="C165" s="10"/>
     </row>
-    <row r="166" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2"/>
       <c r="B166" s="9"/>
       <c r="C166" s="10"/>
     </row>
-    <row r="167" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2"/>
       <c r="B167" s="9"/>
       <c r="C167" s="10"/>
     </row>
-    <row r="168" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2"/>
       <c r="B168" s="9"/>
       <c r="C168" s="10"/>
     </row>
-    <row r="169" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2"/>
       <c r="B169" s="9"/>
       <c r="C169" s="10"/>
     </row>
-    <row r="170" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2"/>
       <c r="B170" s="9"/>
       <c r="C170" s="10"/>
     </row>
-    <row r="171" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2"/>
       <c r="B171" s="9"/>
       <c r="C171" s="10"/>
     </row>
-    <row r="172" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2"/>
       <c r="B172" s="9"/>
       <c r="C172" s="10"/>
     </row>
-    <row r="173" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2"/>
       <c r="B173" s="9"/>
       <c r="C173" s="10"/>
     </row>
-    <row r="174" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2"/>
       <c r="B174" s="9"/>
       <c r="C174" s="10"/>
     </row>
-    <row r="175" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2"/>
       <c r="B175" s="9"/>
       <c r="C175" s="10"/>
     </row>
-    <row r="176" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2"/>
       <c r="B176" s="9"/>
       <c r="C176" s="10"/>
     </row>
-    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2"/>
       <c r="B177" s="9"/>
       <c r="C177" s="10"/>
     </row>
-    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2"/>
       <c r="B178" s="9"/>
       <c r="C178" s="10"/>
     </row>
-    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2"/>
       <c r="B179" s="9"/>
       <c r="C179" s="10"/>
     </row>
-    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2"/>
       <c r="B180" s="9"/>
       <c r="C180" s="10"/>
     </row>
-    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2"/>
       <c r="B181" s="9"/>
       <c r="C181" s="10"/>
     </row>
-    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2"/>
       <c r="B182" s="9"/>
       <c r="C182" s="10"/>
     </row>
-    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2"/>
       <c r="B183" s="9"/>
       <c r="C183" s="10"/>
     </row>
-    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2"/>
       <c r="B184" s="9"/>
       <c r="C184" s="10"/>
     </row>
-    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2"/>
       <c r="B185" s="9"/>
       <c r="C185" s="10"/>
     </row>
-    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2"/>
       <c r="B186" s="9"/>
       <c r="C186" s="10"/>
     </row>
-    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2"/>
       <c r="B187" s="9"/>
       <c r="C187" s="10"/>
     </row>
-    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2"/>
       <c r="B188" s="9"/>
       <c r="C188" s="10"/>
     </row>
-    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2"/>
       <c r="B189" s="9"/>
       <c r="C189" s="10"/>
     </row>
-    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2"/>
       <c r="B190" s="9"/>
       <c r="C190" s="10"/>
     </row>
-    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2"/>
       <c r="B191" s="9"/>
       <c r="C191" s="10"/>
     </row>
-    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2"/>
       <c r="B192" s="9"/>
       <c r="C192" s="10"/>
     </row>
-    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="2"/>
       <c r="B193" s="9"/>
       <c r="C193" s="10"/>
     </row>
-    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2"/>
       <c r="B194" s="9"/>
       <c r="C194" s="10"/>
     </row>
-    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="2"/>
       <c r="B195" s="9"/>
       <c r="C195" s="10"/>
     </row>
-    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="2"/>
       <c r="B196" s="9"/>
       <c r="C196" s="10"/>
     </row>
-    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="2"/>
       <c r="B197" s="9"/>
       <c r="C197" s="10"/>
     </row>
-    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="2"/>
       <c r="B198" s="9"/>
       <c r="C198" s="10"/>
     </row>
-    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="2"/>
       <c r="B199" s="9"/>
       <c r="C199" s="10"/>
     </row>
-    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="2"/>
       <c r="B200" s="9"/>
       <c r="C200" s="10"/>
     </row>
-    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="2"/>
       <c r="B201" s="9"/>
       <c r="C201" s="10"/>
     </row>
-    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2"/>
       <c r="B202" s="9"/>
       <c r="C202" s="10"/>
     </row>
-    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2"/>
       <c r="B203" s="9"/>
       <c r="C203" s="10"/>
     </row>
-    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="2"/>
       <c r="B204" s="9"/>
       <c r="C204" s="10"/>
     </row>
-    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2"/>
       <c r="B205" s="9"/>
       <c r="C205" s="10"/>
     </row>
-    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2"/>
       <c r="B206" s="9"/>
       <c r="C206" s="10"/>
     </row>
-    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2"/>
       <c r="B207" s="9"/>
       <c r="C207" s="10"/>
     </row>
-    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2"/>
       <c r="B208" s="9"/>
       <c r="C208" s="10"/>
     </row>
-    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2"/>
       <c r="B209" s="9"/>
       <c r="C209" s="10"/>
     </row>
-    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2"/>
       <c r="B210" s="9"/>
       <c r="C210" s="10"/>
     </row>
-    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2"/>
       <c r="B211" s="9"/>
       <c r="C211" s="10"/>
     </row>
-    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2"/>
       <c r="B212" s="9"/>
       <c r="C212" s="10"/>
     </row>
-    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2"/>
       <c r="B213" s="9"/>
       <c r="C213" s="10"/>
     </row>
-    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2"/>
       <c r="B214" s="9"/>
       <c r="C214" s="10"/>
     </row>
-    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="2"/>
       <c r="B215" s="9"/>
       <c r="C215" s="10"/>
     </row>
-    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="2"/>
       <c r="B216" s="9"/>
       <c r="C216" s="10"/>
     </row>
-    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2"/>
       <c r="B217" s="9"/>
       <c r="C217" s="10"/>
     </row>
-    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="2"/>
       <c r="B218" s="9"/>
       <c r="C218" s="10"/>
     </row>
-    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="2"/>
       <c r="B219" s="9"/>
       <c r="C219" s="10"/>
     </row>
-    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="2"/>
       <c r="B220" s="9"/>
       <c r="C220" s="10"/>
     </row>
-    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="2"/>
       <c r="B221" s="9"/>
       <c r="C221" s="10"/>
     </row>
-    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="2"/>
       <c r="B222" s="9"/>
       <c r="C222" s="10"/>
     </row>
-    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2"/>
       <c r="B223" s="9"/>
       <c r="C223" s="10"/>
     </row>
-    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="2"/>
       <c r="B224" s="9"/>
       <c r="C224" s="10"/>
     </row>
-    <row r="225" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="2"/>
       <c r="B225" s="9"/>
       <c r="C225" s="10"/>
     </row>
-    <row r="226" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2"/>
       <c r="B226" s="9"/>
       <c r="C226" s="10"/>
     </row>
-    <row r="227" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2"/>
       <c r="B227" s="9"/>
       <c r="C227" s="10"/>
     </row>
-    <row r="228" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="2"/>
       <c r="B228" s="9"/>
       <c r="C228" s="10"/>
     </row>
-    <row r="229" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="2"/>
       <c r="B229" s="9"/>
       <c r="C229" s="10"/>
     </row>
-    <row r="230" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="2"/>
       <c r="B230" s="9"/>
       <c r="C230" s="10"/>
     </row>
-    <row r="231" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="2"/>
       <c r="B231" s="9"/>
       <c r="C231" s="10"/>
     </row>
-    <row r="232" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="2"/>
       <c r="B232" s="9"/>
       <c r="C232" s="10"/>
     </row>
-    <row r="233" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="2"/>
       <c r="B233" s="9"/>
       <c r="C233" s="10"/>
     </row>
-    <row r="234" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="2"/>
       <c r="B234" s="9"/>
       <c r="C234" s="10"/>
     </row>
-    <row r="235" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="2"/>
       <c r="B235" s="9"/>
       <c r="C235" s="10"/>
     </row>
-    <row r="236" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="2"/>
       <c r="B236" s="9"/>
       <c r="C236" s="10"/>
     </row>
-    <row r="237" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="2"/>
       <c r="B237" s="9"/>
       <c r="C237" s="10"/>
     </row>
-    <row r="238" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="2"/>
       <c r="B238" s="9"/>
       <c r="C238" s="10"/>
     </row>
-    <row r="239" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="2"/>
       <c r="B239" s="9"/>
       <c r="C239" s="10"/>
     </row>
-    <row r="240" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="2"/>
       <c r="B240" s="9"/>
       <c r="C240" s="10"/>
     </row>
-    <row r="241" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="2"/>
       <c r="B241" s="9"/>
       <c r="C241" s="10"/>
     </row>
-    <row r="242" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="2"/>
       <c r="B242" s="9"/>
       <c r="C242" s="10"/>
     </row>
-    <row r="243" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="2"/>
       <c r="B243" s="9"/>
       <c r="C243" s="10"/>
     </row>
-    <row r="244" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="2"/>
       <c r="B244" s="9"/>
       <c r="C244" s="10"/>
     </row>
-    <row r="245" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="2"/>
       <c r="B245" s="9"/>
       <c r="C245" s="10"/>
     </row>
-    <row r="246" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="2"/>
       <c r="B246" s="9"/>
       <c r="C246" s="10"/>
     </row>
-    <row r="247" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="2"/>
       <c r="B247" s="9"/>
       <c r="C247" s="10"/>
     </row>
-    <row r="248" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="2"/>
       <c r="B248" s="9"/>
       <c r="C248" s="10"/>
     </row>
-    <row r="249" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="2"/>
       <c r="B249" s="9"/>
       <c r="C249" s="10"/>

</xml_diff>

<commit_message>
RTM - TC - Wireframe - UI - Release plan about Mariam
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI material\QA\Online-Mobile-Store-WebSite\RTM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ITI\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB2C803-8269-4C47-8FF4-04AA3415BE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56DFD89-DDDC-468B-93E4-7B3F3E00FB79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="188">
   <si>
     <t>SRS ID</t>
   </si>
@@ -400,13 +400,7 @@
     <t>TC_Client_020</t>
   </si>
   <si>
-    <t>WireFrame_Cart_004</t>
-  </si>
-  <si>
     <t>Wireframe_Client_002                        Wireframe_Client_003.jpg</t>
-  </si>
-  <si>
-    <t>WireFrame_Cart_005</t>
   </si>
   <si>
     <t>TC_Register_001         TC_Register_020         TC_Register_021        TC_Register_022        TC_Register_023         TC_Register_024        TC_Register_025         TC_Register_026</t>
@@ -654,6 +648,27 @@
   <si>
     <t>checkout.html
 checkout.js</t>
+  </si>
+  <si>
+    <t>CD_OrderHistory                                           SD_OrderHistory                                                 UI_OrderHistory_001</t>
+  </si>
+  <si>
+    <t>History.html                                                            History.js</t>
+  </si>
+  <si>
+    <t>CD_OrderHistory                                           SD_OrderHistory                                               UI_OrderHistory_001</t>
+  </si>
+  <si>
+    <t>CD_Cart                                                                FC_Cart                                                                                         SD_Cart_001                                                       UI_Cart_001</t>
+  </si>
+  <si>
+    <t>cart.html                                                            cart.js</t>
+  </si>
+  <si>
+    <t>WireFrame_Cart_002</t>
+  </si>
+  <si>
+    <t>CD_Cart                                                                FC_Cart                                                                                         SD_Cart_001                                                       UI_Cart_002</t>
   </si>
 </sst>
 </file>
@@ -1060,20 +1075,20 @@
   <dimension ref="A1:E249"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E55" sqref="E55"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="37.44140625" customWidth="1"/>
-    <col min="3" max="3" width="42.33203125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="38.44140625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="37.6640625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="37.7109375" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1084,64 +1099,64 @@
         <v>82</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="59.4" customHeight="1" x14ac:dyDescent="0.35">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="59.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>68</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>69</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>70</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="73.95" customHeight="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1152,30 +1167,30 @@
         <v>71</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>72</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="82.2" customHeight="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="82.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1186,30 +1201,30 @@
         <v>68</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>73</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1220,30 +1235,30 @@
         <v>68</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>74</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="109.95" customHeight="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="109.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -1254,13 +1269,13 @@
         <v>75</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="90.6" customHeight="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -1271,13 +1286,13 @@
         <v>76</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1288,13 +1303,13 @@
         <v>77</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="61.2" customHeight="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="61.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1305,13 +1320,13 @@
         <v>78</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
@@ -1322,81 +1337,81 @@
         <v>68</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>79</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="55.95" customHeight="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="55.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>80</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>80</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="88.95" customHeight="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="88.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>68</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="55.95" customHeight="1" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="55.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>2</v>
       </c>
@@ -1404,16 +1419,16 @@
         <v>96</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="88.2" customHeight="1" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="88.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>3</v>
       </c>
@@ -1421,16 +1436,16 @@
         <v>96</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>4</v>
       </c>
@@ -1441,13 +1456,13 @@
         <v>91</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>5</v>
       </c>
@@ -1455,16 +1470,16 @@
         <v>7</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
@@ -1475,13 +1490,13 @@
         <v>92</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>95</v>
       </c>
@@ -1492,132 +1507,132 @@
         <v>93</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>83</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C27" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="E27" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="D27" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>84</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>85</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>85</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>86</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>42</v>
       </c>
@@ -1628,15 +1643,15 @@
         <v>87</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>43</v>
@@ -1645,30 +1660,30 @@
         <v>88</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D35" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="E35" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="E35" s="10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>44</v>
       </c>
@@ -1678,9 +1693,14 @@
       <c r="C36" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D36" s="15"/>
-    </row>
-    <row r="37" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D36" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>45</v>
       </c>
@@ -1690,9 +1710,14 @@
       <c r="C37" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D37" s="15"/>
-    </row>
-    <row r="38" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D37" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>46</v>
       </c>
@@ -1702,9 +1727,14 @@
       <c r="C38" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D38" s="15"/>
-    </row>
-    <row r="39" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="D38" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="39.75" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>47</v>
       </c>
@@ -1714,9 +1744,14 @@
       <c r="C39" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="15"/>
-    </row>
-    <row r="40" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="D39" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="39.75" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>48</v>
       </c>
@@ -1726,9 +1761,14 @@
       <c r="C40" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D40" s="15"/>
-    </row>
-    <row r="41" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="D40" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="39.75" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>49</v>
       </c>
@@ -1738,9 +1778,14 @@
       <c r="C41" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D41" s="15"/>
-    </row>
-    <row r="42" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="D41" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="39.75" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>50</v>
       </c>
@@ -1750,9 +1795,14 @@
       <c r="C42" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D42" s="15"/>
-    </row>
-    <row r="43" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="D42" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="39.75" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>51</v>
       </c>
@@ -1762,9 +1812,14 @@
       <c r="C43" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D43" s="15"/>
-    </row>
-    <row r="44" spans="1:5" ht="67.2" x14ac:dyDescent="0.35">
+      <c r="D43" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="65.25" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>52</v>
       </c>
@@ -1772,16 +1827,16 @@
         <v>62</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>99</v>
       </c>
@@ -1791,9 +1846,14 @@
       <c r="C45" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D45" s="15"/>
-    </row>
-    <row r="46" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D45" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>53</v>
       </c>
@@ -1803,9 +1863,14 @@
       <c r="C46" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D46" s="15"/>
-    </row>
-    <row r="47" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D46" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>54</v>
       </c>
@@ -1815,9 +1880,14 @@
       <c r="C47" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D47" s="15"/>
-    </row>
-    <row r="48" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D47" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>55</v>
       </c>
@@ -1827,9 +1897,14 @@
       <c r="C48" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D48" s="15"/>
-    </row>
-    <row r="49" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D48" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>56</v>
       </c>
@@ -1839,9 +1914,14 @@
       <c r="C49" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D49" s="15"/>
-    </row>
-    <row r="50" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D49" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>57</v>
       </c>
@@ -1851,9 +1931,14 @@
       <c r="C50" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D50" s="15"/>
-    </row>
-    <row r="51" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D50" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>100</v>
       </c>
@@ -1861,11 +1946,16 @@
         <v>112</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="D51" s="15"/>
-    </row>
-    <row r="52" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>101</v>
       </c>
@@ -1873,11 +1963,16 @@
         <v>66</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="D52" s="15"/>
-    </row>
-    <row r="53" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>102</v>
       </c>
@@ -1888,13 +1983,13 @@
         <v>81</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>103</v>
       </c>
@@ -1905,13 +2000,13 @@
         <v>81</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>104</v>
       </c>
@@ -1922,1086 +2017,1086 @@
         <v>81</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="10"/>
       <c r="D56" s="15"/>
     </row>
-    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="10"/>
       <c r="D57" s="15"/>
     </row>
-    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="10"/>
       <c r="D58" s="15"/>
     </row>
-    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="9"/>
       <c r="C59" s="10"/>
       <c r="D59" s="15"/>
     </row>
-    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="9"/>
       <c r="C60" s="10"/>
       <c r="D60" s="15"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="9"/>
       <c r="C61" s="10"/>
       <c r="D61" s="15"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="9"/>
       <c r="C62" s="10"/>
       <c r="D62" s="15"/>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="9"/>
       <c r="C63" s="10"/>
       <c r="D63" s="15"/>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="9"/>
       <c r="C64" s="10"/>
       <c r="D64" s="15"/>
     </row>
-    <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="9"/>
       <c r="C65" s="10"/>
       <c r="D65" s="15"/>
     </row>
-    <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="9"/>
       <c r="C66" s="10"/>
       <c r="D66" s="15"/>
     </row>
-    <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="9"/>
       <c r="C67" s="10"/>
       <c r="D67" s="15"/>
     </row>
-    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="9"/>
       <c r="C68" s="10"/>
       <c r="D68" s="15"/>
     </row>
-    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="9"/>
       <c r="C69" s="10"/>
       <c r="D69" s="15"/>
     </row>
-    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="9"/>
       <c r="C70" s="10"/>
       <c r="D70" s="15"/>
     </row>
-    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="9"/>
       <c r="C71" s="10"/>
       <c r="D71" s="15"/>
     </row>
-    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="9"/>
       <c r="C72" s="10"/>
       <c r="D72" s="15"/>
     </row>
-    <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="9"/>
       <c r="C73" s="10"/>
       <c r="D73" s="15"/>
     </row>
-    <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="9"/>
       <c r="C74" s="10"/>
       <c r="D74" s="15"/>
     </row>
-    <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="9"/>
       <c r="C75" s="10"/>
       <c r="D75" s="15"/>
     </row>
-    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="9"/>
       <c r="C76" s="10"/>
       <c r="D76" s="15"/>
     </row>
-    <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="9"/>
       <c r="C77" s="10"/>
       <c r="D77" s="15"/>
     </row>
-    <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="9"/>
       <c r="C78" s="10"/>
       <c r="D78" s="15"/>
     </row>
-    <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="9"/>
       <c r="C79" s="10"/>
       <c r="D79" s="15"/>
     </row>
-    <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="9"/>
       <c r="C80" s="10"/>
       <c r="D80" s="15"/>
     </row>
-    <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="9"/>
       <c r="C81" s="10"/>
       <c r="D81" s="15"/>
     </row>
-    <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="9"/>
       <c r="C82" s="10"/>
       <c r="D82" s="15"/>
     </row>
-    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="9"/>
       <c r="C83" s="10"/>
       <c r="D83" s="15"/>
     </row>
-    <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="9"/>
       <c r="C84" s="10"/>
       <c r="D84" s="15"/>
     </row>
-    <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="9"/>
       <c r="C85" s="10"/>
       <c r="D85" s="15"/>
     </row>
-    <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="9"/>
       <c r="C86" s="10"/>
       <c r="D86" s="15"/>
     </row>
-    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="9"/>
       <c r="C87" s="10"/>
       <c r="D87" s="15"/>
     </row>
-    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="9"/>
       <c r="C88" s="10"/>
       <c r="D88" s="15"/>
     </row>
-    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="9"/>
       <c r="C89" s="10"/>
       <c r="D89" s="15"/>
     </row>
-    <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="9"/>
       <c r="C90" s="10"/>
       <c r="D90" s="15"/>
     </row>
-    <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="9"/>
       <c r="C91" s="10"/>
       <c r="D91" s="15"/>
     </row>
-    <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="9"/>
       <c r="C92" s="10"/>
       <c r="D92" s="15"/>
     </row>
-    <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="9"/>
       <c r="C93" s="10"/>
       <c r="D93" s="15"/>
     </row>
-    <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="9"/>
       <c r="C94" s="10"/>
       <c r="D94" s="15"/>
     </row>
-    <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="9"/>
       <c r="C95" s="10"/>
       <c r="D95" s="15"/>
     </row>
-    <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="9"/>
       <c r="C96" s="10"/>
       <c r="D96" s="15"/>
     </row>
-    <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="9"/>
       <c r="C97" s="10"/>
       <c r="D97" s="15"/>
     </row>
-    <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="9"/>
       <c r="C98" s="10"/>
       <c r="D98" s="15"/>
     </row>
-    <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="9"/>
       <c r="C99" s="10"/>
       <c r="D99" s="15"/>
     </row>
-    <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="9"/>
       <c r="C100" s="10"/>
       <c r="D100" s="15"/>
     </row>
-    <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="9"/>
       <c r="C101" s="10"/>
       <c r="D101" s="15"/>
     </row>
-    <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="9"/>
       <c r="C102" s="10"/>
       <c r="D102" s="15"/>
     </row>
-    <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="9"/>
       <c r="C103" s="10"/>
       <c r="D103" s="15"/>
     </row>
-    <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="9"/>
       <c r="C104" s="10"/>
       <c r="D104" s="15"/>
     </row>
-    <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="9"/>
       <c r="C105" s="10"/>
       <c r="D105" s="15"/>
     </row>
-    <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="9"/>
       <c r="C106" s="10"/>
       <c r="D106" s="15"/>
     </row>
-    <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="9"/>
       <c r="C107" s="10"/>
       <c r="D107" s="15"/>
     </row>
-    <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="9"/>
       <c r="C108" s="10"/>
       <c r="D108" s="15"/>
     </row>
-    <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="9"/>
       <c r="C109" s="10"/>
       <c r="D109" s="15"/>
     </row>
-    <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="9"/>
       <c r="C110" s="10"/>
       <c r="D110" s="15"/>
     </row>
-    <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="9"/>
       <c r="C111" s="10"/>
       <c r="D111" s="15"/>
     </row>
-    <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="9"/>
       <c r="C112" s="10"/>
       <c r="D112" s="15"/>
     </row>
-    <row r="113" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="9"/>
       <c r="C113" s="10"/>
       <c r="D113" s="15"/>
     </row>
-    <row r="114" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="9"/>
       <c r="C114" s="10"/>
       <c r="D114" s="15"/>
     </row>
-    <row r="115" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="9"/>
       <c r="C115" s="10"/>
       <c r="D115" s="15"/>
     </row>
-    <row r="116" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="9"/>
       <c r="C116" s="10"/>
       <c r="D116" s="15"/>
     </row>
-    <row r="117" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="9"/>
       <c r="C117" s="10"/>
       <c r="D117" s="15"/>
     </row>
-    <row r="118" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="9"/>
       <c r="C118" s="10"/>
       <c r="D118" s="15"/>
     </row>
-    <row r="119" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="9"/>
       <c r="C119" s="10"/>
       <c r="D119" s="15"/>
     </row>
-    <row r="120" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="9"/>
       <c r="C120" s="10"/>
       <c r="D120" s="15"/>
     </row>
-    <row r="121" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="9"/>
       <c r="C121" s="10"/>
       <c r="D121" s="15"/>
     </row>
-    <row r="122" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="9"/>
       <c r="C122" s="10"/>
       <c r="D122" s="15"/>
     </row>
-    <row r="123" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="9"/>
       <c r="C123" s="10"/>
       <c r="D123" s="15"/>
     </row>
-    <row r="124" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="9"/>
       <c r="C124" s="10"/>
       <c r="D124" s="15"/>
     </row>
-    <row r="125" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="9"/>
       <c r="C125" s="10"/>
       <c r="D125" s="15"/>
     </row>
-    <row r="126" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="9"/>
       <c r="C126" s="10"/>
       <c r="D126" s="15"/>
     </row>
-    <row r="127" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="9"/>
       <c r="C127" s="10"/>
       <c r="D127" s="15"/>
     </row>
-    <row r="128" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="9"/>
       <c r="C128" s="10"/>
       <c r="D128" s="15"/>
     </row>
-    <row r="129" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="9"/>
       <c r="C129" s="10"/>
       <c r="D129" s="15"/>
     </row>
-    <row r="130" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="9"/>
       <c r="C130" s="10"/>
       <c r="D130" s="15"/>
     </row>
-    <row r="131" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="9"/>
       <c r="C131" s="10"/>
       <c r="D131" s="15"/>
     </row>
-    <row r="132" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="9"/>
       <c r="C132" s="10"/>
       <c r="D132" s="15"/>
     </row>
-    <row r="133" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="9"/>
       <c r="C133" s="10"/>
       <c r="D133" s="15"/>
     </row>
-    <row r="134" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="9"/>
       <c r="C134" s="10"/>
       <c r="D134" s="15"/>
     </row>
-    <row r="135" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="9"/>
       <c r="C135" s="10"/>
       <c r="D135" s="15"/>
     </row>
-    <row r="136" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="9"/>
       <c r="C136" s="10"/>
       <c r="D136" s="15"/>
     </row>
-    <row r="137" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="B137" s="9"/>
       <c r="C137" s="10"/>
       <c r="D137" s="15"/>
     </row>
-    <row r="138" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
       <c r="B138" s="9"/>
       <c r="C138" s="10"/>
       <c r="D138" s="15"/>
     </row>
-    <row r="139" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
       <c r="B139" s="9"/>
       <c r="C139" s="10"/>
       <c r="D139" s="15"/>
     </row>
-    <row r="140" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140" s="9"/>
       <c r="C140" s="10"/>
       <c r="D140" s="15"/>
     </row>
-    <row r="141" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141" s="9"/>
       <c r="C141" s="10"/>
       <c r="D141" s="15"/>
     </row>
-    <row r="142" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142" s="9"/>
       <c r="C142" s="10"/>
       <c r="D142" s="15"/>
     </row>
-    <row r="143" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
       <c r="B143" s="9"/>
       <c r="C143" s="10"/>
       <c r="D143" s="15"/>
     </row>
-    <row r="144" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
       <c r="B144" s="9"/>
       <c r="C144" s="10"/>
       <c r="D144" s="15"/>
     </row>
-    <row r="145" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
       <c r="B145" s="9"/>
       <c r="C145" s="10"/>
       <c r="D145" s="15"/>
     </row>
-    <row r="146" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
       <c r="B146" s="9"/>
       <c r="C146" s="10"/>
       <c r="D146" s="15"/>
     </row>
-    <row r="147" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
       <c r="B147" s="9"/>
       <c r="C147" s="10"/>
       <c r="D147" s="15"/>
     </row>
-    <row r="148" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
       <c r="B148" s="9"/>
       <c r="C148" s="10"/>
       <c r="D148" s="15"/>
     </row>
-    <row r="149" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
       <c r="B149" s="9"/>
       <c r="C149" s="10"/>
       <c r="D149" s="15"/>
     </row>
-    <row r="150" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
       <c r="B150" s="9"/>
       <c r="C150" s="10"/>
       <c r="D150" s="15"/>
     </row>
-    <row r="151" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2"/>
       <c r="B151" s="9"/>
       <c r="C151" s="10"/>
       <c r="D151" s="15"/>
     </row>
-    <row r="152" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2"/>
       <c r="B152" s="9"/>
       <c r="C152" s="10"/>
       <c r="D152" s="15"/>
     </row>
-    <row r="153" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2"/>
       <c r="B153" s="9"/>
       <c r="C153" s="10"/>
       <c r="D153" s="15"/>
     </row>
-    <row r="154" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2"/>
       <c r="B154" s="9"/>
       <c r="C154" s="10"/>
       <c r="D154" s="15"/>
     </row>
-    <row r="155" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2"/>
       <c r="B155" s="9"/>
       <c r="C155" s="10"/>
       <c r="D155" s="15"/>
     </row>
-    <row r="156" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2"/>
       <c r="B156" s="9"/>
       <c r="C156" s="10"/>
       <c r="D156" s="15"/>
     </row>
-    <row r="157" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2"/>
       <c r="B157" s="9"/>
       <c r="C157" s="10"/>
       <c r="D157" s="15"/>
     </row>
-    <row r="158" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2"/>
       <c r="B158" s="9"/>
       <c r="C158" s="10"/>
       <c r="D158" s="15"/>
     </row>
-    <row r="159" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2"/>
       <c r="B159" s="9"/>
       <c r="C159" s="10"/>
       <c r="D159" s="15"/>
     </row>
-    <row r="160" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2"/>
       <c r="B160" s="9"/>
       <c r="C160" s="10"/>
       <c r="D160" s="15"/>
     </row>
-    <row r="161" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2"/>
       <c r="B161" s="9"/>
       <c r="C161" s="10"/>
       <c r="D161" s="15"/>
     </row>
-    <row r="162" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2"/>
       <c r="B162" s="9"/>
       <c r="C162" s="10"/>
       <c r="D162" s="15"/>
     </row>
-    <row r="163" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
       <c r="B163" s="9"/>
       <c r="C163" s="10"/>
       <c r="D163" s="15"/>
     </row>
-    <row r="164" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2"/>
       <c r="B164" s="9"/>
       <c r="C164" s="10"/>
     </row>
-    <row r="165" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2"/>
       <c r="B165" s="9"/>
       <c r="C165" s="10"/>
     </row>
-    <row r="166" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2"/>
       <c r="B166" s="9"/>
       <c r="C166" s="10"/>
     </row>
-    <row r="167" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2"/>
       <c r="B167" s="9"/>
       <c r="C167" s="10"/>
     </row>
-    <row r="168" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2"/>
       <c r="B168" s="9"/>
       <c r="C168" s="10"/>
     </row>
-    <row r="169" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2"/>
       <c r="B169" s="9"/>
       <c r="C169" s="10"/>
     </row>
-    <row r="170" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2"/>
       <c r="B170" s="9"/>
       <c r="C170" s="10"/>
     </row>
-    <row r="171" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2"/>
       <c r="B171" s="9"/>
       <c r="C171" s="10"/>
     </row>
-    <row r="172" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2"/>
       <c r="B172" s="9"/>
       <c r="C172" s="10"/>
     </row>
-    <row r="173" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2"/>
       <c r="B173" s="9"/>
       <c r="C173" s="10"/>
     </row>
-    <row r="174" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2"/>
       <c r="B174" s="9"/>
       <c r="C174" s="10"/>
     </row>
-    <row r="175" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2"/>
       <c r="B175" s="9"/>
       <c r="C175" s="10"/>
     </row>
-    <row r="176" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2"/>
       <c r="B176" s="9"/>
       <c r="C176" s="10"/>
     </row>
-    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2"/>
       <c r="B177" s="9"/>
       <c r="C177" s="10"/>
     </row>
-    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2"/>
       <c r="B178" s="9"/>
       <c r="C178" s="10"/>
     </row>
-    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2"/>
       <c r="B179" s="9"/>
       <c r="C179" s="10"/>
     </row>
-    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2"/>
       <c r="B180" s="9"/>
       <c r="C180" s="10"/>
     </row>
-    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2"/>
       <c r="B181" s="9"/>
       <c r="C181" s="10"/>
     </row>
-    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2"/>
       <c r="B182" s="9"/>
       <c r="C182" s="10"/>
     </row>
-    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2"/>
       <c r="B183" s="9"/>
       <c r="C183" s="10"/>
     </row>
-    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2"/>
       <c r="B184" s="9"/>
       <c r="C184" s="10"/>
     </row>
-    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2"/>
       <c r="B185" s="9"/>
       <c r="C185" s="10"/>
     </row>
-    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2"/>
       <c r="B186" s="9"/>
       <c r="C186" s="10"/>
     </row>
-    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2"/>
       <c r="B187" s="9"/>
       <c r="C187" s="10"/>
     </row>
-    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2"/>
       <c r="B188" s="9"/>
       <c r="C188" s="10"/>
     </row>
-    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2"/>
       <c r="B189" s="9"/>
       <c r="C189" s="10"/>
     </row>
-    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2"/>
       <c r="B190" s="9"/>
       <c r="C190" s="10"/>
     </row>
-    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2"/>
       <c r="B191" s="9"/>
       <c r="C191" s="10"/>
     </row>
-    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2"/>
       <c r="B192" s="9"/>
       <c r="C192" s="10"/>
     </row>
-    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="2"/>
       <c r="B193" s="9"/>
       <c r="C193" s="10"/>
     </row>
-    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2"/>
       <c r="B194" s="9"/>
       <c r="C194" s="10"/>
     </row>
-    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="2"/>
       <c r="B195" s="9"/>
       <c r="C195" s="10"/>
     </row>
-    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="2"/>
       <c r="B196" s="9"/>
       <c r="C196" s="10"/>
     </row>
-    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="2"/>
       <c r="B197" s="9"/>
       <c r="C197" s="10"/>
     </row>
-    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="2"/>
       <c r="B198" s="9"/>
       <c r="C198" s="10"/>
     </row>
-    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="2"/>
       <c r="B199" s="9"/>
       <c r="C199" s="10"/>
     </row>
-    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="2"/>
       <c r="B200" s="9"/>
       <c r="C200" s="10"/>
     </row>
-    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="2"/>
       <c r="B201" s="9"/>
       <c r="C201" s="10"/>
     </row>
-    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2"/>
       <c r="B202" s="9"/>
       <c r="C202" s="10"/>
     </row>
-    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2"/>
       <c r="B203" s="9"/>
       <c r="C203" s="10"/>
     </row>
-    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="2"/>
       <c r="B204" s="9"/>
       <c r="C204" s="10"/>
     </row>
-    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2"/>
       <c r="B205" s="9"/>
       <c r="C205" s="10"/>
     </row>
-    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2"/>
       <c r="B206" s="9"/>
       <c r="C206" s="10"/>
     </row>
-    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2"/>
       <c r="B207" s="9"/>
       <c r="C207" s="10"/>
     </row>
-    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2"/>
       <c r="B208" s="9"/>
       <c r="C208" s="10"/>
     </row>
-    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2"/>
       <c r="B209" s="9"/>
       <c r="C209" s="10"/>
     </row>
-    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2"/>
       <c r="B210" s="9"/>
       <c r="C210" s="10"/>
     </row>
-    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2"/>
       <c r="B211" s="9"/>
       <c r="C211" s="10"/>
     </row>
-    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2"/>
       <c r="B212" s="9"/>
       <c r="C212" s="10"/>
     </row>
-    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2"/>
       <c r="B213" s="9"/>
       <c r="C213" s="10"/>
     </row>
-    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2"/>
       <c r="B214" s="9"/>
       <c r="C214" s="10"/>
     </row>
-    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="2"/>
       <c r="B215" s="9"/>
       <c r="C215" s="10"/>
     </row>
-    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="2"/>
       <c r="B216" s="9"/>
       <c r="C216" s="10"/>
     </row>
-    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2"/>
       <c r="B217" s="9"/>
       <c r="C217" s="10"/>
     </row>
-    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="2"/>
       <c r="B218" s="9"/>
       <c r="C218" s="10"/>
     </row>
-    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="2"/>
       <c r="B219" s="9"/>
       <c r="C219" s="10"/>
     </row>
-    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="2"/>
       <c r="B220" s="9"/>
       <c r="C220" s="10"/>
     </row>
-    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="2"/>
       <c r="B221" s="9"/>
       <c r="C221" s="10"/>
     </row>
-    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="2"/>
       <c r="B222" s="9"/>
       <c r="C222" s="10"/>
     </row>
-    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2"/>
       <c r="B223" s="9"/>
       <c r="C223" s="10"/>
     </row>
-    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="2"/>
       <c r="B224" s="9"/>
       <c r="C224" s="10"/>
     </row>
-    <row r="225" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="2"/>
       <c r="B225" s="9"/>
       <c r="C225" s="10"/>
     </row>
-    <row r="226" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2"/>
       <c r="B226" s="9"/>
       <c r="C226" s="10"/>
     </row>
-    <row r="227" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2"/>
       <c r="B227" s="9"/>
       <c r="C227" s="10"/>
     </row>
-    <row r="228" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="2"/>
       <c r="B228" s="9"/>
       <c r="C228" s="10"/>
     </row>
-    <row r="229" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="2"/>
       <c r="B229" s="9"/>
       <c r="C229" s="10"/>
     </row>
-    <row r="230" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="2"/>
       <c r="B230" s="9"/>
       <c r="C230" s="10"/>
     </row>
-    <row r="231" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="2"/>
       <c r="B231" s="9"/>
       <c r="C231" s="10"/>
     </row>
-    <row r="232" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="2"/>
       <c r="B232" s="9"/>
       <c r="C232" s="10"/>
     </row>
-    <row r="233" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="2"/>
       <c r="B233" s="9"/>
       <c r="C233" s="10"/>
     </row>
-    <row r="234" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="2"/>
       <c r="B234" s="9"/>
       <c r="C234" s="10"/>
     </row>
-    <row r="235" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="2"/>
       <c r="B235" s="9"/>
       <c r="C235" s="10"/>
     </row>
-    <row r="236" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="2"/>
       <c r="B236" s="9"/>
       <c r="C236" s="10"/>
     </row>
-    <row r="237" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="2"/>
       <c r="B237" s="9"/>
       <c r="C237" s="10"/>
     </row>
-    <row r="238" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="2"/>
       <c r="B238" s="9"/>
       <c r="C238" s="10"/>
     </row>
-    <row r="239" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="2"/>
       <c r="B239" s="9"/>
       <c r="C239" s="10"/>
     </row>
-    <row r="240" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="2"/>
       <c r="B240" s="9"/>
       <c r="C240" s="10"/>
     </row>
-    <row r="241" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="2"/>
       <c r="B241" s="9"/>
       <c r="C241" s="10"/>
     </row>
-    <row r="242" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="2"/>
       <c r="B242" s="9"/>
       <c r="C242" s="10"/>
     </row>
-    <row r="243" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="2"/>
       <c r="B243" s="9"/>
       <c r="C243" s="10"/>
     </row>
-    <row r="244" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="2"/>
       <c r="B244" s="9"/>
       <c r="C244" s="10"/>
     </row>
-    <row r="245" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="2"/>
       <c r="B245" s="9"/>
       <c r="C245" s="10"/>
     </row>
-    <row r="246" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="2"/>
       <c r="B246" s="9"/>
       <c r="C246" s="10"/>
     </row>
-    <row r="247" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="2"/>
       <c r="B247" s="9"/>
       <c r="C247" s="10"/>
     </row>
-    <row r="248" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="2"/>
       <c r="B248" s="9"/>
       <c r="C248" s="10"/>
     </row>
-    <row r="249" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="2"/>
       <c r="B249" s="9"/>
       <c r="C249" s="10"/>

</xml_diff>

<commit_message>
update SRS & Test cases & RTM for supplier feature
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ITI\Online-Mobile-Store-WebSite\RTM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI9M-Testing\Core\QA\WorkShop\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56DFD89-DDDC-468B-93E4-7B3F3E00FB79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B05F9E-C849-4CE3-A3C3-A897D743C06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="195">
   <si>
     <t>SRS ID</t>
   </si>
@@ -159,13 +159,7 @@
     <t>SRS_Supplier_007</t>
   </si>
   <si>
-    <t>TC_Supplier_007</t>
-  </si>
-  <si>
     <t>SRS_Supplier_008</t>
-  </si>
-  <si>
-    <t>TC_Supplier_008</t>
   </si>
   <si>
     <t>SRS_Client_001</t>
@@ -438,41 +432,10 @@
  TC_Register_006        TC_Register_014           TC_Register_020          TC_Register_021        TC_Register_022        TC_Register_023        TC_Register_024           TC_Register_025        TC_Register_026	</t>
   </si>
   <si>
-    <t>TC_Supplier_001
-TC_Supplier_009                        TC_Supplier_018</t>
-  </si>
-  <si>
-    <t>TC_Supplier_002                                                            TC_Supplier_009
-TC_Supplier_010                      TC_Supplier_018</t>
-  </si>
-  <si>
-    <t>TC_Supplier_003                                                        TC_Supplier_009
-TC_Supplier_011                TC_Supplier_018</t>
-  </si>
-  <si>
-    <t>TC_Supplier_004                                                      
-TC_Supplier_012</t>
-  </si>
-  <si>
-    <t>TC_Supplier_013               TC_Supplier_018</t>
-  </si>
-  <si>
-    <t>TC_Supplier_005                                                       TC_Supplier_014
-TC_Supplier_015</t>
-  </si>
-  <si>
-    <t>TC_Supplier_006                                                  
-TC_Supplier_016</t>
-  </si>
-  <si>
     <t>SRS_Supplier_009</t>
   </si>
   <si>
     <t>SRS_Supplier_010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                   
-TC_Supplier_017</t>
   </si>
   <si>
     <t>System Design ID</t>
@@ -488,13 +451,6 @@
     <t>CD_AddNewProduct_page
 FC_AddNewProduct_page
 SD_AddNewProduct_002
-UI_AddNewProduct_002
-UI_AddNewProduct_003</t>
-  </si>
-  <si>
-    <t>CD_AddNewProduct_page
-FC_AddNewProduct_page
-SD_AddNewProduct_002
 UI_AddNewProduct_004</t>
   </si>
   <si>
@@ -607,12 +563,6 @@
     <t>ClassDiagram_SupplierUpdatePage
 FlowChart_SupplierUpdatePage
 SequenceDiagram_SupplierUpdatePage</t>
-  </si>
-  <si>
-    <t>ClassDiagram_SupplierUpdatePage
-FlowChart_SupplierUpdatePage
-SequenceDiagram_SupplierUpdatePage
-UI_SupplierUpdatePage</t>
   </si>
   <si>
     <t>edit.html
@@ -669,6 +619,81 @@
   </si>
   <si>
     <t>CD_Cart                                                                FC_Cart                                                                                         SD_Cart_001                                                       UI_Cart_002</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_011</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_012</t>
+  </si>
+  <si>
+    <t>SRS_Supplier_013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_Supplier_001
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_Supplier_003                                                            TC_Supplier_004
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD_AddNewProduct_page
+FC_AddNewProduct_page
+SD_AddNewProduct_002
+UI_AddNewProduct_002
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_Supplier_005                                                      </t>
+  </si>
+  <si>
+    <t>CD_AddNewProduct_page
+FC_AddNewProduct_page
+SD_AddNewProduct_002
+UI_AddNewProduct_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_Supplier_006                                                   
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_Supplier_07             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_Supplier_008                                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_Supplier_009                                           
+</t>
+  </si>
+  <si>
+    <t>TC_Supplier_010</t>
+  </si>
+  <si>
+    <t>TC_Supplier_017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClassDiagram_SupplierUpdatePage
+FlowChart_SupplierUpdatePage
+SequenceDiagram_SupplierUpdatePage
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                   
+TC_Supplier_020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                   
+TC_Supplier_021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                   
+TC_Supplier_019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                   
+TC_Supplier_002                   TC_Supplier_011               TC_Supplier_012                           TC_Supplier_013                              TC_Supplier_014                               TC_Supplier_015                                     TC_Supplier_016                                 TC_Supplier_018                               TC_Supplier_022</t>
   </si>
 </sst>
 </file>
@@ -1072,23 +1097,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E249"/>
+  <dimension ref="A1:E252"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="37.7109375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="37.44140625" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="38.44140625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="37.6640625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1096,67 +1121,67 @@
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="59.45" customHeight="1" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="59.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="73.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1164,33 +1189,33 @@
         <v>12</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="82.15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="82.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1198,33 +1223,33 @@
         <v>15</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1232,33 +1257,33 @@
         <v>19</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="109.9" customHeight="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="109.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -1266,16 +1291,16 @@
         <v>22</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="90.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -1283,16 +1308,16 @@
         <v>24</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1300,16 +1325,16 @@
         <v>26</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="61.15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="61.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1317,16 +1342,16 @@
         <v>28</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
@@ -1334,135 +1359,135 @@
         <v>30</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D15" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="55.9" customHeight="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="55.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="88.9" customHeight="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="88.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="55.9" customHeight="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="55.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="88.15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="88.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>5</v>
       </c>
@@ -1470,1636 +1495,1687 @@
         <v>7</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="70.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>97</v>
-      </c>
       <c r="C25" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="155.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>126</v>
+        <v>179</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="103.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>127</v>
+        <v>180</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>138</v>
+        <v>181</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="93.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>128</v>
+        <v>182</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>139</v>
+        <v>183</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="106.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>129</v>
+        <v>184</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="85.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>130</v>
+        <v>185</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="85.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>131</v>
+        <v>186</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>132</v>
+        <v>187</v>
       </c>
       <c r="C32" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="86.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C34" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="D32" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="E32" s="10" t="s">
+      <c r="D34" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="179.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="83.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E39" s="10" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="16" t="s">
+    <row r="40" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="40.799999999999997" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="40.799999999999997" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="40.799999999999997" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="40.799999999999997" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="40.799999999999997" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="67.2" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C48" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D33" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D34" s="15" t="s">
+      <c r="D48" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="E48" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="E34" s="10" t="s">
+    </row>
+    <row r="49" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C55" s="10" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="C35" s="16" t="s">
+      <c r="D55" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E56" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="D35" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="39.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="39.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="39.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="39.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="39.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="65.25" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B50" s="4" t="s">
+    </row>
+    <row r="57" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B57" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C50" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B51" s="4" t="s">
+      <c r="C57" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B58" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C51" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D53" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D54" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D55" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="E55" s="10" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="15"/>
-    </row>
-    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="15"/>
-    </row>
-    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="15"/>
-    </row>
-    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C58" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
-      <c r="B59" s="9"/>
+      <c r="B59" s="2"/>
       <c r="C59" s="10"/>
       <c r="D59" s="15"/>
     </row>
-    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
-      <c r="B60" s="9"/>
+      <c r="B60" s="2"/>
       <c r="C60" s="10"/>
       <c r="D60" s="15"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
-      <c r="B61" s="9"/>
+      <c r="B61" s="2"/>
       <c r="C61" s="10"/>
       <c r="D61" s="15"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="9"/>
       <c r="C62" s="10"/>
       <c r="D62" s="15"/>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="9"/>
       <c r="C63" s="10"/>
       <c r="D63" s="15"/>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="9"/>
       <c r="C64" s="10"/>
       <c r="D64" s="15"/>
     </row>
-    <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="9"/>
       <c r="C65" s="10"/>
       <c r="D65" s="15"/>
     </row>
-    <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="9"/>
       <c r="C66" s="10"/>
       <c r="D66" s="15"/>
     </row>
-    <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" s="9"/>
       <c r="C67" s="10"/>
       <c r="D67" s="15"/>
     </row>
-    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" s="9"/>
       <c r="C68" s="10"/>
       <c r="D68" s="15"/>
     </row>
-    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="9"/>
       <c r="C69" s="10"/>
       <c r="D69" s="15"/>
     </row>
-    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" s="9"/>
       <c r="C70" s="10"/>
       <c r="D70" s="15"/>
     </row>
-    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="9"/>
       <c r="C71" s="10"/>
       <c r="D71" s="15"/>
     </row>
-    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="9"/>
       <c r="C72" s="10"/>
       <c r="D72" s="15"/>
     </row>
-    <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="9"/>
       <c r="C73" s="10"/>
       <c r="D73" s="15"/>
     </row>
-    <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="9"/>
       <c r="C74" s="10"/>
       <c r="D74" s="15"/>
     </row>
-    <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="9"/>
       <c r="C75" s="10"/>
       <c r="D75" s="15"/>
     </row>
-    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="9"/>
       <c r="C76" s="10"/>
       <c r="D76" s="15"/>
     </row>
-    <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" s="9"/>
       <c r="C77" s="10"/>
       <c r="D77" s="15"/>
     </row>
-    <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" s="9"/>
       <c r="C78" s="10"/>
       <c r="D78" s="15"/>
     </row>
-    <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" s="9"/>
       <c r="C79" s="10"/>
       <c r="D79" s="15"/>
     </row>
-    <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" s="9"/>
       <c r="C80" s="10"/>
       <c r="D80" s="15"/>
     </row>
-    <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="B81" s="9"/>
       <c r="C81" s="10"/>
       <c r="D81" s="15"/>
     </row>
-    <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
       <c r="B82" s="9"/>
       <c r="C82" s="10"/>
       <c r="D82" s="15"/>
     </row>
-    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2"/>
       <c r="B83" s="9"/>
       <c r="C83" s="10"/>
       <c r="D83" s="15"/>
     </row>
-    <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
       <c r="B84" s="9"/>
       <c r="C84" s="10"/>
       <c r="D84" s="15"/>
     </row>
-    <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2"/>
       <c r="B85" s="9"/>
       <c r="C85" s="10"/>
       <c r="D85" s="15"/>
     </row>
-    <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" s="9"/>
       <c r="C86" s="10"/>
       <c r="D86" s="15"/>
     </row>
-    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
       <c r="B87" s="9"/>
       <c r="C87" s="10"/>
       <c r="D87" s="15"/>
     </row>
-    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
       <c r="B88" s="9"/>
       <c r="C88" s="10"/>
       <c r="D88" s="15"/>
     </row>
-    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" s="9"/>
       <c r="C89" s="10"/>
       <c r="D89" s="15"/>
     </row>
-    <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
       <c r="B90" s="9"/>
       <c r="C90" s="10"/>
       <c r="D90" s="15"/>
     </row>
-    <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
       <c r="B91" s="9"/>
       <c r="C91" s="10"/>
       <c r="D91" s="15"/>
     </row>
-    <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
       <c r="B92" s="9"/>
       <c r="C92" s="10"/>
       <c r="D92" s="15"/>
     </row>
-    <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
       <c r="B93" s="9"/>
       <c r="C93" s="10"/>
       <c r="D93" s="15"/>
     </row>
-    <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
       <c r="B94" s="9"/>
       <c r="C94" s="10"/>
       <c r="D94" s="15"/>
     </row>
-    <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2"/>
       <c r="B95" s="9"/>
       <c r="C95" s="10"/>
       <c r="D95" s="15"/>
     </row>
-    <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
       <c r="B96" s="9"/>
       <c r="C96" s="10"/>
       <c r="D96" s="15"/>
     </row>
-    <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
       <c r="B97" s="9"/>
       <c r="C97" s="10"/>
       <c r="D97" s="15"/>
     </row>
-    <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
       <c r="B98" s="9"/>
       <c r="C98" s="10"/>
       <c r="D98" s="15"/>
     </row>
-    <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
       <c r="B99" s="9"/>
       <c r="C99" s="10"/>
       <c r="D99" s="15"/>
     </row>
-    <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
       <c r="B100" s="9"/>
       <c r="C100" s="10"/>
       <c r="D100" s="15"/>
     </row>
-    <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
       <c r="B101" s="9"/>
       <c r="C101" s="10"/>
       <c r="D101" s="15"/>
     </row>
-    <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
       <c r="B102" s="9"/>
       <c r="C102" s="10"/>
       <c r="D102" s="15"/>
     </row>
-    <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
       <c r="B103" s="9"/>
       <c r="C103" s="10"/>
       <c r="D103" s="15"/>
     </row>
-    <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="B104" s="9"/>
       <c r="C104" s="10"/>
       <c r="D104" s="15"/>
     </row>
-    <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
       <c r="B105" s="9"/>
       <c r="C105" s="10"/>
       <c r="D105" s="15"/>
     </row>
-    <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="B106" s="9"/>
       <c r="C106" s="10"/>
       <c r="D106" s="15"/>
     </row>
-    <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" s="9"/>
       <c r="C107" s="10"/>
       <c r="D107" s="15"/>
     </row>
-    <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
       <c r="B108" s="9"/>
       <c r="C108" s="10"/>
       <c r="D108" s="15"/>
     </row>
-    <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2"/>
       <c r="B109" s="9"/>
       <c r="C109" s="10"/>
       <c r="D109" s="15"/>
     </row>
-    <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="B110" s="9"/>
       <c r="C110" s="10"/>
       <c r="D110" s="15"/>
     </row>
-    <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2"/>
       <c r="B111" s="9"/>
       <c r="C111" s="10"/>
       <c r="D111" s="15"/>
     </row>
-    <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
       <c r="B112" s="9"/>
       <c r="C112" s="10"/>
       <c r="D112" s="15"/>
     </row>
-    <row r="113" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
       <c r="B113" s="9"/>
       <c r="C113" s="10"/>
       <c r="D113" s="15"/>
     </row>
-    <row r="114" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="B114" s="9"/>
       <c r="C114" s="10"/>
       <c r="D114" s="15"/>
     </row>
-    <row r="115" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2"/>
       <c r="B115" s="9"/>
       <c r="C115" s="10"/>
       <c r="D115" s="15"/>
     </row>
-    <row r="116" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2"/>
       <c r="B116" s="9"/>
       <c r="C116" s="10"/>
       <c r="D116" s="15"/>
     </row>
-    <row r="117" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2"/>
       <c r="B117" s="9"/>
       <c r="C117" s="10"/>
       <c r="D117" s="15"/>
     </row>
-    <row r="118" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2"/>
       <c r="B118" s="9"/>
       <c r="C118" s="10"/>
       <c r="D118" s="15"/>
     </row>
-    <row r="119" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2"/>
       <c r="B119" s="9"/>
       <c r="C119" s="10"/>
       <c r="D119" s="15"/>
     </row>
-    <row r="120" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2"/>
       <c r="B120" s="9"/>
       <c r="C120" s="10"/>
       <c r="D120" s="15"/>
     </row>
-    <row r="121" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2"/>
       <c r="B121" s="9"/>
       <c r="C121" s="10"/>
       <c r="D121" s="15"/>
     </row>
-    <row r="122" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2"/>
       <c r="B122" s="9"/>
       <c r="C122" s="10"/>
       <c r="D122" s="15"/>
     </row>
-    <row r="123" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2"/>
       <c r="B123" s="9"/>
       <c r="C123" s="10"/>
       <c r="D123" s="15"/>
     </row>
-    <row r="124" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2"/>
       <c r="B124" s="9"/>
       <c r="C124" s="10"/>
       <c r="D124" s="15"/>
     </row>
-    <row r="125" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2"/>
       <c r="B125" s="9"/>
       <c r="C125" s="10"/>
       <c r="D125" s="15"/>
     </row>
-    <row r="126" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2"/>
       <c r="B126" s="9"/>
       <c r="C126" s="10"/>
       <c r="D126" s="15"/>
     </row>
-    <row r="127" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2"/>
       <c r="B127" s="9"/>
       <c r="C127" s="10"/>
       <c r="D127" s="15"/>
     </row>
-    <row r="128" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2"/>
       <c r="B128" s="9"/>
       <c r="C128" s="10"/>
       <c r="D128" s="15"/>
     </row>
-    <row r="129" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2"/>
       <c r="B129" s="9"/>
       <c r="C129" s="10"/>
       <c r="D129" s="15"/>
     </row>
-    <row r="130" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2"/>
       <c r="B130" s="9"/>
       <c r="C130" s="10"/>
       <c r="D130" s="15"/>
     </row>
-    <row r="131" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2"/>
       <c r="B131" s="9"/>
       <c r="C131" s="10"/>
       <c r="D131" s="15"/>
     </row>
-    <row r="132" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2"/>
       <c r="B132" s="9"/>
       <c r="C132" s="10"/>
       <c r="D132" s="15"/>
     </row>
-    <row r="133" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2"/>
       <c r="B133" s="9"/>
       <c r="C133" s="10"/>
       <c r="D133" s="15"/>
     </row>
-    <row r="134" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2"/>
       <c r="B134" s="9"/>
       <c r="C134" s="10"/>
       <c r="D134" s="15"/>
     </row>
-    <row r="135" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2"/>
       <c r="B135" s="9"/>
       <c r="C135" s="10"/>
       <c r="D135" s="15"/>
     </row>
-    <row r="136" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2"/>
       <c r="B136" s="9"/>
       <c r="C136" s="10"/>
       <c r="D136" s="15"/>
     </row>
-    <row r="137" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2"/>
       <c r="B137" s="9"/>
       <c r="C137" s="10"/>
       <c r="D137" s="15"/>
     </row>
-    <row r="138" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2"/>
       <c r="B138" s="9"/>
       <c r="C138" s="10"/>
       <c r="D138" s="15"/>
     </row>
-    <row r="139" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2"/>
       <c r="B139" s="9"/>
       <c r="C139" s="10"/>
       <c r="D139" s="15"/>
     </row>
-    <row r="140" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2"/>
       <c r="B140" s="9"/>
       <c r="C140" s="10"/>
       <c r="D140" s="15"/>
     </row>
-    <row r="141" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2"/>
       <c r="B141" s="9"/>
       <c r="C141" s="10"/>
       <c r="D141" s="15"/>
     </row>
-    <row r="142" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2"/>
       <c r="B142" s="9"/>
       <c r="C142" s="10"/>
       <c r="D142" s="15"/>
     </row>
-    <row r="143" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2"/>
       <c r="B143" s="9"/>
       <c r="C143" s="10"/>
       <c r="D143" s="15"/>
     </row>
-    <row r="144" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2"/>
       <c r="B144" s="9"/>
       <c r="C144" s="10"/>
       <c r="D144" s="15"/>
     </row>
-    <row r="145" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2"/>
       <c r="B145" s="9"/>
       <c r="C145" s="10"/>
       <c r="D145" s="15"/>
     </row>
-    <row r="146" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2"/>
       <c r="B146" s="9"/>
       <c r="C146" s="10"/>
       <c r="D146" s="15"/>
     </row>
-    <row r="147" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2"/>
       <c r="B147" s="9"/>
       <c r="C147" s="10"/>
       <c r="D147" s="15"/>
     </row>
-    <row r="148" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2"/>
       <c r="B148" s="9"/>
       <c r="C148" s="10"/>
       <c r="D148" s="15"/>
     </row>
-    <row r="149" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2"/>
       <c r="B149" s="9"/>
       <c r="C149" s="10"/>
       <c r="D149" s="15"/>
     </row>
-    <row r="150" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2"/>
       <c r="B150" s="9"/>
       <c r="C150" s="10"/>
       <c r="D150" s="15"/>
     </row>
-    <row r="151" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2"/>
       <c r="B151" s="9"/>
       <c r="C151" s="10"/>
       <c r="D151" s="15"/>
     </row>
-    <row r="152" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2"/>
       <c r="B152" s="9"/>
       <c r="C152" s="10"/>
       <c r="D152" s="15"/>
     </row>
-    <row r="153" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2"/>
       <c r="B153" s="9"/>
       <c r="C153" s="10"/>
       <c r="D153" s="15"/>
     </row>
-    <row r="154" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="2"/>
       <c r="B154" s="9"/>
       <c r="C154" s="10"/>
       <c r="D154" s="15"/>
     </row>
-    <row r="155" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="2"/>
       <c r="B155" s="9"/>
       <c r="C155" s="10"/>
       <c r="D155" s="15"/>
     </row>
-    <row r="156" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="2"/>
       <c r="B156" s="9"/>
       <c r="C156" s="10"/>
       <c r="D156" s="15"/>
     </row>
-    <row r="157" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="2"/>
       <c r="B157" s="9"/>
       <c r="C157" s="10"/>
       <c r="D157" s="15"/>
     </row>
-    <row r="158" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="2"/>
       <c r="B158" s="9"/>
       <c r="C158" s="10"/>
       <c r="D158" s="15"/>
     </row>
-    <row r="159" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2"/>
       <c r="B159" s="9"/>
       <c r="C159" s="10"/>
       <c r="D159" s="15"/>
     </row>
-    <row r="160" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="2"/>
       <c r="B160" s="9"/>
       <c r="C160" s="10"/>
       <c r="D160" s="15"/>
     </row>
-    <row r="161" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="2"/>
       <c r="B161" s="9"/>
       <c r="C161" s="10"/>
       <c r="D161" s="15"/>
     </row>
-    <row r="162" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="2"/>
       <c r="B162" s="9"/>
       <c r="C162" s="10"/>
       <c r="D162" s="15"/>
     </row>
-    <row r="163" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="2"/>
       <c r="B163" s="9"/>
       <c r="C163" s="10"/>
       <c r="D163" s="15"/>
     </row>
-    <row r="164" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="2"/>
       <c r="B164" s="9"/>
       <c r="C164" s="10"/>
-    </row>
-    <row r="165" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D164" s="15"/>
+    </row>
+    <row r="165" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="2"/>
       <c r="B165" s="9"/>
       <c r="C165" s="10"/>
-    </row>
-    <row r="166" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D165" s="15"/>
+    </row>
+    <row r="166" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="2"/>
       <c r="B166" s="9"/>
       <c r="C166" s="10"/>
-    </row>
-    <row r="167" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D166" s="15"/>
+    </row>
+    <row r="167" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="2"/>
       <c r="B167" s="9"/>
       <c r="C167" s="10"/>
     </row>
-    <row r="168" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="2"/>
       <c r="B168" s="9"/>
       <c r="C168" s="10"/>
     </row>
-    <row r="169" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="2"/>
       <c r="B169" s="9"/>
       <c r="C169" s="10"/>
     </row>
-    <row r="170" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="2"/>
       <c r="B170" s="9"/>
       <c r="C170" s="10"/>
     </row>
-    <row r="171" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="2"/>
       <c r="B171" s="9"/>
       <c r="C171" s="10"/>
     </row>
-    <row r="172" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="2"/>
       <c r="B172" s="9"/>
       <c r="C172" s="10"/>
     </row>
-    <row r="173" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="2"/>
       <c r="B173" s="9"/>
       <c r="C173" s="10"/>
     </row>
-    <row r="174" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="2"/>
       <c r="B174" s="9"/>
       <c r="C174" s="10"/>
     </row>
-    <row r="175" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="2"/>
       <c r="B175" s="9"/>
       <c r="C175" s="10"/>
     </row>
-    <row r="176" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="2"/>
       <c r="B176" s="9"/>
       <c r="C176" s="10"/>
     </row>
-    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="2"/>
       <c r="B177" s="9"/>
       <c r="C177" s="10"/>
     </row>
-    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="2"/>
       <c r="B178" s="9"/>
       <c r="C178" s="10"/>
     </row>
-    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="2"/>
       <c r="B179" s="9"/>
       <c r="C179" s="10"/>
     </row>
-    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="2"/>
       <c r="B180" s="9"/>
       <c r="C180" s="10"/>
     </row>
-    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="2"/>
       <c r="B181" s="9"/>
       <c r="C181" s="10"/>
     </row>
-    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="2"/>
       <c r="B182" s="9"/>
       <c r="C182" s="10"/>
     </row>
-    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="2"/>
       <c r="B183" s="9"/>
       <c r="C183" s="10"/>
     </row>
-    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="2"/>
       <c r="B184" s="9"/>
       <c r="C184" s="10"/>
     </row>
-    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="2"/>
       <c r="B185" s="9"/>
       <c r="C185" s="10"/>
     </row>
-    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="2"/>
       <c r="B186" s="9"/>
       <c r="C186" s="10"/>
     </row>
-    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="2"/>
       <c r="B187" s="9"/>
       <c r="C187" s="10"/>
     </row>
-    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="2"/>
       <c r="B188" s="9"/>
       <c r="C188" s="10"/>
     </row>
-    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="2"/>
       <c r="B189" s="9"/>
       <c r="C189" s="10"/>
     </row>
-    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="2"/>
       <c r="B190" s="9"/>
       <c r="C190" s="10"/>
     </row>
-    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="2"/>
       <c r="B191" s="9"/>
       <c r="C191" s="10"/>
     </row>
-    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="2"/>
       <c r="B192" s="9"/>
       <c r="C192" s="10"/>
     </row>
-    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="2"/>
       <c r="B193" s="9"/>
       <c r="C193" s="10"/>
     </row>
-    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="2"/>
       <c r="B194" s="9"/>
       <c r="C194" s="10"/>
     </row>
-    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="2"/>
       <c r="B195" s="9"/>
       <c r="C195" s="10"/>
     </row>
-    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="2"/>
       <c r="B196" s="9"/>
       <c r="C196" s="10"/>
     </row>
-    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="2"/>
       <c r="B197" s="9"/>
       <c r="C197" s="10"/>
     </row>
-    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="2"/>
       <c r="B198" s="9"/>
       <c r="C198" s="10"/>
     </row>
-    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="2"/>
       <c r="B199" s="9"/>
       <c r="C199" s="10"/>
     </row>
-    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="2"/>
       <c r="B200" s="9"/>
       <c r="C200" s="10"/>
     </row>
-    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="2"/>
       <c r="B201" s="9"/>
       <c r="C201" s="10"/>
     </row>
-    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="2"/>
       <c r="B202" s="9"/>
       <c r="C202" s="10"/>
     </row>
-    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="2"/>
       <c r="B203" s="9"/>
       <c r="C203" s="10"/>
     </row>
-    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="2"/>
       <c r="B204" s="9"/>
       <c r="C204" s="10"/>
     </row>
-    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="2"/>
       <c r="B205" s="9"/>
       <c r="C205" s="10"/>
     </row>
-    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="2"/>
       <c r="B206" s="9"/>
       <c r="C206" s="10"/>
     </row>
-    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="2"/>
       <c r="B207" s="9"/>
       <c r="C207" s="10"/>
     </row>
-    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="2"/>
       <c r="B208" s="9"/>
       <c r="C208" s="10"/>
     </row>
-    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="2"/>
       <c r="B209" s="9"/>
       <c r="C209" s="10"/>
     </row>
-    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="2"/>
       <c r="B210" s="9"/>
       <c r="C210" s="10"/>
     </row>
-    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="2"/>
       <c r="B211" s="9"/>
       <c r="C211" s="10"/>
     </row>
-    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2"/>
       <c r="B212" s="9"/>
       <c r="C212" s="10"/>
     </row>
-    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="2"/>
       <c r="B213" s="9"/>
       <c r="C213" s="10"/>
     </row>
-    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="2"/>
       <c r="B214" s="9"/>
       <c r="C214" s="10"/>
     </row>
-    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="2"/>
       <c r="B215" s="9"/>
       <c r="C215" s="10"/>
     </row>
-    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="2"/>
       <c r="B216" s="9"/>
       <c r="C216" s="10"/>
     </row>
-    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="2"/>
       <c r="B217" s="9"/>
       <c r="C217" s="10"/>
     </row>
-    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="2"/>
       <c r="B218" s="9"/>
       <c r="C218" s="10"/>
     </row>
-    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="2"/>
       <c r="B219" s="9"/>
       <c r="C219" s="10"/>
     </row>
-    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="2"/>
       <c r="B220" s="9"/>
       <c r="C220" s="10"/>
     </row>
-    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="2"/>
       <c r="B221" s="9"/>
       <c r="C221" s="10"/>
     </row>
-    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="2"/>
       <c r="B222" s="9"/>
       <c r="C222" s="10"/>
     </row>
-    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="2"/>
       <c r="B223" s="9"/>
       <c r="C223" s="10"/>
     </row>
-    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="2"/>
       <c r="B224" s="9"/>
       <c r="C224" s="10"/>
     </row>
-    <row r="225" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="2"/>
       <c r="B225" s="9"/>
       <c r="C225" s="10"/>
     </row>
-    <row r="226" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="2"/>
       <c r="B226" s="9"/>
       <c r="C226" s="10"/>
     </row>
-    <row r="227" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="2"/>
       <c r="B227" s="9"/>
       <c r="C227" s="10"/>
     </row>
-    <row r="228" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="2"/>
       <c r="B228" s="9"/>
       <c r="C228" s="10"/>
     </row>
-    <row r="229" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="2"/>
       <c r="B229" s="9"/>
       <c r="C229" s="10"/>
     </row>
-    <row r="230" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="2"/>
       <c r="B230" s="9"/>
       <c r="C230" s="10"/>
     </row>
-    <row r="231" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="2"/>
       <c r="B231" s="9"/>
       <c r="C231" s="10"/>
     </row>
-    <row r="232" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="2"/>
       <c r="B232" s="9"/>
       <c r="C232" s="10"/>
     </row>
-    <row r="233" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="2"/>
       <c r="B233" s="9"/>
       <c r="C233" s="10"/>
     </row>
-    <row r="234" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="2"/>
       <c r="B234" s="9"/>
       <c r="C234" s="10"/>
     </row>
-    <row r="235" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="2"/>
       <c r="B235" s="9"/>
       <c r="C235" s="10"/>
     </row>
-    <row r="236" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="2"/>
       <c r="B236" s="9"/>
       <c r="C236" s="10"/>
     </row>
-    <row r="237" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="2"/>
       <c r="B237" s="9"/>
       <c r="C237" s="10"/>
     </row>
-    <row r="238" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="2"/>
       <c r="B238" s="9"/>
       <c r="C238" s="10"/>
     </row>
-    <row r="239" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="2"/>
       <c r="B239" s="9"/>
       <c r="C239" s="10"/>
     </row>
-    <row r="240" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="2"/>
       <c r="B240" s="9"/>
       <c r="C240" s="10"/>
     </row>
-    <row r="241" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="2"/>
       <c r="B241" s="9"/>
       <c r="C241" s="10"/>
     </row>
-    <row r="242" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="2"/>
       <c r="B242" s="9"/>
       <c r="C242" s="10"/>
     </row>
-    <row r="243" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="2"/>
       <c r="B243" s="9"/>
       <c r="C243" s="10"/>
     </row>
-    <row r="244" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="2"/>
       <c r="B244" s="9"/>
       <c r="C244" s="10"/>
     </row>
-    <row r="245" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="2"/>
       <c r="B245" s="9"/>
       <c r="C245" s="10"/>
     </row>
-    <row r="246" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="2"/>
       <c r="B246" s="9"/>
       <c r="C246" s="10"/>
     </row>
-    <row r="247" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="2"/>
       <c r="B247" s="9"/>
       <c r="C247" s="10"/>
     </row>
-    <row r="248" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="2"/>
       <c r="B248" s="9"/>
       <c r="C248" s="10"/>
     </row>
-    <row r="249" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="2"/>
       <c r="B249" s="9"/>
       <c r="C249" s="10"/>
+    </row>
+    <row r="250" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A250" s="2"/>
+      <c r="B250" s="9"/>
+      <c r="C250" s="10"/>
+    </row>
+    <row r="251" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A251" s="2"/>
+      <c r="B251" s="9"/>
+      <c r="C251" s="10"/>
+    </row>
+    <row r="252" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A252" s="2"/>
+      <c r="B252" s="9"/>
+      <c r="C252" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Update test documents: RTM, SRS, Bug Report, Test Cases
</commit_message>
<xml_diff>
--- a/RTM/Traceability-Matrix.xlsx
+++ b/RTM/Traceability-Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ITI\Online-Mobile-Store-WebSite\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45C9D0A-0BEB-4828-9A9E-45F7E712506A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE1B50F-E945-4434-AC0D-EBEC0721F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -402,9 +402,6 @@
 TC_Register_021           </t>
   </si>
   <si>
-    <t>TC_Register_016             TC_Register_028              TC_Register_029</t>
-  </si>
-  <si>
     <t xml:space="preserve">TC_Register_002                TC_Register_003              TC_Register_004              TC_Register_005              TC_Register_007          TC_Register_009         TC_Register_010             TC_Register_011             TC_Register_012              TC_Register_013              TC_Register_015            TC_Register_016             TC_Register_017     
  TC_Register_018       TC_Register_019       
 TC_Register_027        TC_Register_028      
@@ -692,6 +689,9 @@
   </si>
   <si>
     <t>TC_Register_011                           TC_Register_035</t>
+  </si>
+  <si>
+    <t>TC_Register_016             TC_Register_028              TC_Register_029                        TC_Register_036</t>
   </si>
 </sst>
 </file>
@@ -1098,8 +1098,8 @@
   <dimension ref="A1:E252"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1122,10 +1122,10 @@
         <v>79</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="59.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -1133,16 +1133,16 @@
         <v>8</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>65</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.3">
@@ -1156,10 +1156,10 @@
         <v>66</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.3">
@@ -1173,10 +1173,10 @@
         <v>67</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -1190,10 +1190,10 @@
         <v>68</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.3">
@@ -1207,10 +1207,10 @@
         <v>69</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="82.15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1224,10 +1224,10 @@
         <v>65</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -1235,16 +1235,16 @@
         <v>16</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>70</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.3">
@@ -1258,10 +1258,10 @@
         <v>65</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.3">
@@ -1269,16 +1269,16 @@
         <v>18</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>71</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="109.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1286,16 +1286,16 @@
         <v>20</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>72</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1309,10 +1309,10 @@
         <v>73</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.3">
@@ -1326,10 +1326,10 @@
         <v>74</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="61.15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1343,10 +1343,10 @@
         <v>75</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -1360,10 +1360,10 @@
         <v>65</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="132.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1371,16 +1371,16 @@
         <v>28</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>116</v>
+        <v>194</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>76</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="55.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1388,16 +1388,16 @@
         <v>30</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>77</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.3">
@@ -1405,16 +1405,16 @@
         <v>31</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>77</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="88.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1422,16 +1422,16 @@
         <v>32</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>65</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="55.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1442,13 +1442,13 @@
         <v>93</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="88.15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1459,13 +1459,13 @@
         <v>93</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.3">
@@ -1479,10 +1479,10 @@
         <v>88</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
@@ -1493,13 +1493,13 @@
         <v>7</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -1513,10 +1513,10 @@
         <v>89</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.3">
@@ -1530,10 +1530,10 @@
         <v>90</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="155.44999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -1541,16 +1541,16 @@
         <v>33</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>80</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="103.15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1558,16 +1558,16 @@
         <v>34</v>
       </c>
       <c r="B27" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="D27" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="C27" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>176</v>
-      </c>
       <c r="E27" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1575,16 +1575,16 @@
         <v>35</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="D28" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="E28" s="10" t="s">
         <v>153</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="106.15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1592,16 +1592,16 @@
         <v>36</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>81</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="85.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1609,16 +1609,16 @@
         <v>37</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>81</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="85.15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1626,16 +1626,16 @@
         <v>38</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>82</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.3">
@@ -1643,16 +1643,16 @@
         <v>39</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>83</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.3">
@@ -1660,101 +1660,101 @@
         <v>40</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C33" s="16" t="s">
         <v>84</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="86.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>85</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="179.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D35" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E35" s="10" t="s">
         <v>156</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="83.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="77.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1768,10 +1768,10 @@
         <v>87</v>
       </c>
       <c r="D39" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E39" s="10" t="s">
         <v>164</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1785,10 +1785,10 @@
         <v>87</v>
       </c>
       <c r="D40" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E40" s="10" t="s">
         <v>164</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1802,10 +1802,10 @@
         <v>87</v>
       </c>
       <c r="D41" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E41" s="10" t="s">
         <v>164</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="39.75" x14ac:dyDescent="0.3">
@@ -1819,10 +1819,10 @@
         <v>87</v>
       </c>
       <c r="D42" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E42" s="10" t="s">
         <v>164</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="39.75" x14ac:dyDescent="0.3">
@@ -1836,10 +1836,10 @@
         <v>87</v>
       </c>
       <c r="D43" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E43" s="10" t="s">
         <v>164</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="39.75" x14ac:dyDescent="0.3">
@@ -1853,10 +1853,10 @@
         <v>87</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="39.75" x14ac:dyDescent="0.3">
@@ -1870,10 +1870,10 @@
         <v>87</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="39.75" x14ac:dyDescent="0.3">
@@ -1887,10 +1887,10 @@
         <v>87</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="65.25" x14ac:dyDescent="0.3">
@@ -1904,10 +1904,10 @@
         <v>112</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1921,10 +1921,10 @@
         <v>86</v>
       </c>
       <c r="D48" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E48" s="10" t="s">
         <v>167</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1938,10 +1938,10 @@
         <v>86</v>
       </c>
       <c r="D49" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E49" s="10" t="s">
         <v>167</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1955,10 +1955,10 @@
         <v>86</v>
       </c>
       <c r="D50" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E50" s="10" t="s">
         <v>167</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1972,10 +1972,10 @@
         <v>86</v>
       </c>
       <c r="D51" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E51" s="10" t="s">
         <v>167</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1989,10 +1989,10 @@
         <v>86</v>
       </c>
       <c r="D52" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E52" s="10" t="s">
         <v>167</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -2006,10 +2006,10 @@
         <v>86</v>
       </c>
       <c r="D53" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E53" s="10" t="s">
         <v>167</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -2023,10 +2023,10 @@
         <v>86</v>
       </c>
       <c r="D54" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E54" s="10" t="s">
         <v>167</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -2037,13 +2037,13 @@
         <v>63</v>
       </c>
       <c r="C55" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="D55" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="D55" s="10" t="s">
-        <v>170</v>
-      </c>
       <c r="E55" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -2057,10 +2057,10 @@
         <v>78</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -2074,10 +2074,10 @@
         <v>78</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -2091,10 +2091,10 @@
         <v>78</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>